<commit_message>
add : implémenter besoins dans SystemeNerveux
</commit_message>
<xml_diff>
--- a/doc/chiffrier_sim_vie.xlsx
+++ b/doc/chiffrier_sim_vie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travail\sim_vie\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27425D42-986F-4C75-AECB-727442574D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACE011D-EBC5-4434-A56F-45A41A297269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="655">
   <si>
     <t>Chiffrier de documentation de projets</t>
   </si>
@@ -2200,6 +2200,9 @@
   </si>
   <si>
     <t>Yanis</t>
+  </si>
+  <si>
+    <t>05/12/2025</t>
   </si>
 </sst>
 </file>
@@ -3471,7 +3474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="315">
+  <cellXfs count="314">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3997,10 +4000,10 @@
     <xf numFmtId="164" fontId="29" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="29" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="29" fillId="3" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4206,7 +4209,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10516,8 +10518,8 @@
   </sheetPr>
   <dimension ref="B1:H141"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="B41" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -15600,10 +15602,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:U200"/>
+  <dimension ref="B2:U198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -15615,7 +15617,8 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="9" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
     <col min="10" max="10" width="20.5703125" customWidth="1"/>
     <col min="11" max="12" width="9.42578125" customWidth="1"/>
     <col min="13" max="13" width="20.5703125" customWidth="1"/>
@@ -15921,7 +15924,7 @@
       <c r="E14" s="231" t="s">
         <v>639</v>
       </c>
-      <c r="F14" s="244"/>
+      <c r="F14" s="243"/>
       <c r="G14" s="217"/>
       <c r="H14" s="231"/>
       <c r="I14" s="216"/>
@@ -15948,7 +15951,7 @@
       <c r="E15" s="231" t="s">
         <v>639</v>
       </c>
-      <c r="F15" s="244"/>
+      <c r="F15" s="243"/>
       <c r="G15" s="217"/>
       <c r="H15" s="231"/>
       <c r="I15" s="216"/>
@@ -15975,7 +15978,7 @@
       <c r="E16" s="231" t="s">
         <v>639</v>
       </c>
-      <c r="F16" s="244"/>
+      <c r="F16" s="243"/>
       <c r="G16" s="217"/>
       <c r="H16" s="231"/>
       <c r="I16" s="216"/>
@@ -16046,7 +16049,7 @@
       <c r="E19" s="231" t="s">
         <v>639</v>
       </c>
-      <c r="F19" s="244"/>
+      <c r="F19" s="243"/>
       <c r="G19" s="217"/>
       <c r="H19" s="231"/>
       <c r="I19" s="216"/>
@@ -16073,7 +16076,7 @@
       <c r="E20" s="231" t="s">
         <v>639</v>
       </c>
-      <c r="F20" s="244"/>
+      <c r="F20" s="243"/>
       <c r="G20" s="217"/>
       <c r="H20" s="231"/>
       <c r="I20" s="216"/>
@@ -16144,7 +16147,7 @@
       <c r="E23" s="231" t="s">
         <v>639</v>
       </c>
-      <c r="F23" s="244"/>
+      <c r="F23" s="243"/>
       <c r="G23" s="217"/>
       <c r="H23" s="231"/>
       <c r="I23" s="216"/>
@@ -16160,12 +16163,12 @@
       <c r="T23" s="308"/>
       <c r="U23" s="309"/>
     </row>
-    <row r="24" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="24" spans="2:21" ht="20.25" customHeight="1">
       <c r="B24" s="218"/>
       <c r="C24" s="229"/>
       <c r="D24" s="218"/>
       <c r="E24" s="231"/>
-      <c r="F24" s="314"/>
+      <c r="F24" s="232"/>
       <c r="G24" s="217"/>
       <c r="H24" s="231"/>
       <c r="I24" s="216"/>
@@ -16181,14 +16184,14 @@
       <c r="T24" s="308"/>
       <c r="U24" s="309"/>
     </row>
-    <row r="25" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="25" spans="2:21" ht="20.25" customHeight="1">
       <c r="B25" s="242" t="s">
         <v>630</v>
       </c>
       <c r="C25" s="229"/>
       <c r="D25" s="218"/>
       <c r="E25" s="231"/>
-      <c r="F25" s="314"/>
+      <c r="F25" s="232"/>
       <c r="G25" s="217"/>
       <c r="H25" s="231"/>
       <c r="I25" s="216"/>
@@ -16204,7 +16207,7 @@
       <c r="T25" s="308"/>
       <c r="U25" s="309"/>
     </row>
-    <row r="26" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="26" spans="2:21" ht="20.25" customHeight="1">
       <c r="B26" s="218"/>
       <c r="C26" s="229" t="s">
         <v>647</v>
@@ -16213,7 +16216,7 @@
         <v>648</v>
       </c>
       <c r="E26" s="231"/>
-      <c r="F26" s="314"/>
+      <c r="F26" s="232"/>
       <c r="G26" s="217"/>
       <c r="H26" s="231"/>
       <c r="I26" s="216"/>
@@ -16229,7 +16232,7 @@
       <c r="T26" s="308"/>
       <c r="U26" s="309"/>
     </row>
-    <row r="27" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="27" spans="2:21" ht="20.25" customHeight="1">
       <c r="B27" s="218"/>
       <c r="C27" s="229" t="s">
         <v>646</v>
@@ -16238,7 +16241,7 @@
         <v>648</v>
       </c>
       <c r="E27" s="231"/>
-      <c r="F27" s="314"/>
+      <c r="F27" s="232"/>
       <c r="G27" s="217"/>
       <c r="H27" s="231"/>
       <c r="I27" s="216"/>
@@ -16254,7 +16257,7 @@
       <c r="T27" s="308"/>
       <c r="U27" s="309"/>
     </row>
-    <row r="28" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="28" spans="2:21" ht="20.25" customHeight="1">
       <c r="B28" s="242" t="s">
         <v>360</v>
       </c>
@@ -16288,7 +16291,7 @@
       <c r="E29" s="231" t="s">
         <v>639</v>
       </c>
-      <c r="F29" s="244"/>
+      <c r="F29" s="243"/>
       <c r="G29" s="217"/>
       <c r="H29" s="231"/>
       <c r="I29" s="216"/>
@@ -16304,7 +16307,7 @@
       <c r="T29" s="308"/>
       <c r="U29" s="309"/>
     </row>
-    <row r="30" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="30" spans="2:21" ht="20.25" customHeight="1">
       <c r="B30" s="242"/>
       <c r="C30" s="229" t="s">
         <v>644</v>
@@ -16313,10 +16316,12 @@
         <v>643</v>
       </c>
       <c r="E30" s="231"/>
-      <c r="F30" s="314"/>
+      <c r="F30" s="232"/>
       <c r="G30" s="217"/>
-      <c r="H30" s="231"/>
-      <c r="I30" s="216"/>
+      <c r="H30" s="244" t="s">
+        <v>654</v>
+      </c>
+      <c r="I30" s="243"/>
       <c r="J30" s="217"/>
       <c r="K30" s="231"/>
       <c r="L30" s="216"/>
@@ -16329,14 +16334,14 @@
       <c r="T30" s="308"/>
       <c r="U30" s="309"/>
     </row>
-    <row r="31" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="31" spans="2:21" ht="20.25" customHeight="1">
       <c r="B31" s="242" t="s">
         <v>649</v>
       </c>
       <c r="C31" s="229"/>
       <c r="D31" s="218"/>
       <c r="E31" s="231"/>
-      <c r="F31" s="314"/>
+      <c r="F31" s="232"/>
       <c r="G31" s="217"/>
       <c r="H31" s="231"/>
       <c r="I31" s="216"/>
@@ -16352,7 +16357,7 @@
       <c r="T31" s="308"/>
       <c r="U31" s="309"/>
     </row>
-    <row r="32" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="32" spans="2:21" ht="20.25" customHeight="1">
       <c r="B32" s="242"/>
       <c r="C32" s="229" t="s">
         <v>650</v>
@@ -16361,10 +16366,12 @@
         <v>643</v>
       </c>
       <c r="E32" s="231"/>
-      <c r="F32" s="314"/>
+      <c r="F32" s="232"/>
       <c r="G32" s="217"/>
-      <c r="H32" s="231"/>
-      <c r="I32" s="216"/>
+      <c r="H32" s="244" t="s">
+        <v>654</v>
+      </c>
+      <c r="I32" s="243"/>
       <c r="J32" s="217"/>
       <c r="K32" s="231"/>
       <c r="L32" s="216"/>
@@ -16377,7 +16384,7 @@
       <c r="T32" s="308"/>
       <c r="U32" s="309"/>
     </row>
-    <row r="33" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="33" spans="2:21" ht="20.25" customHeight="1">
       <c r="B33" s="242"/>
       <c r="C33" s="229" t="s">
         <v>651</v>
@@ -16386,10 +16393,12 @@
         <v>643</v>
       </c>
       <c r="E33" s="231"/>
-      <c r="F33" s="314"/>
+      <c r="F33" s="232"/>
       <c r="G33" s="217"/>
-      <c r="H33" s="231"/>
-      <c r="I33" s="216"/>
+      <c r="H33" s="244" t="s">
+        <v>654</v>
+      </c>
+      <c r="I33" s="243"/>
       <c r="J33" s="217"/>
       <c r="K33" s="231"/>
       <c r="L33" s="216"/>
@@ -16402,14 +16411,14 @@
       <c r="T33" s="308"/>
       <c r="U33" s="309"/>
     </row>
-    <row r="34" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="34" spans="2:21" ht="20.25" customHeight="1">
       <c r="B34" s="242" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C34" s="229"/>
       <c r="D34" s="218"/>
       <c r="E34" s="231"/>
-      <c r="F34" s="314"/>
+      <c r="F34" s="232"/>
       <c r="G34" s="217"/>
       <c r="H34" s="231"/>
       <c r="I34" s="216"/>
@@ -16425,7 +16434,7 @@
       <c r="T34" s="308"/>
       <c r="U34" s="309"/>
     </row>
-    <row r="35" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="35" spans="2:21" ht="20.25" customHeight="1">
       <c r="B35" s="242"/>
       <c r="C35" s="229" t="s">
         <v>652</v>
@@ -16434,10 +16443,12 @@
         <v>643</v>
       </c>
       <c r="E35" s="231"/>
-      <c r="F35" s="314"/>
+      <c r="F35" s="232"/>
       <c r="G35" s="217"/>
-      <c r="H35" s="231"/>
-      <c r="I35" s="216"/>
+      <c r="H35" s="244" t="s">
+        <v>654</v>
+      </c>
+      <c r="I35" s="243"/>
       <c r="J35" s="217"/>
       <c r="K35" s="231"/>
       <c r="L35" s="216"/>
@@ -16450,14 +16461,12 @@
       <c r="T35" s="308"/>
       <c r="U35" s="309"/>
     </row>
-    <row r="36" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
-      <c r="B36" s="242" t="s">
-        <v>362</v>
-      </c>
+    <row r="36" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B36" s="242"/>
       <c r="C36" s="229"/>
       <c r="D36" s="218"/>
       <c r="E36" s="231"/>
-      <c r="F36" s="314"/>
+      <c r="F36" s="232"/>
       <c r="G36" s="217"/>
       <c r="H36" s="231"/>
       <c r="I36" s="216"/>
@@ -16473,16 +16482,12 @@
       <c r="T36" s="308"/>
       <c r="U36" s="309"/>
     </row>
-    <row r="37" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="37" spans="2:21" ht="20.25" customHeight="1">
       <c r="B37" s="242"/>
-      <c r="C37" s="229" t="s">
-        <v>652</v>
-      </c>
-      <c r="D37" s="218" t="s">
-        <v>643</v>
-      </c>
+      <c r="C37" s="229"/>
+      <c r="D37" s="218"/>
       <c r="E37" s="231"/>
-      <c r="F37" s="314"/>
+      <c r="F37" s="232"/>
       <c r="G37" s="217"/>
       <c r="H37" s="231"/>
       <c r="I37" s="216"/>
@@ -16498,12 +16503,14 @@
       <c r="T37" s="308"/>
       <c r="U37" s="309"/>
     </row>
-    <row r="38" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
-      <c r="B38" s="242"/>
-      <c r="C38" s="229"/>
+    <row r="38" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B38" s="242" t="s">
+        <v>425</v>
+      </c>
+      <c r="C38" s="218"/>
       <c r="D38" s="218"/>
       <c r="E38" s="231"/>
-      <c r="F38" s="314"/>
+      <c r="F38" s="232"/>
       <c r="G38" s="217"/>
       <c r="H38" s="231"/>
       <c r="I38" s="216"/>
@@ -16519,15 +16526,21 @@
       <c r="T38" s="308"/>
       <c r="U38" s="309"/>
     </row>
-    <row r="39" spans="2:21" s="243" customFormat="1" ht="20.25" customHeight="1">
+    <row r="39" spans="2:21" ht="20.25" customHeight="1">
       <c r="B39" s="242"/>
-      <c r="C39" s="229"/>
-      <c r="D39" s="218"/>
+      <c r="C39" s="229" t="s">
+        <v>645</v>
+      </c>
+      <c r="D39" s="218" t="s">
+        <v>653</v>
+      </c>
       <c r="E39" s="231"/>
-      <c r="F39" s="314"/>
+      <c r="F39" s="232"/>
       <c r="G39" s="217"/>
-      <c r="H39" s="231"/>
-      <c r="I39" s="216"/>
+      <c r="H39" s="244" t="s">
+        <v>654</v>
+      </c>
+      <c r="I39" s="243"/>
       <c r="J39" s="217"/>
       <c r="K39" s="231"/>
       <c r="L39" s="216"/>
@@ -16541,16 +16554,20 @@
       <c r="U39" s="309"/>
     </row>
     <row r="40" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B40" s="242" t="s">
-        <v>425</v>
-      </c>
-      <c r="C40" s="218"/>
-      <c r="D40" s="218"/>
+      <c r="B40" s="242"/>
+      <c r="C40" s="229" t="s">
+        <v>635</v>
+      </c>
+      <c r="D40" s="218" t="s">
+        <v>653</v>
+      </c>
       <c r="E40" s="231"/>
       <c r="F40" s="232"/>
       <c r="G40" s="217"/>
-      <c r="H40" s="231"/>
-      <c r="I40" s="216"/>
+      <c r="H40" s="244" t="s">
+        <v>654</v>
+      </c>
+      <c r="I40" s="243"/>
       <c r="J40" s="217"/>
       <c r="K40" s="231"/>
       <c r="L40" s="216"/>
@@ -16565,12 +16582,8 @@
     </row>
     <row r="41" spans="2:21" ht="20.25" customHeight="1">
       <c r="B41" s="242"/>
-      <c r="C41" s="229" t="s">
-        <v>645</v>
-      </c>
-      <c r="D41" s="229" t="s">
-        <v>653</v>
-      </c>
+      <c r="C41" s="218"/>
+      <c r="D41" s="218"/>
       <c r="E41" s="231"/>
       <c r="F41" s="232"/>
       <c r="G41" s="217"/>
@@ -16590,12 +16603,7 @@
     </row>
     <row r="42" spans="2:21" ht="20.25" customHeight="1">
       <c r="B42" s="242"/>
-      <c r="C42" s="229" t="s">
-        <v>635</v>
-      </c>
-      <c r="D42" s="229" t="s">
-        <v>653</v>
-      </c>
+      <c r="D42" s="218"/>
       <c r="E42" s="231"/>
       <c r="F42" s="232"/>
       <c r="G42" s="217"/>
@@ -16614,7 +16622,9 @@
       <c r="U42" s="309"/>
     </row>
     <row r="43" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B43" s="242"/>
+      <c r="B43" s="242" t="s">
+        <v>479</v>
+      </c>
       <c r="C43" s="218"/>
       <c r="D43" s="218"/>
       <c r="E43" s="231"/>
@@ -16636,6 +16646,9 @@
     </row>
     <row r="44" spans="2:21" ht="20.25" customHeight="1">
       <c r="B44" s="242"/>
+      <c r="C44" s="229" t="s">
+        <v>636</v>
+      </c>
       <c r="D44" s="218"/>
       <c r="E44" s="231"/>
       <c r="F44" s="232"/>
@@ -16655,10 +16668,7 @@
       <c r="U44" s="309"/>
     </row>
     <row r="45" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B45" s="242" t="s">
-        <v>479</v>
-      </c>
-      <c r="C45" s="218"/>
+      <c r="B45" s="242"/>
       <c r="D45" s="218"/>
       <c r="E45" s="231"/>
       <c r="F45" s="232"/>
@@ -16678,10 +16688,10 @@
       <c r="U45" s="309"/>
     </row>
     <row r="46" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B46" s="242"/>
-      <c r="C46" s="229" t="s">
-        <v>636</v>
-      </c>
+      <c r="B46" s="242" t="s">
+        <v>427</v>
+      </c>
+      <c r="C46" s="218"/>
       <c r="D46" s="218"/>
       <c r="E46" s="231"/>
       <c r="F46" s="232"/>
@@ -16701,7 +16711,10 @@
       <c r="U46" s="309"/>
     </row>
     <row r="47" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B47" s="242"/>
+      <c r="B47" s="218"/>
+      <c r="C47" s="229" t="s">
+        <v>636</v>
+      </c>
       <c r="D47" s="218"/>
       <c r="E47" s="231"/>
       <c r="F47" s="232"/>
@@ -16721,9 +16734,7 @@
       <c r="U47" s="309"/>
     </row>
     <row r="48" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B48" s="242" t="s">
-        <v>427</v>
-      </c>
+      <c r="B48" s="218"/>
       <c r="C48" s="218"/>
       <c r="D48" s="218"/>
       <c r="E48" s="231"/>
@@ -16745,9 +16756,7 @@
     </row>
     <row r="49" spans="2:21" ht="20.25" customHeight="1">
       <c r="B49" s="218"/>
-      <c r="C49" s="229" t="s">
-        <v>636</v>
-      </c>
+      <c r="C49" s="218"/>
       <c r="D49" s="218"/>
       <c r="E49" s="231"/>
       <c r="F49" s="232"/>
@@ -19647,18 +19656,18 @@
       <c r="B187" s="218"/>
       <c r="C187" s="218"/>
       <c r="D187" s="218"/>
-      <c r="E187" s="231"/>
-      <c r="F187" s="232"/>
-      <c r="G187" s="217"/>
-      <c r="H187" s="231"/>
-      <c r="I187" s="216"/>
-      <c r="J187" s="217"/>
-      <c r="K187" s="231"/>
-      <c r="L187" s="216"/>
-      <c r="M187" s="217"/>
-      <c r="N187" s="231"/>
-      <c r="O187" s="216"/>
-      <c r="P187" s="217"/>
+      <c r="E187" s="219"/>
+      <c r="F187" s="220"/>
+      <c r="G187" s="221"/>
+      <c r="H187" s="219"/>
+      <c r="I187" s="218"/>
+      <c r="J187" s="221"/>
+      <c r="K187" s="219"/>
+      <c r="L187" s="218"/>
+      <c r="M187" s="221"/>
+      <c r="N187" s="219"/>
+      <c r="O187" s="218"/>
+      <c r="P187" s="221"/>
       <c r="R187" s="307"/>
       <c r="S187" s="308"/>
       <c r="T187" s="308"/>
@@ -19668,18 +19677,18 @@
       <c r="B188" s="218"/>
       <c r="C188" s="218"/>
       <c r="D188" s="218"/>
-      <c r="E188" s="231"/>
-      <c r="F188" s="232"/>
-      <c r="G188" s="217"/>
-      <c r="H188" s="231"/>
-      <c r="I188" s="216"/>
-      <c r="J188" s="217"/>
-      <c r="K188" s="231"/>
-      <c r="L188" s="216"/>
-      <c r="M188" s="217"/>
-      <c r="N188" s="231"/>
-      <c r="O188" s="216"/>
-      <c r="P188" s="217"/>
+      <c r="E188" s="222"/>
+      <c r="F188" s="218"/>
+      <c r="G188" s="221"/>
+      <c r="H188" s="222"/>
+      <c r="I188" s="218"/>
+      <c r="J188" s="221"/>
+      <c r="K188" s="222"/>
+      <c r="L188" s="218"/>
+      <c r="M188" s="221"/>
+      <c r="N188" s="222"/>
+      <c r="O188" s="218"/>
+      <c r="P188" s="221"/>
       <c r="R188" s="307"/>
       <c r="S188" s="308"/>
       <c r="T188" s="308"/>
@@ -19689,16 +19698,16 @@
       <c r="B189" s="218"/>
       <c r="C189" s="218"/>
       <c r="D189" s="218"/>
-      <c r="E189" s="219"/>
-      <c r="F189" s="220"/>
+      <c r="E189" s="222"/>
+      <c r="F189" s="218"/>
       <c r="G189" s="221"/>
-      <c r="H189" s="219"/>
+      <c r="H189" s="222"/>
       <c r="I189" s="218"/>
       <c r="J189" s="221"/>
-      <c r="K189" s="219"/>
+      <c r="K189" s="222"/>
       <c r="L189" s="218"/>
       <c r="M189" s="221"/>
-      <c r="N189" s="219"/>
+      <c r="N189" s="222"/>
       <c r="O189" s="218"/>
       <c r="P189" s="221"/>
       <c r="R189" s="307"/>
@@ -19710,18 +19719,18 @@
       <c r="B190" s="218"/>
       <c r="C190" s="218"/>
       <c r="D190" s="218"/>
-      <c r="E190" s="222"/>
-      <c r="F190" s="218"/>
-      <c r="G190" s="221"/>
-      <c r="H190" s="222"/>
-      <c r="I190" s="218"/>
-      <c r="J190" s="221"/>
-      <c r="K190" s="222"/>
-      <c r="L190" s="218"/>
-      <c r="M190" s="221"/>
-      <c r="N190" s="222"/>
-      <c r="O190" s="218"/>
-      <c r="P190" s="221"/>
+      <c r="E190" s="219"/>
+      <c r="F190" s="223"/>
+      <c r="G190" s="224"/>
+      <c r="H190" s="219"/>
+      <c r="I190" s="223"/>
+      <c r="J190" s="224"/>
+      <c r="K190" s="219"/>
+      <c r="L190" s="223"/>
+      <c r="M190" s="224"/>
+      <c r="N190" s="219"/>
+      <c r="O190" s="223"/>
+      <c r="P190" s="224"/>
       <c r="R190" s="307"/>
       <c r="S190" s="308"/>
       <c r="T190" s="308"/>
@@ -19732,36 +19741,36 @@
       <c r="C191" s="218"/>
       <c r="D191" s="218"/>
       <c r="E191" s="222"/>
-      <c r="F191" s="218"/>
-      <c r="G191" s="221"/>
+      <c r="F191" s="223"/>
+      <c r="G191" s="224"/>
       <c r="H191" s="222"/>
-      <c r="I191" s="218"/>
-      <c r="J191" s="221"/>
+      <c r="I191" s="223"/>
+      <c r="J191" s="224"/>
       <c r="K191" s="222"/>
-      <c r="L191" s="218"/>
-      <c r="M191" s="221"/>
+      <c r="L191" s="223"/>
+      <c r="M191" s="224"/>
       <c r="N191" s="222"/>
-      <c r="O191" s="218"/>
-      <c r="P191" s="221"/>
+      <c r="O191" s="223"/>
+      <c r="P191" s="224"/>
       <c r="R191" s="307"/>
       <c r="S191" s="308"/>
       <c r="T191" s="308"/>
       <c r="U191" s="309"/>
     </row>
     <row r="192" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B192" s="218"/>
+      <c r="B192" s="229"/>
       <c r="C192" s="218"/>
       <c r="D192" s="218"/>
-      <c r="E192" s="219"/>
+      <c r="E192" s="222"/>
       <c r="F192" s="223"/>
       <c r="G192" s="224"/>
-      <c r="H192" s="219"/>
+      <c r="H192" s="222"/>
       <c r="I192" s="223"/>
       <c r="J192" s="224"/>
-      <c r="K192" s="219"/>
+      <c r="K192" s="222"/>
       <c r="L192" s="223"/>
       <c r="M192" s="224"/>
-      <c r="N192" s="219"/>
+      <c r="N192" s="222"/>
       <c r="O192" s="223"/>
       <c r="P192" s="224"/>
       <c r="R192" s="307"/>
@@ -19773,16 +19782,16 @@
       <c r="B193" s="218"/>
       <c r="C193" s="218"/>
       <c r="D193" s="218"/>
-      <c r="E193" s="222"/>
+      <c r="E193" s="219"/>
       <c r="F193" s="223"/>
       <c r="G193" s="224"/>
-      <c r="H193" s="222"/>
+      <c r="H193" s="219"/>
       <c r="I193" s="223"/>
       <c r="J193" s="224"/>
-      <c r="K193" s="222"/>
+      <c r="K193" s="219"/>
       <c r="L193" s="223"/>
       <c r="M193" s="224"/>
-      <c r="N193" s="222"/>
+      <c r="N193" s="219"/>
       <c r="O193" s="223"/>
       <c r="P193" s="224"/>
       <c r="R193" s="307"/>
@@ -19791,7 +19800,7 @@
       <c r="U193" s="309"/>
     </row>
     <row r="194" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B194" s="229"/>
+      <c r="B194" s="218"/>
       <c r="C194" s="218"/>
       <c r="D194" s="218"/>
       <c r="E194" s="222"/>
@@ -19815,16 +19824,16 @@
       <c r="B195" s="218"/>
       <c r="C195" s="218"/>
       <c r="D195" s="218"/>
-      <c r="E195" s="219"/>
+      <c r="E195" s="222"/>
       <c r="F195" s="223"/>
       <c r="G195" s="224"/>
-      <c r="H195" s="219"/>
+      <c r="H195" s="222"/>
       <c r="I195" s="223"/>
       <c r="J195" s="224"/>
-      <c r="K195" s="219"/>
+      <c r="K195" s="222"/>
       <c r="L195" s="223"/>
       <c r="M195" s="224"/>
-      <c r="N195" s="219"/>
+      <c r="N195" s="222"/>
       <c r="O195" s="223"/>
       <c r="P195" s="224"/>
       <c r="R195" s="307"/>
@@ -19836,16 +19845,16 @@
       <c r="B196" s="218"/>
       <c r="C196" s="218"/>
       <c r="D196" s="218"/>
-      <c r="E196" s="222"/>
+      <c r="E196" s="219"/>
       <c r="F196" s="223"/>
       <c r="G196" s="224"/>
-      <c r="H196" s="222"/>
+      <c r="H196" s="219"/>
       <c r="I196" s="223"/>
       <c r="J196" s="224"/>
-      <c r="K196" s="222"/>
+      <c r="K196" s="219"/>
       <c r="L196" s="223"/>
       <c r="M196" s="224"/>
-      <c r="N196" s="222"/>
+      <c r="N196" s="219"/>
       <c r="O196" s="223"/>
       <c r="P196" s="224"/>
       <c r="R196" s="307"/>
@@ -19853,120 +19862,78 @@
       <c r="T196" s="308"/>
       <c r="U196" s="309"/>
     </row>
-    <row r="197" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B197" s="218"/>
-      <c r="C197" s="218"/>
-      <c r="D197" s="218"/>
-      <c r="E197" s="222"/>
-      <c r="F197" s="223"/>
-      <c r="G197" s="224"/>
-      <c r="H197" s="222"/>
-      <c r="I197" s="223"/>
-      <c r="J197" s="224"/>
-      <c r="K197" s="222"/>
-      <c r="L197" s="223"/>
-      <c r="M197" s="224"/>
-      <c r="N197" s="222"/>
-      <c r="O197" s="223"/>
-      <c r="P197" s="224"/>
-      <c r="R197" s="307"/>
-      <c r="S197" s="308"/>
-      <c r="T197" s="308"/>
-      <c r="U197" s="309"/>
-    </row>
-    <row r="198" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B198" s="218"/>
-      <c r="C198" s="218"/>
-      <c r="D198" s="218"/>
-      <c r="E198" s="219"/>
-      <c r="F198" s="223"/>
-      <c r="G198" s="224"/>
-      <c r="H198" s="219"/>
-      <c r="I198" s="223"/>
-      <c r="J198" s="224"/>
-      <c r="K198" s="219"/>
-      <c r="L198" s="223"/>
-      <c r="M198" s="224"/>
-      <c r="N198" s="219"/>
-      <c r="O198" s="223"/>
-      <c r="P198" s="224"/>
-      <c r="R198" s="307"/>
-      <c r="S198" s="308"/>
-      <c r="T198" s="308"/>
-      <c r="U198" s="309"/>
-    </row>
-    <row r="199" spans="2:21" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B199" s="225"/>
-      <c r="C199" s="226"/>
-      <c r="D199" s="227"/>
-      <c r="E199" s="230"/>
-      <c r="F199" s="226"/>
-      <c r="G199" s="228"/>
-      <c r="H199" s="230"/>
-      <c r="I199" s="226"/>
-      <c r="J199" s="228"/>
-      <c r="K199" s="230"/>
-      <c r="L199" s="226"/>
-      <c r="M199" s="228"/>
-      <c r="N199" s="230"/>
-      <c r="O199" s="226"/>
-      <c r="P199" s="228"/>
-      <c r="R199" s="310"/>
-      <c r="S199" s="311"/>
-      <c r="T199" s="311"/>
-      <c r="U199" s="312"/>
-    </row>
-    <row r="200" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B200" s="186"/>
-      <c r="C200" s="186"/>
-      <c r="D200" s="186"/>
-      <c r="E200" s="186"/>
-      <c r="F200" s="186"/>
-      <c r="G200" s="186"/>
-      <c r="H200" s="186"/>
-      <c r="I200" s="186"/>
-      <c r="J200" s="186"/>
-      <c r="K200" s="186"/>
-      <c r="L200" s="186"/>
-      <c r="M200" s="186"/>
-      <c r="N200" s="186"/>
-      <c r="O200" s="186"/>
-      <c r="P200" s="186"/>
-      <c r="Q200" s="186"/>
+    <row r="197" spans="2:21" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B197" s="225"/>
+      <c r="C197" s="226"/>
+      <c r="D197" s="227"/>
+      <c r="E197" s="230"/>
+      <c r="F197" s="226"/>
+      <c r="G197" s="228"/>
+      <c r="H197" s="230"/>
+      <c r="I197" s="226"/>
+      <c r="J197" s="228"/>
+      <c r="K197" s="230"/>
+      <c r="L197" s="226"/>
+      <c r="M197" s="228"/>
+      <c r="N197" s="230"/>
+      <c r="O197" s="226"/>
+      <c r="P197" s="228"/>
+      <c r="R197" s="310"/>
+      <c r="S197" s="311"/>
+      <c r="T197" s="311"/>
+      <c r="U197" s="312"/>
+    </row>
+    <row r="198" spans="2:21" ht="15.75" customHeight="1">
+      <c r="B198" s="186"/>
+      <c r="C198" s="186"/>
+      <c r="D198" s="186"/>
+      <c r="E198" s="186"/>
+      <c r="F198" s="186"/>
+      <c r="G198" s="186"/>
+      <c r="H198" s="186"/>
+      <c r="I198" s="186"/>
+      <c r="J198" s="186"/>
+      <c r="K198" s="186"/>
+      <c r="L198" s="186"/>
+      <c r="M198" s="186"/>
+      <c r="N198" s="186"/>
+      <c r="O198" s="186"/>
+      <c r="P198" s="186"/>
+      <c r="Q198" s="186"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="H3:P3"/>
-    <mergeCell ref="R6:U199"/>
+    <mergeCell ref="R6:U197"/>
   </mergeCells>
-  <conditionalFormatting sqref="D40:D198 B28:B198 B12:D27 C42 C28:C34 C36:C40 C45:C46 C49:C205">
-    <cfRule type="expression" dxfId="5" priority="2">
+  <conditionalFormatting sqref="B12:D27 C28:C38 B28:B196 D38 C40 C43:C44 C47:C203 D41:D196">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>IF((B12&lt;&gt;"")*AND(F12&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41 C43">
-    <cfRule type="expression" dxfId="4" priority="4">
-      <formula>IF((C41&lt;&gt;"")*AND(G42&lt;&gt;""),1,0)</formula>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>IF((C35&lt;&gt;"")*AND(G38&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28:D39">
-    <cfRule type="expression" dxfId="3" priority="9">
+  <conditionalFormatting sqref="C39 C41">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>IF((C39&lt;&gt;"")*AND(G40&lt;&gt;""),1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="expression" dxfId="2" priority="14">
+      <formula>IF((C46&lt;&gt;"")*AND(G45&lt;&gt;""),1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:D37">
+    <cfRule type="expression" dxfId="1" priority="10">
       <formula>IF((C28&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="2" priority="11">
-      <formula>IF((C35&lt;&gt;"")*AND(G38&lt;&gt;""),1,0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>IF((C37&lt;&gt;"")*AND(G40&lt;&gt;""),1,0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="0" priority="13">
-      <formula>IF((C48&lt;&gt;"")*AND(G47&lt;&gt;""),1,0)</formula>
+  <conditionalFormatting sqref="D39:D40">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>IF((D39&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
add : maj chiffrier fix : erreur logique
</commit_message>
<xml_diff>
--- a/doc/chiffrier_sim_vie.xlsx
+++ b/doc/chiffrier_sim_vie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travail\sim_vie\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACE011D-EBC5-4434-A56F-45A41A297269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C994FE-BE65-4586-9275-53CF16CB40CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Méthodes SCRUM" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="673">
   <si>
     <t>Chiffrier de documentation de projets</t>
   </si>
@@ -2203,6 +2203,60 @@
   </si>
   <si>
     <t>05/12/2025</t>
+  </si>
+  <si>
+    <t>Expérimentations neuronales</t>
+  </si>
+  <si>
+    <t>Tenter un système d'accumulation des stimulis</t>
+  </si>
+  <si>
+    <t>Explorer l'orientation pour la rendre plus fluide</t>
+  </si>
+  <si>
+    <t>Réduire le champ sensoriel</t>
+  </si>
+  <si>
+    <t>Incorporer immobilisation de la créature</t>
+  </si>
+  <si>
+    <t>Ajouter une notion de : ça prend du temps pour manger</t>
+  </si>
+  <si>
+    <t>Vérifiier si on peut implémenter un peu plus de gestion de jauges dans l'action manger</t>
+  </si>
+  <si>
+    <t>Actions</t>
+  </si>
+  <si>
+    <t>Manger :</t>
+  </si>
+  <si>
+    <t>Reproduction :</t>
+  </si>
+  <si>
+    <t>Une notion de temps</t>
+  </si>
+  <si>
+    <t>Créer une nouvelle créature</t>
+  </si>
+  <si>
+    <t>Revoir les jauges qui sont concernés par cette action (envie_reproduction dans maj)</t>
+  </si>
+  <si>
+    <t>Interface :</t>
+  </si>
+  <si>
+    <t>Créer le deuxième onglet (infos créatures)</t>
+  </si>
+  <si>
+    <t>Ajouter la connexion des jauges à l'onglet</t>
+  </si>
+  <si>
+    <t>Ajouter la gestion de clique sur une créature</t>
+  </si>
+  <si>
+    <t>Effacer les créatures qui sont mortes</t>
   </si>
 </sst>
 </file>
@@ -4034,14 +4088,110 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -4052,110 +4202,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4163,18 +4229,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4213,7 +4267,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="0" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="0" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="0" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment wrapText="0" shrinkToFit="0"/>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -7492,16 +7606,16 @@
       <c r="W10" s="29"/>
     </row>
     <row r="11" spans="1:107" thickBot="1">
-      <c r="G11" s="261" t="s">
+      <c r="G11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="H11" s="262"/>
-      <c r="I11" s="262"/>
-      <c r="J11" s="262"/>
-      <c r="K11" s="262"/>
-      <c r="L11" s="262"/>
-      <c r="M11" s="262"/>
-      <c r="N11" s="263"/>
+      <c r="H11" s="282"/>
+      <c r="I11" s="282"/>
+      <c r="J11" s="282"/>
+      <c r="K11" s="282"/>
+      <c r="L11" s="282"/>
+      <c r="M11" s="282"/>
+      <c r="N11" s="283"/>
       <c r="O11" s="48"/>
       <c r="P11" s="39"/>
       <c r="Q11" s="39"/>
@@ -7539,66 +7653,66 @@
       <c r="AW11" s="47"/>
       <c r="AX11" s="113"/>
       <c r="AY11" s="115"/>
-      <c r="BD11" s="261" t="s">
+      <c r="BD11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="BE11" s="262"/>
-      <c r="BF11" s="262"/>
-      <c r="BG11" s="262"/>
-      <c r="BH11" s="262"/>
-      <c r="BI11" s="262"/>
-      <c r="BJ11" s="262"/>
-      <c r="BK11" s="263"/>
-      <c r="BP11" s="261" t="s">
+      <c r="BE11" s="282"/>
+      <c r="BF11" s="282"/>
+      <c r="BG11" s="282"/>
+      <c r="BH11" s="282"/>
+      <c r="BI11" s="282"/>
+      <c r="BJ11" s="282"/>
+      <c r="BK11" s="283"/>
+      <c r="BP11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="BQ11" s="262"/>
-      <c r="BR11" s="262"/>
-      <c r="BS11" s="262"/>
-      <c r="BT11" s="262"/>
-      <c r="BU11" s="262"/>
-      <c r="BV11" s="262"/>
-      <c r="BW11" s="263"/>
-      <c r="CA11" s="261" t="s">
+      <c r="BQ11" s="282"/>
+      <c r="BR11" s="282"/>
+      <c r="BS11" s="282"/>
+      <c r="BT11" s="282"/>
+      <c r="BU11" s="282"/>
+      <c r="BV11" s="282"/>
+      <c r="BW11" s="283"/>
+      <c r="CA11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="CB11" s="262"/>
-      <c r="CC11" s="262"/>
-      <c r="CD11" s="262"/>
-      <c r="CE11" s="262"/>
-      <c r="CF11" s="262"/>
-      <c r="CG11" s="262"/>
-      <c r="CH11" s="263"/>
-      <c r="CL11" s="261" t="s">
+      <c r="CB11" s="282"/>
+      <c r="CC11" s="282"/>
+      <c r="CD11" s="282"/>
+      <c r="CE11" s="282"/>
+      <c r="CF11" s="282"/>
+      <c r="CG11" s="282"/>
+      <c r="CH11" s="283"/>
+      <c r="CL11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="CM11" s="262"/>
-      <c r="CN11" s="262"/>
-      <c r="CO11" s="262"/>
-      <c r="CP11" s="262"/>
-      <c r="CQ11" s="262"/>
-      <c r="CR11" s="262"/>
-      <c r="CS11" s="263"/>
-      <c r="CV11" s="261" t="s">
+      <c r="CM11" s="282"/>
+      <c r="CN11" s="282"/>
+      <c r="CO11" s="282"/>
+      <c r="CP11" s="282"/>
+      <c r="CQ11" s="282"/>
+      <c r="CR11" s="282"/>
+      <c r="CS11" s="283"/>
+      <c r="CV11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="CW11" s="262"/>
-      <c r="CX11" s="262"/>
-      <c r="CY11" s="262"/>
-      <c r="CZ11" s="262"/>
-      <c r="DA11" s="262"/>
-      <c r="DB11" s="262"/>
-      <c r="DC11" s="263"/>
+      <c r="CW11" s="282"/>
+      <c r="CX11" s="282"/>
+      <c r="CY11" s="282"/>
+      <c r="CZ11" s="282"/>
+      <c r="DA11" s="282"/>
+      <c r="DB11" s="282"/>
+      <c r="DC11" s="283"/>
     </row>
     <row r="12" spans="1:107" thickBot="1">
-      <c r="G12" s="264"/>
-      <c r="H12" s="265"/>
-      <c r="I12" s="265"/>
-      <c r="J12" s="265"/>
-      <c r="K12" s="265"/>
-      <c r="L12" s="265"/>
-      <c r="M12" s="265"/>
-      <c r="N12" s="266"/>
+      <c r="G12" s="284"/>
+      <c r="H12" s="285"/>
+      <c r="I12" s="285"/>
+      <c r="J12" s="285"/>
+      <c r="K12" s="285"/>
+      <c r="L12" s="285"/>
+      <c r="M12" s="285"/>
+      <c r="N12" s="286"/>
       <c r="O12" s="40"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
@@ -7609,49 +7723,49 @@
       <c r="V12" s="29"/>
       <c r="W12" s="29"/>
       <c r="AX12" s="42"/>
-      <c r="AY12" s="258" t="s">
+      <c r="AY12" s="290" t="s">
         <v>323</v>
       </c>
-      <c r="BD12" s="264"/>
-      <c r="BE12" s="265"/>
-      <c r="BF12" s="265"/>
-      <c r="BG12" s="265"/>
-      <c r="BH12" s="265"/>
-      <c r="BI12" s="265"/>
-      <c r="BJ12" s="265"/>
-      <c r="BK12" s="266"/>
-      <c r="BP12" s="264"/>
-      <c r="BQ12" s="265"/>
-      <c r="BR12" s="265"/>
-      <c r="BS12" s="265"/>
-      <c r="BT12" s="265"/>
-      <c r="BU12" s="265"/>
-      <c r="BV12" s="265"/>
-      <c r="BW12" s="266"/>
-      <c r="CA12" s="264"/>
-      <c r="CB12" s="265"/>
-      <c r="CC12" s="265"/>
-      <c r="CD12" s="265"/>
-      <c r="CE12" s="265"/>
-      <c r="CF12" s="265"/>
-      <c r="CG12" s="265"/>
-      <c r="CH12" s="266"/>
-      <c r="CL12" s="264"/>
-      <c r="CM12" s="265"/>
-      <c r="CN12" s="265"/>
-      <c r="CO12" s="265"/>
-      <c r="CP12" s="265"/>
-      <c r="CQ12" s="265"/>
-      <c r="CR12" s="265"/>
-      <c r="CS12" s="266"/>
-      <c r="CV12" s="264"/>
-      <c r="CW12" s="265"/>
-      <c r="CX12" s="265"/>
-      <c r="CY12" s="265"/>
-      <c r="CZ12" s="265"/>
-      <c r="DA12" s="265"/>
-      <c r="DB12" s="265"/>
-      <c r="DC12" s="266"/>
+      <c r="BD12" s="284"/>
+      <c r="BE12" s="285"/>
+      <c r="BF12" s="285"/>
+      <c r="BG12" s="285"/>
+      <c r="BH12" s="285"/>
+      <c r="BI12" s="285"/>
+      <c r="BJ12" s="285"/>
+      <c r="BK12" s="286"/>
+      <c r="BP12" s="284"/>
+      <c r="BQ12" s="285"/>
+      <c r="BR12" s="285"/>
+      <c r="BS12" s="285"/>
+      <c r="BT12" s="285"/>
+      <c r="BU12" s="285"/>
+      <c r="BV12" s="285"/>
+      <c r="BW12" s="286"/>
+      <c r="CA12" s="284"/>
+      <c r="CB12" s="285"/>
+      <c r="CC12" s="285"/>
+      <c r="CD12" s="285"/>
+      <c r="CE12" s="285"/>
+      <c r="CF12" s="285"/>
+      <c r="CG12" s="285"/>
+      <c r="CH12" s="286"/>
+      <c r="CL12" s="284"/>
+      <c r="CM12" s="285"/>
+      <c r="CN12" s="285"/>
+      <c r="CO12" s="285"/>
+      <c r="CP12" s="285"/>
+      <c r="CQ12" s="285"/>
+      <c r="CR12" s="285"/>
+      <c r="CS12" s="286"/>
+      <c r="CV12" s="284"/>
+      <c r="CW12" s="285"/>
+      <c r="CX12" s="285"/>
+      <c r="CY12" s="285"/>
+      <c r="CZ12" s="285"/>
+      <c r="DA12" s="285"/>
+      <c r="DB12" s="285"/>
+      <c r="DC12" s="286"/>
     </row>
     <row r="13" spans="1:107" thickBot="1">
       <c r="G13" s="40"/>
@@ -7670,7 +7784,7 @@
       <c r="V13" s="29"/>
       <c r="W13" s="29"/>
       <c r="AX13" s="42"/>
-      <c r="AY13" s="259"/>
+      <c r="AY13" s="291"/>
       <c r="BD13" s="40"/>
       <c r="BG13" s="29"/>
       <c r="BH13" s="29"/>
@@ -7695,16 +7809,16 @@
       <c r="DC13" s="42"/>
     </row>
     <row r="14" spans="1:107" thickBot="1">
-      <c r="G14" s="267" t="s">
+      <c r="G14" s="287" t="s">
         <v>325</v>
       </c>
-      <c r="H14" s="268"/>
-      <c r="I14" s="268"/>
-      <c r="J14" s="268"/>
-      <c r="K14" s="268"/>
-      <c r="L14" s="268"/>
-      <c r="M14" s="268"/>
-      <c r="N14" s="269"/>
+      <c r="H14" s="288"/>
+      <c r="I14" s="288"/>
+      <c r="J14" s="288"/>
+      <c r="K14" s="288"/>
+      <c r="L14" s="288"/>
+      <c r="M14" s="288"/>
+      <c r="N14" s="289"/>
       <c r="O14" s="40"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="29"/>
@@ -7715,57 +7829,57 @@
       <c r="V14" s="29"/>
       <c r="W14" s="29"/>
       <c r="AX14" s="42"/>
-      <c r="AY14" s="259"/>
-      <c r="BD14" s="267" t="s">
+      <c r="AY14" s="291"/>
+      <c r="BD14" s="287" t="s">
         <v>338</v>
       </c>
-      <c r="BE14" s="268"/>
-      <c r="BF14" s="268"/>
-      <c r="BG14" s="268"/>
-      <c r="BH14" s="268"/>
-      <c r="BI14" s="268"/>
-      <c r="BJ14" s="268"/>
-      <c r="BK14" s="269"/>
-      <c r="BP14" s="267" t="s">
+      <c r="BE14" s="288"/>
+      <c r="BF14" s="288"/>
+      <c r="BG14" s="288"/>
+      <c r="BH14" s="288"/>
+      <c r="BI14" s="288"/>
+      <c r="BJ14" s="288"/>
+      <c r="BK14" s="289"/>
+      <c r="BP14" s="287" t="s">
         <v>327</v>
       </c>
-      <c r="BQ14" s="268"/>
-      <c r="BR14" s="268"/>
-      <c r="BS14" s="268"/>
-      <c r="BT14" s="268"/>
-      <c r="BU14" s="268"/>
-      <c r="BV14" s="268"/>
-      <c r="BW14" s="269"/>
-      <c r="CA14" s="267" t="s">
+      <c r="BQ14" s="288"/>
+      <c r="BR14" s="288"/>
+      <c r="BS14" s="288"/>
+      <c r="BT14" s="288"/>
+      <c r="BU14" s="288"/>
+      <c r="BV14" s="288"/>
+      <c r="BW14" s="289"/>
+      <c r="CA14" s="287" t="s">
         <v>326</v>
       </c>
-      <c r="CB14" s="268"/>
-      <c r="CC14" s="268"/>
-      <c r="CD14" s="268"/>
-      <c r="CE14" s="268"/>
-      <c r="CF14" s="268"/>
-      <c r="CG14" s="268"/>
-      <c r="CH14" s="269"/>
-      <c r="CL14" s="267" t="s">
+      <c r="CB14" s="288"/>
+      <c r="CC14" s="288"/>
+      <c r="CD14" s="288"/>
+      <c r="CE14" s="288"/>
+      <c r="CF14" s="288"/>
+      <c r="CG14" s="288"/>
+      <c r="CH14" s="289"/>
+      <c r="CL14" s="287" t="s">
         <v>329</v>
       </c>
-      <c r="CM14" s="268"/>
-      <c r="CN14" s="268"/>
-      <c r="CO14" s="268"/>
-      <c r="CP14" s="268"/>
-      <c r="CQ14" s="268"/>
-      <c r="CR14" s="268"/>
-      <c r="CS14" s="269"/>
-      <c r="CV14" s="267" t="s">
+      <c r="CM14" s="288"/>
+      <c r="CN14" s="288"/>
+      <c r="CO14" s="288"/>
+      <c r="CP14" s="288"/>
+      <c r="CQ14" s="288"/>
+      <c r="CR14" s="288"/>
+      <c r="CS14" s="289"/>
+      <c r="CV14" s="287" t="s">
         <v>328</v>
       </c>
-      <c r="CW14" s="268"/>
-      <c r="CX14" s="268"/>
-      <c r="CY14" s="268"/>
-      <c r="CZ14" s="268"/>
-      <c r="DA14" s="268"/>
-      <c r="DB14" s="268"/>
-      <c r="DC14" s="269"/>
+      <c r="CW14" s="288"/>
+      <c r="CX14" s="288"/>
+      <c r="CY14" s="288"/>
+      <c r="CZ14" s="288"/>
+      <c r="DA14" s="288"/>
+      <c r="DB14" s="288"/>
+      <c r="DC14" s="289"/>
     </row>
     <row r="15" spans="1:107" thickBot="1">
       <c r="G15" s="117"/>
@@ -7786,7 +7900,7 @@
       <c r="V15" s="29"/>
       <c r="W15" s="29"/>
       <c r="AX15" s="42"/>
-      <c r="AY15" s="259"/>
+      <c r="AY15" s="291"/>
       <c r="BD15" s="117"/>
       <c r="BE15" s="116"/>
       <c r="BF15" s="114"/>
@@ -7847,7 +7961,7 @@
       <c r="V16" s="29"/>
       <c r="W16" s="29"/>
       <c r="AX16" s="42"/>
-      <c r="AY16" s="259"/>
+      <c r="AY16" s="291"/>
       <c r="BD16" s="40"/>
       <c r="BE16" s="29"/>
       <c r="BF16" s="29"/>
@@ -7899,16 +8013,16 @@
       <c r="M17" s="29"/>
       <c r="N17" s="29"/>
       <c r="O17" s="40"/>
-      <c r="P17" s="270"/>
+      <c r="P17" s="293"/>
       <c r="Q17" s="246"/>
       <c r="R17" s="246"/>
       <c r="S17" s="29"/>
-      <c r="T17" s="270"/>
+      <c r="T17" s="293"/>
       <c r="U17" s="246"/>
       <c r="V17" s="246"/>
       <c r="W17" s="246"/>
       <c r="AX17" s="42"/>
-      <c r="AY17" s="259"/>
+      <c r="AY17" s="291"/>
       <c r="BD17" s="40"/>
       <c r="BE17" s="29"/>
       <c r="BF17" s="29"/>
@@ -7926,14 +8040,14 @@
       <c r="BV17" s="29"/>
       <c r="BW17" s="46"/>
       <c r="CA17" s="40"/>
-      <c r="CB17" s="271" t="s">
+      <c r="CB17" s="255" t="s">
         <v>349</v>
       </c>
-      <c r="CC17" s="256"/>
-      <c r="CD17" s="256"/>
-      <c r="CE17" s="256"/>
-      <c r="CF17" s="256"/>
-      <c r="CG17" s="257"/>
+      <c r="CC17" s="258"/>
+      <c r="CD17" s="258"/>
+      <c r="CE17" s="258"/>
+      <c r="CF17" s="258"/>
+      <c r="CG17" s="259"/>
       <c r="CH17" s="46"/>
       <c r="CL17" s="40"/>
       <c r="CM17" s="29"/>
@@ -7956,96 +8070,96 @@
       <c r="G18" s="41"/>
       <c r="O18" s="41"/>
       <c r="AX18" s="42"/>
-      <c r="AY18" s="259"/>
+      <c r="AY18" s="291"/>
       <c r="BD18" s="41"/>
-      <c r="BE18" s="255" t="s">
+      <c r="BE18" s="269" t="s">
         <v>335</v>
       </c>
-      <c r="BF18" s="256"/>
-      <c r="BG18" s="256"/>
-      <c r="BH18" s="256"/>
-      <c r="BI18" s="256"/>
-      <c r="BJ18" s="257"/>
+      <c r="BF18" s="258"/>
+      <c r="BG18" s="258"/>
+      <c r="BH18" s="258"/>
+      <c r="BI18" s="258"/>
+      <c r="BJ18" s="259"/>
       <c r="BK18" s="42"/>
       <c r="BP18" s="41"/>
-      <c r="BQ18" s="255" t="s">
+      <c r="BQ18" s="269" t="s">
         <v>331</v>
       </c>
-      <c r="BR18" s="256"/>
-      <c r="BS18" s="256"/>
-      <c r="BT18" s="256"/>
-      <c r="BU18" s="256"/>
-      <c r="BV18" s="257"/>
+      <c r="BR18" s="258"/>
+      <c r="BS18" s="258"/>
+      <c r="BT18" s="258"/>
+      <c r="BU18" s="258"/>
+      <c r="BV18" s="259"/>
       <c r="BW18" s="42"/>
       <c r="CA18" s="41"/>
-      <c r="CB18" s="272" t="s">
+      <c r="CB18" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="CC18" s="273"/>
-      <c r="CD18" s="255"/>
-      <c r="CE18" s="257"/>
-      <c r="CF18" s="272" t="s">
+      <c r="CC18" s="271"/>
+      <c r="CD18" s="269"/>
+      <c r="CE18" s="259"/>
+      <c r="CF18" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="CG18" s="273"/>
+      <c r="CG18" s="271"/>
       <c r="CH18" s="42"/>
       <c r="CL18" s="41"/>
-      <c r="CM18" s="271" t="s">
+      <c r="CM18" s="255" t="s">
         <v>354</v>
       </c>
-      <c r="CN18" s="256"/>
-      <c r="CO18" s="256"/>
-      <c r="CP18" s="256"/>
-      <c r="CQ18" s="256"/>
-      <c r="CR18" s="257"/>
+      <c r="CN18" s="258"/>
+      <c r="CO18" s="258"/>
+      <c r="CP18" s="258"/>
+      <c r="CQ18" s="258"/>
+      <c r="CR18" s="259"/>
       <c r="CS18" s="42"/>
       <c r="CV18" s="41"/>
-      <c r="CW18" s="271" t="s">
+      <c r="CW18" s="255" t="s">
         <v>359</v>
       </c>
-      <c r="CX18" s="256"/>
-      <c r="CY18" s="256"/>
-      <c r="CZ18" s="256"/>
-      <c r="DA18" s="256"/>
-      <c r="DB18" s="257"/>
+      <c r="CX18" s="258"/>
+      <c r="CY18" s="258"/>
+      <c r="CZ18" s="258"/>
+      <c r="DA18" s="258"/>
+      <c r="DB18" s="259"/>
       <c r="DC18" s="42"/>
     </row>
     <row r="19" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G19" s="41"/>
       <c r="O19" s="41"/>
       <c r="AX19" s="42"/>
-      <c r="AY19" s="259"/>
+      <c r="AY19" s="291"/>
       <c r="BD19" s="41"/>
-      <c r="BE19" s="255" t="s">
+      <c r="BE19" s="269" t="s">
         <v>336</v>
       </c>
-      <c r="BF19" s="256"/>
-      <c r="BG19" s="256"/>
-      <c r="BH19" s="256"/>
-      <c r="BI19" s="256"/>
-      <c r="BJ19" s="257"/>
+      <c r="BF19" s="258"/>
+      <c r="BG19" s="258"/>
+      <c r="BH19" s="258"/>
+      <c r="BI19" s="258"/>
+      <c r="BJ19" s="259"/>
       <c r="BK19" s="42"/>
       <c r="BP19" s="41"/>
-      <c r="BQ19" s="255" t="s">
+      <c r="BQ19" s="269" t="s">
         <v>330</v>
       </c>
-      <c r="BR19" s="256"/>
-      <c r="BS19" s="256"/>
-      <c r="BT19" s="256"/>
-      <c r="BU19" s="256"/>
-      <c r="BV19" s="257"/>
+      <c r="BR19" s="258"/>
+      <c r="BS19" s="258"/>
+      <c r="BT19" s="258"/>
+      <c r="BU19" s="258"/>
+      <c r="BV19" s="259"/>
       <c r="BW19" s="42"/>
       <c r="CA19" s="41"/>
       <c r="CH19" s="42"/>
       <c r="CL19" s="41"/>
-      <c r="CM19" s="271" t="s">
+      <c r="CM19" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN19" s="256"/>
-      <c r="CO19" s="256"/>
-      <c r="CP19" s="256"/>
-      <c r="CQ19" s="256"/>
-      <c r="CR19" s="257"/>
+      <c r="CN19" s="258"/>
+      <c r="CO19" s="258"/>
+      <c r="CP19" s="258"/>
+      <c r="CQ19" s="258"/>
+      <c r="CR19" s="259"/>
       <c r="CS19" s="42"/>
       <c r="CV19" s="41"/>
       <c r="DC19" s="42"/>
@@ -8054,114 +8168,114 @@
       <c r="G20" s="41"/>
       <c r="O20" s="41"/>
       <c r="AX20" s="42"/>
-      <c r="AY20" s="259"/>
+      <c r="AY20" s="291"/>
       <c r="BD20" s="41"/>
       <c r="BK20" s="42"/>
       <c r="BP20" s="41"/>
       <c r="BW20" s="42"/>
       <c r="CA20" s="41"/>
-      <c r="CB20" s="271" t="s">
+      <c r="CB20" s="255" t="s">
         <v>350</v>
       </c>
-      <c r="CC20" s="256"/>
-      <c r="CD20" s="256"/>
-      <c r="CE20" s="256"/>
-      <c r="CF20" s="256"/>
-      <c r="CG20" s="257"/>
+      <c r="CC20" s="258"/>
+      <c r="CD20" s="258"/>
+      <c r="CE20" s="258"/>
+      <c r="CF20" s="258"/>
+      <c r="CG20" s="259"/>
       <c r="CH20" s="42"/>
       <c r="CL20" s="41"/>
       <c r="CS20" s="42"/>
       <c r="CV20" s="41"/>
-      <c r="CW20" s="271" t="s">
+      <c r="CW20" s="255" t="s">
         <v>360</v>
       </c>
-      <c r="CX20" s="256"/>
-      <c r="CY20" s="256"/>
-      <c r="CZ20" s="256"/>
-      <c r="DA20" s="256"/>
-      <c r="DB20" s="257"/>
+      <c r="CX20" s="258"/>
+      <c r="CY20" s="258"/>
+      <c r="CZ20" s="258"/>
+      <c r="DA20" s="258"/>
+      <c r="DB20" s="259"/>
       <c r="DC20" s="42"/>
     </row>
     <row r="21" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G21" s="41"/>
       <c r="O21" s="41"/>
       <c r="AX21" s="42"/>
-      <c r="AY21" s="259"/>
+      <c r="AY21" s="291"/>
       <c r="BD21" s="41"/>
-      <c r="BE21" s="255" t="s">
+      <c r="BE21" s="269" t="s">
         <v>337</v>
       </c>
-      <c r="BF21" s="256"/>
-      <c r="BG21" s="256"/>
-      <c r="BH21" s="256"/>
-      <c r="BI21" s="256"/>
-      <c r="BJ21" s="257"/>
+      <c r="BF21" s="258"/>
+      <c r="BG21" s="258"/>
+      <c r="BH21" s="258"/>
+      <c r="BI21" s="258"/>
+      <c r="BJ21" s="259"/>
       <c r="BK21" s="42"/>
       <c r="BP21" s="41"/>
-      <c r="BQ21" s="255" t="s">
+      <c r="BQ21" s="269" t="s">
         <v>332</v>
       </c>
-      <c r="BR21" s="256"/>
-      <c r="BS21" s="256"/>
-      <c r="BT21" s="256"/>
-      <c r="BU21" s="256"/>
-      <c r="BV21" s="257"/>
+      <c r="BR21" s="258"/>
+      <c r="BS21" s="258"/>
+      <c r="BT21" s="258"/>
+      <c r="BU21" s="258"/>
+      <c r="BV21" s="259"/>
       <c r="BW21" s="42"/>
       <c r="CA21" s="41"/>
-      <c r="CB21" s="271" t="s">
+      <c r="CB21" s="255" t="s">
         <v>336</v>
       </c>
-      <c r="CC21" s="256"/>
-      <c r="CD21" s="256"/>
-      <c r="CE21" s="256"/>
-      <c r="CF21" s="256"/>
-      <c r="CG21" s="257"/>
+      <c r="CC21" s="258"/>
+      <c r="CD21" s="258"/>
+      <c r="CE21" s="258"/>
+      <c r="CF21" s="258"/>
+      <c r="CG21" s="259"/>
       <c r="CH21" s="42"/>
       <c r="CL21" s="41"/>
-      <c r="CM21" s="271" t="s">
+      <c r="CM21" s="255" t="s">
         <v>356</v>
       </c>
-      <c r="CN21" s="256"/>
-      <c r="CO21" s="256"/>
-      <c r="CP21" s="256"/>
-      <c r="CQ21" s="256"/>
-      <c r="CR21" s="257"/>
+      <c r="CN21" s="258"/>
+      <c r="CO21" s="258"/>
+      <c r="CP21" s="258"/>
+      <c r="CQ21" s="258"/>
+      <c r="CR21" s="259"/>
       <c r="CS21" s="42"/>
       <c r="CV21" s="41"/>
-      <c r="CW21" s="271" t="s">
+      <c r="CW21" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CX21" s="256"/>
-      <c r="CY21" s="256"/>
-      <c r="CZ21" s="256"/>
-      <c r="DA21" s="256"/>
-      <c r="DB21" s="257"/>
+      <c r="CX21" s="258"/>
+      <c r="CY21" s="258"/>
+      <c r="CZ21" s="258"/>
+      <c r="DA21" s="258"/>
+      <c r="DB21" s="259"/>
       <c r="DC21" s="42"/>
     </row>
     <row r="22" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G22" s="41"/>
       <c r="O22" s="41"/>
       <c r="AX22" s="42"/>
-      <c r="AY22" s="259"/>
+      <c r="AY22" s="291"/>
       <c r="BD22" s="41"/>
-      <c r="BE22" s="255" t="s">
+      <c r="BE22" s="269" t="s">
         <v>336</v>
       </c>
-      <c r="BF22" s="256"/>
-      <c r="BG22" s="256"/>
-      <c r="BH22" s="256"/>
-      <c r="BI22" s="256"/>
-      <c r="BJ22" s="257"/>
+      <c r="BF22" s="258"/>
+      <c r="BG22" s="258"/>
+      <c r="BH22" s="258"/>
+      <c r="BI22" s="258"/>
+      <c r="BJ22" s="259"/>
       <c r="BK22" s="42"/>
       <c r="BP22" s="41"/>
-      <c r="BQ22" s="255" t="s">
+      <c r="BQ22" s="269" t="s">
         <v>330</v>
       </c>
-      <c r="BR22" s="256"/>
-      <c r="BS22" s="256"/>
-      <c r="BT22" s="256"/>
-      <c r="BU22" s="256"/>
-      <c r="BV22" s="257"/>
+      <c r="BR22" s="258"/>
+      <c r="BS22" s="258"/>
+      <c r="BT22" s="258"/>
+      <c r="BU22" s="258"/>
+      <c r="BV22" s="259"/>
       <c r="BW22" s="42"/>
       <c r="CA22" s="41"/>
       <c r="CH22" s="42"/>
@@ -8174,7 +8288,7 @@
       <c r="G23" s="41"/>
       <c r="O23" s="41"/>
       <c r="AX23" s="42"/>
-      <c r="AY23" s="259"/>
+      <c r="AY23" s="291"/>
       <c r="BD23" s="41"/>
       <c r="BK23" s="42"/>
       <c r="BP23" s="41"/>
@@ -8183,57 +8297,57 @@
       <c r="CB23" s="29"/>
       <c r="CC23" s="29"/>
       <c r="CD23" s="29"/>
-      <c r="CE23" s="282" t="s">
+      <c r="CE23" s="278" t="s">
         <v>348</v>
       </c>
-      <c r="CF23" s="283"/>
-      <c r="CG23" s="283"/>
-      <c r="CH23" s="284"/>
+      <c r="CF23" s="279"/>
+      <c r="CG23" s="279"/>
+      <c r="CH23" s="280"/>
       <c r="CL23" s="41"/>
-      <c r="CM23" s="271" t="s">
+      <c r="CM23" s="255" t="s">
         <v>357</v>
       </c>
-      <c r="CN23" s="256"/>
-      <c r="CO23" s="256"/>
-      <c r="CP23" s="256"/>
-      <c r="CQ23" s="256"/>
-      <c r="CR23" s="257"/>
+      <c r="CN23" s="258"/>
+      <c r="CO23" s="258"/>
+      <c r="CP23" s="258"/>
+      <c r="CQ23" s="258"/>
+      <c r="CR23" s="259"/>
       <c r="CS23" s="42"/>
       <c r="CV23" s="41"/>
-      <c r="CW23" s="271" t="s">
+      <c r="CW23" s="255" t="s">
         <v>361</v>
       </c>
-      <c r="CX23" s="256"/>
-      <c r="CY23" s="256"/>
-      <c r="CZ23" s="256"/>
-      <c r="DA23" s="256"/>
-      <c r="DB23" s="257"/>
+      <c r="CX23" s="258"/>
+      <c r="CY23" s="258"/>
+      <c r="CZ23" s="258"/>
+      <c r="DA23" s="258"/>
+      <c r="DB23" s="259"/>
       <c r="DC23" s="42"/>
     </row>
     <row r="24" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G24" s="41"/>
       <c r="O24" s="41"/>
       <c r="AX24" s="42"/>
-      <c r="AY24" s="259"/>
+      <c r="AY24" s="291"/>
       <c r="BD24" s="41"/>
-      <c r="BE24" s="255" t="s">
+      <c r="BE24" s="269" t="s">
         <v>339</v>
       </c>
-      <c r="BF24" s="256"/>
-      <c r="BG24" s="256"/>
-      <c r="BH24" s="256"/>
-      <c r="BI24" s="256"/>
-      <c r="BJ24" s="257"/>
+      <c r="BF24" s="258"/>
+      <c r="BG24" s="258"/>
+      <c r="BH24" s="258"/>
+      <c r="BI24" s="258"/>
+      <c r="BJ24" s="259"/>
       <c r="BK24" s="42"/>
       <c r="BP24" s="41"/>
-      <c r="BQ24" s="255" t="s">
+      <c r="BQ24" s="269" t="s">
         <v>333</v>
       </c>
-      <c r="BR24" s="256"/>
-      <c r="BS24" s="256"/>
-      <c r="BT24" s="256"/>
-      <c r="BU24" s="256"/>
-      <c r="BV24" s="257"/>
+      <c r="BR24" s="258"/>
+      <c r="BS24" s="258"/>
+      <c r="BT24" s="258"/>
+      <c r="BU24" s="258"/>
+      <c r="BV24" s="259"/>
       <c r="BW24" s="42"/>
       <c r="CA24" s="40"/>
       <c r="CB24" s="29"/>
@@ -8244,60 +8358,60 @@
       <c r="CG24" s="29"/>
       <c r="CH24" s="46"/>
       <c r="CL24" s="41"/>
-      <c r="CM24" s="271" t="s">
+      <c r="CM24" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN24" s="256"/>
-      <c r="CO24" s="256"/>
-      <c r="CP24" s="256"/>
-      <c r="CQ24" s="256"/>
-      <c r="CR24" s="257"/>
+      <c r="CN24" s="258"/>
+      <c r="CO24" s="258"/>
+      <c r="CP24" s="258"/>
+      <c r="CQ24" s="258"/>
+      <c r="CR24" s="259"/>
       <c r="CS24" s="42"/>
       <c r="CV24" s="41"/>
-      <c r="CW24" s="271" t="s">
+      <c r="CW24" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CX24" s="256"/>
-      <c r="CY24" s="256"/>
-      <c r="CZ24" s="256"/>
-      <c r="DA24" s="256"/>
-      <c r="DB24" s="257"/>
+      <c r="CX24" s="258"/>
+      <c r="CY24" s="258"/>
+      <c r="CZ24" s="258"/>
+      <c r="DA24" s="258"/>
+      <c r="DB24" s="259"/>
       <c r="DC24" s="42"/>
     </row>
     <row r="25" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G25" s="41"/>
       <c r="O25" s="41"/>
       <c r="AX25" s="42"/>
-      <c r="AY25" s="259"/>
+      <c r="AY25" s="291"/>
       <c r="BD25" s="41"/>
-      <c r="BE25" s="255" t="s">
+      <c r="BE25" s="269" t="s">
         <v>336</v>
       </c>
-      <c r="BF25" s="256"/>
-      <c r="BG25" s="256"/>
-      <c r="BH25" s="256"/>
-      <c r="BI25" s="256"/>
-      <c r="BJ25" s="257"/>
+      <c r="BF25" s="258"/>
+      <c r="BG25" s="258"/>
+      <c r="BH25" s="258"/>
+      <c r="BI25" s="258"/>
+      <c r="BJ25" s="259"/>
       <c r="BK25" s="42"/>
       <c r="BP25" s="41"/>
-      <c r="BQ25" s="255" t="s">
+      <c r="BQ25" s="269" t="s">
         <v>330</v>
       </c>
-      <c r="BR25" s="256"/>
-      <c r="BS25" s="256"/>
-      <c r="BT25" s="256"/>
-      <c r="BU25" s="256"/>
-      <c r="BV25" s="257"/>
+      <c r="BR25" s="258"/>
+      <c r="BS25" s="258"/>
+      <c r="BT25" s="258"/>
+      <c r="BU25" s="258"/>
+      <c r="BV25" s="259"/>
       <c r="BW25" s="42"/>
       <c r="CA25" s="41"/>
-      <c r="CB25" s="271" t="s">
+      <c r="CB25" s="255" t="s">
         <v>343</v>
       </c>
-      <c r="CC25" s="280"/>
-      <c r="CD25" s="280"/>
-      <c r="CE25" s="280"/>
-      <c r="CF25" s="280"/>
-      <c r="CG25" s="281"/>
+      <c r="CC25" s="256"/>
+      <c r="CD25" s="256"/>
+      <c r="CE25" s="256"/>
+      <c r="CF25" s="256"/>
+      <c r="CG25" s="257"/>
       <c r="CH25" s="42"/>
       <c r="CL25" s="41"/>
       <c r="CS25" s="42"/>
@@ -8308,128 +8422,128 @@
       <c r="G26" s="41"/>
       <c r="O26" s="41"/>
       <c r="AX26" s="42"/>
-      <c r="AY26" s="259"/>
+      <c r="AY26" s="291"/>
       <c r="BD26" s="41"/>
       <c r="BK26" s="42"/>
       <c r="BP26" s="41"/>
       <c r="BW26" s="42"/>
       <c r="CA26" s="41"/>
-      <c r="CB26" s="272" t="s">
+      <c r="CB26" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="CC26" s="273"/>
-      <c r="CD26" s="255"/>
-      <c r="CE26" s="257"/>
-      <c r="CF26" s="272" t="s">
+      <c r="CC26" s="271"/>
+      <c r="CD26" s="269"/>
+      <c r="CE26" s="259"/>
+      <c r="CF26" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="CG26" s="273"/>
+      <c r="CG26" s="271"/>
       <c r="CH26" s="42"/>
       <c r="CL26" s="41"/>
-      <c r="CM26" s="255" t="s">
+      <c r="CM26" s="269" t="s">
         <v>331</v>
       </c>
-      <c r="CN26" s="256"/>
-      <c r="CO26" s="256"/>
-      <c r="CP26" s="256"/>
-      <c r="CQ26" s="256"/>
-      <c r="CR26" s="257"/>
+      <c r="CN26" s="258"/>
+      <c r="CO26" s="258"/>
+      <c r="CP26" s="258"/>
+      <c r="CQ26" s="258"/>
+      <c r="CR26" s="259"/>
       <c r="CS26" s="42"/>
       <c r="CV26" s="41"/>
-      <c r="CW26" s="271" t="s">
+      <c r="CW26" s="255" t="s">
         <v>362</v>
       </c>
-      <c r="CX26" s="256"/>
-      <c r="CY26" s="256"/>
-      <c r="CZ26" s="256"/>
-      <c r="DA26" s="256"/>
-      <c r="DB26" s="257"/>
+      <c r="CX26" s="258"/>
+      <c r="CY26" s="258"/>
+      <c r="CZ26" s="258"/>
+      <c r="DA26" s="258"/>
+      <c r="DB26" s="259"/>
       <c r="DC26" s="42"/>
     </row>
     <row r="27" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G27" s="41"/>
       <c r="O27" s="41"/>
       <c r="AX27" s="42"/>
-      <c r="AY27" s="259"/>
+      <c r="AY27" s="291"/>
       <c r="BD27" s="41"/>
-      <c r="BE27" s="255" t="s">
+      <c r="BE27" s="269" t="s">
         <v>340</v>
       </c>
-      <c r="BF27" s="256"/>
-      <c r="BG27" s="256"/>
-      <c r="BH27" s="256"/>
-      <c r="BI27" s="256"/>
-      <c r="BJ27" s="257"/>
+      <c r="BF27" s="258"/>
+      <c r="BG27" s="258"/>
+      <c r="BH27" s="258"/>
+      <c r="BI27" s="258"/>
+      <c r="BJ27" s="259"/>
       <c r="BK27" s="42"/>
       <c r="BP27" s="41"/>
-      <c r="BQ27" s="255" t="s">
+      <c r="BQ27" s="269" t="s">
         <v>334</v>
       </c>
-      <c r="BR27" s="256"/>
-      <c r="BS27" s="256"/>
-      <c r="BT27" s="256"/>
-      <c r="BU27" s="256"/>
-      <c r="BV27" s="257"/>
+      <c r="BR27" s="258"/>
+      <c r="BS27" s="258"/>
+      <c r="BT27" s="258"/>
+      <c r="BU27" s="258"/>
+      <c r="BV27" s="259"/>
       <c r="BW27" s="42"/>
       <c r="CA27" s="41"/>
       <c r="CH27" s="42"/>
       <c r="CL27" s="41"/>
-      <c r="CM27" s="271" t="s">
+      <c r="CM27" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN27" s="256"/>
-      <c r="CO27" s="256"/>
-      <c r="CP27" s="256"/>
-      <c r="CQ27" s="256"/>
-      <c r="CR27" s="257"/>
+      <c r="CN27" s="258"/>
+      <c r="CO27" s="258"/>
+      <c r="CP27" s="258"/>
+      <c r="CQ27" s="258"/>
+      <c r="CR27" s="259"/>
       <c r="CS27" s="42"/>
       <c r="CV27" s="41"/>
-      <c r="CW27" s="271" t="s">
+      <c r="CW27" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CX27" s="256"/>
-      <c r="CY27" s="256"/>
-      <c r="CZ27" s="256"/>
-      <c r="DA27" s="256"/>
-      <c r="DB27" s="257"/>
+      <c r="CX27" s="258"/>
+      <c r="CY27" s="258"/>
+      <c r="CZ27" s="258"/>
+      <c r="DA27" s="258"/>
+      <c r="DB27" s="259"/>
       <c r="DC27" s="42"/>
     </row>
     <row r="28" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G28" s="41"/>
       <c r="O28" s="41"/>
       <c r="AX28" s="42"/>
-      <c r="AY28" s="259"/>
+      <c r="AY28" s="291"/>
       <c r="BD28" s="119"/>
-      <c r="BE28" s="272" t="s">
+      <c r="BE28" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="BF28" s="273"/>
-      <c r="BG28" s="255"/>
-      <c r="BH28" s="257"/>
-      <c r="BI28" s="272" t="s">
+      <c r="BF28" s="271"/>
+      <c r="BG28" s="269"/>
+      <c r="BH28" s="259"/>
+      <c r="BI28" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="BJ28" s="273"/>
+      <c r="BJ28" s="271"/>
       <c r="BK28" s="42"/>
       <c r="BP28" s="41"/>
-      <c r="BQ28" s="255" t="s">
+      <c r="BQ28" s="269" t="s">
         <v>330</v>
       </c>
-      <c r="BR28" s="256"/>
-      <c r="BS28" s="256"/>
-      <c r="BT28" s="256"/>
-      <c r="BU28" s="256"/>
-      <c r="BV28" s="257"/>
+      <c r="BR28" s="258"/>
+      <c r="BS28" s="258"/>
+      <c r="BT28" s="258"/>
+      <c r="BU28" s="258"/>
+      <c r="BV28" s="259"/>
       <c r="BW28" s="42"/>
       <c r="CA28" s="41"/>
-      <c r="CB28" s="271" t="s">
+      <c r="CB28" s="255" t="s">
         <v>344</v>
       </c>
-      <c r="CC28" s="280"/>
-      <c r="CD28" s="280"/>
-      <c r="CE28" s="280"/>
-      <c r="CF28" s="280"/>
-      <c r="CG28" s="281"/>
+      <c r="CC28" s="256"/>
+      <c r="CD28" s="256"/>
+      <c r="CE28" s="256"/>
+      <c r="CF28" s="256"/>
+      <c r="CG28" s="257"/>
       <c r="CH28" s="42"/>
       <c r="CL28" s="41"/>
       <c r="CS28" s="42"/>
@@ -8440,49 +8554,49 @@
       <c r="G29" s="41"/>
       <c r="O29" s="41"/>
       <c r="AX29" s="42"/>
-      <c r="AY29" s="259"/>
+      <c r="AY29" s="291"/>
       <c r="BD29" s="41"/>
       <c r="BK29" s="42"/>
       <c r="BP29" s="41"/>
       <c r="BW29" s="42"/>
       <c r="CA29" s="41"/>
-      <c r="CB29" s="272" t="s">
+      <c r="CB29" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="CC29" s="273"/>
-      <c r="CD29" s="255"/>
-      <c r="CE29" s="257"/>
-      <c r="CF29" s="272" t="s">
+      <c r="CC29" s="271"/>
+      <c r="CD29" s="269"/>
+      <c r="CE29" s="259"/>
+      <c r="CF29" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="CG29" s="273"/>
+      <c r="CG29" s="271"/>
       <c r="CH29" s="42"/>
       <c r="CL29" s="41"/>
-      <c r="CM29" s="255" t="s">
+      <c r="CM29" s="269" t="s">
         <v>332</v>
       </c>
-      <c r="CN29" s="256"/>
-      <c r="CO29" s="256"/>
-      <c r="CP29" s="256"/>
-      <c r="CQ29" s="256"/>
-      <c r="CR29" s="257"/>
+      <c r="CN29" s="258"/>
+      <c r="CO29" s="258"/>
+      <c r="CP29" s="258"/>
+      <c r="CQ29" s="258"/>
+      <c r="CR29" s="259"/>
       <c r="CS29" s="42"/>
       <c r="CV29" s="41"/>
-      <c r="CW29" s="271" t="s">
+      <c r="CW29" s="255" t="s">
         <v>363</v>
       </c>
-      <c r="CX29" s="256"/>
-      <c r="CY29" s="256"/>
-      <c r="CZ29" s="256"/>
-      <c r="DA29" s="256"/>
-      <c r="DB29" s="257"/>
+      <c r="CX29" s="258"/>
+      <c r="CY29" s="258"/>
+      <c r="CZ29" s="258"/>
+      <c r="DA29" s="258"/>
+      <c r="DB29" s="259"/>
       <c r="DC29" s="42"/>
     </row>
     <row r="30" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G30" s="41"/>
       <c r="O30" s="41"/>
       <c r="AX30" s="42"/>
-      <c r="AY30" s="259"/>
+      <c r="AY30" s="291"/>
       <c r="BD30" s="41"/>
       <c r="BK30" s="42"/>
       <c r="BP30" s="41"/>
@@ -8490,44 +8604,44 @@
       <c r="CA30" s="41"/>
       <c r="CH30" s="42"/>
       <c r="CL30" s="41"/>
-      <c r="CM30" s="271" t="s">
+      <c r="CM30" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN30" s="256"/>
-      <c r="CO30" s="256"/>
-      <c r="CP30" s="256"/>
-      <c r="CQ30" s="256"/>
-      <c r="CR30" s="257"/>
+      <c r="CN30" s="258"/>
+      <c r="CO30" s="258"/>
+      <c r="CP30" s="258"/>
+      <c r="CQ30" s="258"/>
+      <c r="CR30" s="259"/>
       <c r="CS30" s="42"/>
       <c r="CV30" s="41"/>
-      <c r="CW30" s="271" t="s">
+      <c r="CW30" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CX30" s="280"/>
-      <c r="CY30" s="280"/>
-      <c r="CZ30" s="280"/>
-      <c r="DA30" s="280"/>
-      <c r="DB30" s="281"/>
+      <c r="CX30" s="256"/>
+      <c r="CY30" s="256"/>
+      <c r="CZ30" s="256"/>
+      <c r="DA30" s="256"/>
+      <c r="DB30" s="257"/>
       <c r="DC30" s="42"/>
     </row>
     <row r="31" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G31" s="41"/>
       <c r="O31" s="41"/>
       <c r="AX31" s="42"/>
-      <c r="AY31" s="259"/>
+      <c r="AY31" s="291"/>
       <c r="BD31" s="41"/>
       <c r="BK31" s="42"/>
       <c r="BP31" s="41"/>
       <c r="BW31" s="42"/>
       <c r="CA31" s="41"/>
-      <c r="CB31" s="271" t="s">
+      <c r="CB31" s="255" t="s">
         <v>345</v>
       </c>
-      <c r="CC31" s="280"/>
-      <c r="CD31" s="280"/>
-      <c r="CE31" s="280"/>
-      <c r="CF31" s="280"/>
-      <c r="CG31" s="281"/>
+      <c r="CC31" s="256"/>
+      <c r="CD31" s="256"/>
+      <c r="CE31" s="256"/>
+      <c r="CF31" s="256"/>
+      <c r="CG31" s="257"/>
       <c r="CH31" s="42"/>
       <c r="CL31" s="41"/>
       <c r="CS31" s="42"/>
@@ -8538,122 +8652,122 @@
       <c r="G32" s="41"/>
       <c r="O32" s="41"/>
       <c r="AX32" s="42"/>
-      <c r="AY32" s="259"/>
+      <c r="AY32" s="291"/>
       <c r="BD32" s="41"/>
-      <c r="BE32" s="274" t="s">
+      <c r="BE32" s="272" t="s">
         <v>277</v>
       </c>
-      <c r="BF32" s="275"/>
-      <c r="BG32" s="275"/>
-      <c r="BH32" s="275"/>
-      <c r="BI32" s="275"/>
-      <c r="BJ32" s="276"/>
+      <c r="BF32" s="273"/>
+      <c r="BG32" s="273"/>
+      <c r="BH32" s="273"/>
+      <c r="BI32" s="273"/>
+      <c r="BJ32" s="274"/>
       <c r="BK32" s="42"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="274" t="s">
+      <c r="BQ32" s="272" t="s">
         <v>352</v>
       </c>
-      <c r="BR32" s="275"/>
-      <c r="BS32" s="275"/>
-      <c r="BT32" s="275"/>
-      <c r="BU32" s="275"/>
-      <c r="BV32" s="276"/>
+      <c r="BR32" s="273"/>
+      <c r="BS32" s="273"/>
+      <c r="BT32" s="273"/>
+      <c r="BU32" s="273"/>
+      <c r="BV32" s="274"/>
       <c r="BW32" s="42"/>
       <c r="CA32" s="41"/>
-      <c r="CB32" s="272" t="s">
+      <c r="CB32" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="CC32" s="273"/>
-      <c r="CD32" s="255"/>
-      <c r="CE32" s="257"/>
-      <c r="CF32" s="272" t="s">
+      <c r="CC32" s="271"/>
+      <c r="CD32" s="269"/>
+      <c r="CE32" s="259"/>
+      <c r="CF32" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="CG32" s="273"/>
+      <c r="CG32" s="271"/>
       <c r="CH32" s="42"/>
       <c r="CL32" s="41"/>
-      <c r="CM32" s="255" t="s">
+      <c r="CM32" s="269" t="s">
         <v>333</v>
       </c>
-      <c r="CN32" s="256"/>
-      <c r="CO32" s="256"/>
-      <c r="CP32" s="256"/>
-      <c r="CQ32" s="256"/>
-      <c r="CR32" s="257"/>
+      <c r="CN32" s="258"/>
+      <c r="CO32" s="258"/>
+      <c r="CP32" s="258"/>
+      <c r="CQ32" s="258"/>
+      <c r="CR32" s="259"/>
       <c r="CS32" s="42"/>
       <c r="CV32" s="41"/>
-      <c r="CW32" s="271" t="s">
+      <c r="CW32" s="255" t="s">
         <v>364</v>
       </c>
-      <c r="CX32" s="256"/>
-      <c r="CY32" s="256"/>
-      <c r="CZ32" s="256"/>
-      <c r="DA32" s="256"/>
-      <c r="DB32" s="257"/>
+      <c r="CX32" s="258"/>
+      <c r="CY32" s="258"/>
+      <c r="CZ32" s="258"/>
+      <c r="DA32" s="258"/>
+      <c r="DB32" s="259"/>
       <c r="DC32" s="42"/>
     </row>
     <row r="33" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G33" s="41"/>
       <c r="O33" s="41"/>
       <c r="AX33" s="42"/>
-      <c r="AY33" s="259"/>
+      <c r="AY33" s="291"/>
       <c r="BD33" s="41"/>
-      <c r="BE33" s="277"/>
-      <c r="BF33" s="278"/>
-      <c r="BG33" s="278"/>
-      <c r="BH33" s="278"/>
-      <c r="BI33" s="278"/>
-      <c r="BJ33" s="279"/>
+      <c r="BE33" s="275"/>
+      <c r="BF33" s="276"/>
+      <c r="BG33" s="276"/>
+      <c r="BH33" s="276"/>
+      <c r="BI33" s="276"/>
+      <c r="BJ33" s="277"/>
       <c r="BK33" s="42"/>
       <c r="BP33" s="41"/>
-      <c r="BQ33" s="277"/>
-      <c r="BR33" s="278"/>
-      <c r="BS33" s="278"/>
-      <c r="BT33" s="278"/>
-      <c r="BU33" s="278"/>
-      <c r="BV33" s="279"/>
+      <c r="BQ33" s="275"/>
+      <c r="BR33" s="276"/>
+      <c r="BS33" s="276"/>
+      <c r="BT33" s="276"/>
+      <c r="BU33" s="276"/>
+      <c r="BV33" s="277"/>
       <c r="BW33" s="42"/>
       <c r="CA33" s="41"/>
       <c r="CH33" s="42"/>
       <c r="CL33" s="41"/>
-      <c r="CM33" s="271" t="s">
+      <c r="CM33" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN33" s="280"/>
-      <c r="CO33" s="280"/>
-      <c r="CP33" s="280"/>
-      <c r="CQ33" s="280"/>
-      <c r="CR33" s="281"/>
+      <c r="CN33" s="256"/>
+      <c r="CO33" s="256"/>
+      <c r="CP33" s="256"/>
+      <c r="CQ33" s="256"/>
+      <c r="CR33" s="257"/>
       <c r="CS33" s="42"/>
       <c r="CV33" s="41"/>
-      <c r="CW33" s="271" t="s">
+      <c r="CW33" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CX33" s="280"/>
-      <c r="CY33" s="280"/>
-      <c r="CZ33" s="280"/>
-      <c r="DA33" s="280"/>
-      <c r="DB33" s="281"/>
+      <c r="CX33" s="256"/>
+      <c r="CY33" s="256"/>
+      <c r="CZ33" s="256"/>
+      <c r="DA33" s="256"/>
+      <c r="DB33" s="257"/>
       <c r="DC33" s="42"/>
     </row>
     <row r="34" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G34" s="41"/>
       <c r="O34" s="41"/>
       <c r="AX34" s="42"/>
-      <c r="AY34" s="259"/>
+      <c r="AY34" s="291"/>
       <c r="BD34" s="41"/>
       <c r="BK34" s="42"/>
       <c r="BP34" s="41"/>
       <c r="BW34" s="42"/>
       <c r="CA34" s="41"/>
-      <c r="CB34" s="271" t="s">
+      <c r="CB34" s="255" t="s">
         <v>346</v>
       </c>
-      <c r="CC34" s="280"/>
-      <c r="CD34" s="280"/>
-      <c r="CE34" s="280"/>
-      <c r="CF34" s="280"/>
-      <c r="CG34" s="281"/>
+      <c r="CC34" s="256"/>
+      <c r="CD34" s="256"/>
+      <c r="CE34" s="256"/>
+      <c r="CF34" s="256"/>
+      <c r="CG34" s="257"/>
       <c r="CH34" s="42"/>
       <c r="CL34" s="41"/>
       <c r="CS34" s="42"/>
@@ -8664,95 +8778,95 @@
       <c r="G35" s="41"/>
       <c r="O35" s="41"/>
       <c r="AX35" s="42"/>
-      <c r="AY35" s="259"/>
+      <c r="AY35" s="291"/>
       <c r="BD35" s="41"/>
       <c r="BK35" s="42"/>
       <c r="BP35" s="41"/>
-      <c r="BQ35" s="271" t="s">
+      <c r="BQ35" s="255" t="s">
         <v>351</v>
       </c>
-      <c r="BR35" s="256"/>
-      <c r="BS35" s="256"/>
-      <c r="BT35" s="256"/>
-      <c r="BU35" s="256"/>
-      <c r="BV35" s="257"/>
+      <c r="BR35" s="258"/>
+      <c r="BS35" s="258"/>
+      <c r="BT35" s="258"/>
+      <c r="BU35" s="258"/>
+      <c r="BV35" s="259"/>
       <c r="BW35" s="42"/>
       <c r="CA35" s="41"/>
-      <c r="CB35" s="272" t="s">
+      <c r="CB35" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="CC35" s="273"/>
-      <c r="CD35" s="255"/>
-      <c r="CE35" s="257"/>
-      <c r="CF35" s="272" t="s">
+      <c r="CC35" s="271"/>
+      <c r="CD35" s="269"/>
+      <c r="CE35" s="259"/>
+      <c r="CF35" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="CG35" s="273"/>
+      <c r="CG35" s="271"/>
       <c r="CH35" s="42"/>
       <c r="CL35" s="41"/>
-      <c r="CM35" s="271" t="s">
+      <c r="CM35" s="255" t="s">
         <v>358</v>
       </c>
-      <c r="CN35" s="256"/>
-      <c r="CO35" s="256"/>
-      <c r="CP35" s="256"/>
-      <c r="CQ35" s="256"/>
-      <c r="CR35" s="257"/>
+      <c r="CN35" s="258"/>
+      <c r="CO35" s="258"/>
+      <c r="CP35" s="258"/>
+      <c r="CQ35" s="258"/>
+      <c r="CR35" s="259"/>
       <c r="CS35" s="42"/>
       <c r="CV35" s="41"/>
-      <c r="CW35" s="271" t="s">
+      <c r="CW35" s="255" t="s">
         <v>365</v>
       </c>
-      <c r="CX35" s="256"/>
-      <c r="CY35" s="256"/>
-      <c r="CZ35" s="256"/>
-      <c r="DA35" s="256"/>
-      <c r="DB35" s="257"/>
+      <c r="CX35" s="258"/>
+      <c r="CY35" s="258"/>
+      <c r="CZ35" s="258"/>
+      <c r="DA35" s="258"/>
+      <c r="DB35" s="259"/>
       <c r="DC35" s="42"/>
     </row>
     <row r="36" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G36" s="41"/>
       <c r="O36" s="41"/>
       <c r="AX36" s="42"/>
-      <c r="AY36" s="259"/>
+      <c r="AY36" s="291"/>
       <c r="BD36" s="41"/>
       <c r="BK36" s="42"/>
       <c r="BP36" s="41"/>
-      <c r="BQ36" s="271" t="s">
+      <c r="BQ36" s="255" t="s">
         <v>353</v>
       </c>
-      <c r="BR36" s="256"/>
-      <c r="BS36" s="256"/>
-      <c r="BT36" s="256"/>
-      <c r="BU36" s="256"/>
-      <c r="BV36" s="257"/>
+      <c r="BR36" s="258"/>
+      <c r="BS36" s="258"/>
+      <c r="BT36" s="258"/>
+      <c r="BU36" s="258"/>
+      <c r="BV36" s="259"/>
       <c r="BW36" s="42"/>
       <c r="CA36" s="41"/>
       <c r="CH36" s="42"/>
       <c r="CL36" s="41"/>
-      <c r="CM36" s="271" t="s">
+      <c r="CM36" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN36" s="280"/>
-      <c r="CO36" s="280"/>
-      <c r="CP36" s="280"/>
-      <c r="CQ36" s="280"/>
-      <c r="CR36" s="281"/>
+      <c r="CN36" s="256"/>
+      <c r="CO36" s="256"/>
+      <c r="CP36" s="256"/>
+      <c r="CQ36" s="256"/>
+      <c r="CR36" s="257"/>
       <c r="CS36" s="42"/>
       <c r="CV36" s="41"/>
-      <c r="CW36" s="285"/>
-      <c r="CX36" s="286"/>
-      <c r="CY36" s="286"/>
-      <c r="CZ36" s="286"/>
-      <c r="DA36" s="286"/>
-      <c r="DB36" s="287"/>
+      <c r="CW36" s="260"/>
+      <c r="CX36" s="261"/>
+      <c r="CY36" s="261"/>
+      <c r="CZ36" s="261"/>
+      <c r="DA36" s="261"/>
+      <c r="DB36" s="262"/>
       <c r="DC36" s="42"/>
     </row>
     <row r="37" spans="7:107" ht="15.75" customHeight="1">
       <c r="G37" s="41"/>
       <c r="O37" s="41"/>
       <c r="AX37" s="42"/>
-      <c r="AY37" s="259"/>
+      <c r="AY37" s="291"/>
       <c r="BD37" s="41"/>
       <c r="BK37" s="42"/>
       <c r="BP37" s="41"/>
@@ -8762,19 +8876,19 @@
       <c r="CL37" s="41"/>
       <c r="CS37" s="42"/>
       <c r="CV37" s="41"/>
-      <c r="CW37" s="288"/>
-      <c r="CX37" s="289"/>
-      <c r="CY37" s="289"/>
-      <c r="CZ37" s="289"/>
-      <c r="DA37" s="289"/>
-      <c r="DB37" s="290"/>
+      <c r="CW37" s="263"/>
+      <c r="CX37" s="264"/>
+      <c r="CY37" s="264"/>
+      <c r="CZ37" s="264"/>
+      <c r="DA37" s="264"/>
+      <c r="DB37" s="265"/>
       <c r="DC37" s="42"/>
     </row>
     <row r="38" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G38" s="41"/>
       <c r="O38" s="41"/>
       <c r="AX38" s="42"/>
-      <c r="AY38" s="259"/>
+      <c r="AY38" s="291"/>
       <c r="BD38" s="41"/>
       <c r="BK38" s="42"/>
       <c r="BP38" s="41"/>
@@ -8784,70 +8898,70 @@
       <c r="CL38" s="41"/>
       <c r="CS38" s="42"/>
       <c r="CV38" s="41"/>
-      <c r="CW38" s="288"/>
-      <c r="CX38" s="289"/>
-      <c r="CY38" s="289"/>
-      <c r="CZ38" s="289"/>
-      <c r="DA38" s="289"/>
-      <c r="DB38" s="290"/>
+      <c r="CW38" s="263"/>
+      <c r="CX38" s="264"/>
+      <c r="CY38" s="264"/>
+      <c r="CZ38" s="264"/>
+      <c r="DA38" s="264"/>
+      <c r="DB38" s="265"/>
       <c r="DC38" s="42"/>
     </row>
     <row r="39" spans="7:107" ht="15.75" customHeight="1">
       <c r="G39" s="41"/>
       <c r="O39" s="41"/>
       <c r="AX39" s="42"/>
-      <c r="AY39" s="259"/>
+      <c r="AY39" s="291"/>
       <c r="BD39" s="41"/>
       <c r="BK39" s="42"/>
       <c r="BP39" s="41"/>
       <c r="BW39" s="42"/>
       <c r="CA39" s="41"/>
-      <c r="CB39" s="274" t="s">
+      <c r="CB39" s="272" t="s">
         <v>347</v>
       </c>
-      <c r="CC39" s="275"/>
-      <c r="CD39" s="275"/>
-      <c r="CE39" s="275"/>
-      <c r="CF39" s="275"/>
-      <c r="CG39" s="276"/>
+      <c r="CC39" s="273"/>
+      <c r="CD39" s="273"/>
+      <c r="CE39" s="273"/>
+      <c r="CF39" s="273"/>
+      <c r="CG39" s="274"/>
       <c r="CH39" s="42"/>
       <c r="CL39" s="41"/>
       <c r="CS39" s="42"/>
       <c r="CV39" s="41"/>
-      <c r="CW39" s="288"/>
-      <c r="CX39" s="289"/>
-      <c r="CY39" s="289"/>
-      <c r="CZ39" s="289"/>
-      <c r="DA39" s="289"/>
-      <c r="DB39" s="290"/>
+      <c r="CW39" s="263"/>
+      <c r="CX39" s="264"/>
+      <c r="CY39" s="264"/>
+      <c r="CZ39" s="264"/>
+      <c r="DA39" s="264"/>
+      <c r="DB39" s="265"/>
       <c r="DC39" s="42"/>
     </row>
     <row r="40" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G40" s="41"/>
       <c r="O40" s="41"/>
       <c r="AX40" s="42"/>
-      <c r="AY40" s="260"/>
+      <c r="AY40" s="292"/>
       <c r="BD40" s="41"/>
       <c r="BK40" s="42"/>
       <c r="BP40" s="41"/>
       <c r="BW40" s="42"/>
       <c r="CA40" s="41"/>
-      <c r="CB40" s="277"/>
-      <c r="CC40" s="278"/>
-      <c r="CD40" s="278"/>
-      <c r="CE40" s="278"/>
-      <c r="CF40" s="278"/>
-      <c r="CG40" s="279"/>
+      <c r="CB40" s="275"/>
+      <c r="CC40" s="276"/>
+      <c r="CD40" s="276"/>
+      <c r="CE40" s="276"/>
+      <c r="CF40" s="276"/>
+      <c r="CG40" s="277"/>
       <c r="CH40" s="42"/>
       <c r="CL40" s="41"/>
       <c r="CS40" s="42"/>
       <c r="CV40" s="41"/>
-      <c r="CW40" s="291"/>
-      <c r="CX40" s="292"/>
-      <c r="CY40" s="292"/>
-      <c r="CZ40" s="292"/>
-      <c r="DA40" s="292"/>
-      <c r="DB40" s="293"/>
+      <c r="CW40" s="266"/>
+      <c r="CX40" s="267"/>
+      <c r="CY40" s="267"/>
+      <c r="CZ40" s="267"/>
+      <c r="DA40" s="267"/>
+      <c r="DB40" s="268"/>
       <c r="DC40" s="42"/>
     </row>
     <row r="41" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
@@ -8910,43 +9024,43 @@
       <c r="M42" s="44"/>
       <c r="N42" s="44"/>
       <c r="O42" s="115"/>
-      <c r="P42" s="255" t="s">
+      <c r="P42" s="269" t="s">
         <v>323</v>
       </c>
-      <c r="Q42" s="256"/>
-      <c r="R42" s="256"/>
-      <c r="S42" s="256"/>
-      <c r="T42" s="256"/>
-      <c r="U42" s="256"/>
-      <c r="V42" s="256"/>
-      <c r="W42" s="256"/>
-      <c r="X42" s="256"/>
-      <c r="Y42" s="256"/>
-      <c r="Z42" s="256"/>
-      <c r="AA42" s="256"/>
-      <c r="AB42" s="256"/>
-      <c r="AC42" s="256"/>
-      <c r="AD42" s="256"/>
-      <c r="AE42" s="256"/>
-      <c r="AF42" s="256"/>
-      <c r="AG42" s="256"/>
-      <c r="AH42" s="256"/>
-      <c r="AI42" s="256"/>
-      <c r="AJ42" s="256"/>
-      <c r="AK42" s="256"/>
-      <c r="AL42" s="256"/>
-      <c r="AM42" s="256"/>
-      <c r="AN42" s="256"/>
-      <c r="AO42" s="256"/>
-      <c r="AP42" s="256"/>
-      <c r="AQ42" s="256"/>
-      <c r="AR42" s="256"/>
-      <c r="AS42" s="256"/>
-      <c r="AT42" s="256"/>
-      <c r="AU42" s="256"/>
-      <c r="AV42" s="256"/>
-      <c r="AW42" s="256"/>
-      <c r="AX42" s="257"/>
+      <c r="Q42" s="258"/>
+      <c r="R42" s="258"/>
+      <c r="S42" s="258"/>
+      <c r="T42" s="258"/>
+      <c r="U42" s="258"/>
+      <c r="V42" s="258"/>
+      <c r="W42" s="258"/>
+      <c r="X42" s="258"/>
+      <c r="Y42" s="258"/>
+      <c r="Z42" s="258"/>
+      <c r="AA42" s="258"/>
+      <c r="AB42" s="258"/>
+      <c r="AC42" s="258"/>
+      <c r="AD42" s="258"/>
+      <c r="AE42" s="258"/>
+      <c r="AF42" s="258"/>
+      <c r="AG42" s="258"/>
+      <c r="AH42" s="258"/>
+      <c r="AI42" s="258"/>
+      <c r="AJ42" s="258"/>
+      <c r="AK42" s="258"/>
+      <c r="AL42" s="258"/>
+      <c r="AM42" s="258"/>
+      <c r="AN42" s="258"/>
+      <c r="AO42" s="258"/>
+      <c r="AP42" s="258"/>
+      <c r="AQ42" s="258"/>
+      <c r="AR42" s="258"/>
+      <c r="AS42" s="258"/>
+      <c r="AT42" s="258"/>
+      <c r="AU42" s="258"/>
+      <c r="AV42" s="258"/>
+      <c r="AW42" s="258"/>
+      <c r="AX42" s="259"/>
       <c r="AY42" s="115"/>
       <c r="BD42" s="43"/>
       <c r="BE42" s="44"/>
@@ -8991,6 +9105,78 @@
     </row>
   </sheetData>
   <mergeCells count="88">
+    <mergeCell ref="P42:AX42"/>
+    <mergeCell ref="AY12:AY40"/>
+    <mergeCell ref="G11:N12"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="T17:W17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="BD11:BK12"/>
+    <mergeCell ref="BD14:BK14"/>
+    <mergeCell ref="BP11:BW12"/>
+    <mergeCell ref="BP14:BW14"/>
+    <mergeCell ref="CA11:CH12"/>
+    <mergeCell ref="CA14:CH14"/>
+    <mergeCell ref="CL11:CS12"/>
+    <mergeCell ref="CL14:CS14"/>
+    <mergeCell ref="CV11:DC12"/>
+    <mergeCell ref="CV14:DC14"/>
+    <mergeCell ref="BQ24:BV24"/>
+    <mergeCell ref="CM18:CR18"/>
+    <mergeCell ref="CM19:CR19"/>
+    <mergeCell ref="CM21:CR21"/>
+    <mergeCell ref="CM24:CR24"/>
+    <mergeCell ref="CM23:CR23"/>
+    <mergeCell ref="BE19:BJ19"/>
+    <mergeCell ref="BE18:BJ18"/>
+    <mergeCell ref="BE21:BJ21"/>
+    <mergeCell ref="BE22:BJ22"/>
+    <mergeCell ref="BQ19:BV19"/>
+    <mergeCell ref="BQ18:BV18"/>
+    <mergeCell ref="BQ21:BV21"/>
+    <mergeCell ref="BQ22:BV22"/>
+    <mergeCell ref="BE24:BJ24"/>
+    <mergeCell ref="BE25:BJ25"/>
+    <mergeCell ref="BE27:BJ27"/>
+    <mergeCell ref="BE28:BF28"/>
+    <mergeCell ref="BI28:BJ28"/>
+    <mergeCell ref="BG28:BH28"/>
+    <mergeCell ref="BE32:BJ33"/>
+    <mergeCell ref="CF29:CG29"/>
+    <mergeCell ref="CD29:CE29"/>
+    <mergeCell ref="CB29:CC29"/>
+    <mergeCell ref="CB28:CG28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="CB39:CG40"/>
+    <mergeCell ref="CB17:CG17"/>
+    <mergeCell ref="CB18:CC18"/>
+    <mergeCell ref="CD18:CE18"/>
+    <mergeCell ref="CF18:CG18"/>
+    <mergeCell ref="CB20:CG20"/>
+    <mergeCell ref="CF26:CG26"/>
+    <mergeCell ref="CD26:CE26"/>
+    <mergeCell ref="CB26:CC26"/>
+    <mergeCell ref="CB25:CG25"/>
+    <mergeCell ref="CE23:CH23"/>
+    <mergeCell ref="CB21:CG21"/>
+    <mergeCell ref="BQ36:BV36"/>
+    <mergeCell ref="CB31:CG31"/>
+    <mergeCell ref="CB32:CC32"/>
+    <mergeCell ref="CD32:CE32"/>
+    <mergeCell ref="CF32:CG32"/>
+    <mergeCell ref="CB34:CG34"/>
+    <mergeCell ref="CB35:CC35"/>
+    <mergeCell ref="CD35:CE35"/>
+    <mergeCell ref="CF35:CG35"/>
+    <mergeCell ref="BQ32:BV33"/>
+    <mergeCell ref="BQ25:BV25"/>
+    <mergeCell ref="BQ27:BV27"/>
+    <mergeCell ref="CM32:CR32"/>
+    <mergeCell ref="CM33:CR33"/>
+    <mergeCell ref="CM35:CR35"/>
+    <mergeCell ref="CM27:CR27"/>
+    <mergeCell ref="CM26:CR26"/>
+    <mergeCell ref="BQ35:BV35"/>
     <mergeCell ref="CM36:CR36"/>
     <mergeCell ref="CW18:DB18"/>
     <mergeCell ref="CW20:DB20"/>
@@ -9007,78 +9193,6 @@
     <mergeCell ref="CW36:DB40"/>
     <mergeCell ref="CM29:CR29"/>
     <mergeCell ref="CM30:CR30"/>
-    <mergeCell ref="BQ25:BV25"/>
-    <mergeCell ref="BQ27:BV27"/>
-    <mergeCell ref="CM32:CR32"/>
-    <mergeCell ref="CM33:CR33"/>
-    <mergeCell ref="CM35:CR35"/>
-    <mergeCell ref="CM27:CR27"/>
-    <mergeCell ref="CM26:CR26"/>
-    <mergeCell ref="BQ35:BV35"/>
-    <mergeCell ref="BQ36:BV36"/>
-    <mergeCell ref="CB31:CG31"/>
-    <mergeCell ref="CB32:CC32"/>
-    <mergeCell ref="CD32:CE32"/>
-    <mergeCell ref="CF32:CG32"/>
-    <mergeCell ref="CB34:CG34"/>
-    <mergeCell ref="CB35:CC35"/>
-    <mergeCell ref="CD35:CE35"/>
-    <mergeCell ref="CF35:CG35"/>
-    <mergeCell ref="BQ32:BV33"/>
-    <mergeCell ref="CB39:CG40"/>
-    <mergeCell ref="CB17:CG17"/>
-    <mergeCell ref="CB18:CC18"/>
-    <mergeCell ref="CD18:CE18"/>
-    <mergeCell ref="CF18:CG18"/>
-    <mergeCell ref="CB20:CG20"/>
-    <mergeCell ref="CF26:CG26"/>
-    <mergeCell ref="CD26:CE26"/>
-    <mergeCell ref="CB26:CC26"/>
-    <mergeCell ref="CB25:CG25"/>
-    <mergeCell ref="CE23:CH23"/>
-    <mergeCell ref="CB21:CG21"/>
-    <mergeCell ref="BE32:BJ33"/>
-    <mergeCell ref="CF29:CG29"/>
-    <mergeCell ref="CD29:CE29"/>
-    <mergeCell ref="CB29:CC29"/>
-    <mergeCell ref="CB28:CG28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BE24:BJ24"/>
-    <mergeCell ref="BE25:BJ25"/>
-    <mergeCell ref="BE27:BJ27"/>
-    <mergeCell ref="BE28:BF28"/>
-    <mergeCell ref="BI28:BJ28"/>
-    <mergeCell ref="BG28:BH28"/>
-    <mergeCell ref="BE19:BJ19"/>
-    <mergeCell ref="BE18:BJ18"/>
-    <mergeCell ref="BE21:BJ21"/>
-    <mergeCell ref="BE22:BJ22"/>
-    <mergeCell ref="BQ19:BV19"/>
-    <mergeCell ref="BQ18:BV18"/>
-    <mergeCell ref="BQ21:BV21"/>
-    <mergeCell ref="BQ22:BV22"/>
-    <mergeCell ref="CL11:CS12"/>
-    <mergeCell ref="CL14:CS14"/>
-    <mergeCell ref="CV11:DC12"/>
-    <mergeCell ref="CV14:DC14"/>
-    <mergeCell ref="BQ24:BV24"/>
-    <mergeCell ref="CM18:CR18"/>
-    <mergeCell ref="CM19:CR19"/>
-    <mergeCell ref="CM21:CR21"/>
-    <mergeCell ref="CM24:CR24"/>
-    <mergeCell ref="CM23:CR23"/>
-    <mergeCell ref="BD11:BK12"/>
-    <mergeCell ref="BD14:BK14"/>
-    <mergeCell ref="BP11:BW12"/>
-    <mergeCell ref="BP14:BW14"/>
-    <mergeCell ref="CA11:CH12"/>
-    <mergeCell ref="CA14:CH14"/>
-    <mergeCell ref="P42:AX42"/>
-    <mergeCell ref="AY12:AY40"/>
-    <mergeCell ref="G11:N12"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="T17:W17"/>
-    <mergeCell ref="P17:R17"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9137,14 +9251,14 @@
         <v>476</v>
       </c>
       <c r="C3" s="28"/>
-      <c r="D3" s="299" t="s">
+      <c r="D3" s="296" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="300"/>
-      <c r="F3" s="300"/>
-      <c r="G3" s="300"/>
-      <c r="H3" s="300"/>
-      <c r="I3" s="301"/>
+      <c r="E3" s="297"/>
+      <c r="F3" s="297"/>
+      <c r="G3" s="297"/>
+      <c r="H3" s="297"/>
+      <c r="I3" s="298"/>
     </row>
     <row r="4" spans="1:16" ht="21" customHeight="1">
       <c r="A4" s="156" t="s">
@@ -9283,15 +9397,15 @@
         <v>375</v>
       </c>
       <c r="F12" s="132"/>
-      <c r="H12" s="294" t="s">
+      <c r="H12" s="299" t="s">
         <v>400</v>
       </c>
-      <c r="I12" s="302"/>
+      <c r="I12" s="300"/>
       <c r="J12" s="140" t="s">
         <v>404</v>
       </c>
       <c r="K12" s="132"/>
-      <c r="M12" s="294" t="s">
+      <c r="M12" s="299" t="s">
         <v>415</v>
       </c>
       <c r="N12" s="295"/>
@@ -9308,15 +9422,15 @@
         <v>368</v>
       </c>
       <c r="F13" s="132"/>
-      <c r="H13" s="294" t="s">
+      <c r="H13" s="299" t="s">
         <v>401</v>
       </c>
-      <c r="I13" s="302"/>
+      <c r="I13" s="300"/>
       <c r="J13" s="140" t="s">
         <v>403</v>
       </c>
       <c r="K13" s="132"/>
-      <c r="M13" s="294" t="s">
+      <c r="M13" s="299" t="s">
         <v>216</v>
       </c>
       <c r="N13" s="295"/>
@@ -9331,15 +9445,15 @@
       </c>
       <c r="E14" s="131"/>
       <c r="F14" s="132"/>
-      <c r="H14" s="294" t="s">
+      <c r="H14" s="299" t="s">
         <v>402</v>
       </c>
-      <c r="I14" s="302"/>
+      <c r="I14" s="300"/>
       <c r="J14" s="140" t="s">
         <v>369</v>
       </c>
       <c r="K14" s="132"/>
-      <c r="M14" s="294" t="s">
+      <c r="M14" s="299" t="s">
         <v>215</v>
       </c>
       <c r="N14" s="295"/>
@@ -9354,11 +9468,11 @@
       </c>
       <c r="E15" s="140"/>
       <c r="F15" s="132"/>
-      <c r="H15" s="297"/>
-      <c r="I15" s="298"/>
+      <c r="H15" s="301"/>
+      <c r="I15" s="302"/>
       <c r="J15" s="140"/>
       <c r="K15" s="132"/>
-      <c r="M15" s="294" t="s">
+      <c r="M15" s="299" t="s">
         <v>211</v>
       </c>
       <c r="N15" s="295"/>
@@ -9373,11 +9487,11 @@
       </c>
       <c r="E16" s="131"/>
       <c r="F16" s="134"/>
-      <c r="H16" s="297"/>
-      <c r="I16" s="298"/>
+      <c r="H16" s="301"/>
+      <c r="I16" s="302"/>
       <c r="J16" s="140"/>
       <c r="K16" s="132"/>
-      <c r="M16" s="294" t="s">
+      <c r="M16" s="299" t="s">
         <v>212</v>
       </c>
       <c r="N16" s="295"/>
@@ -9396,7 +9510,7 @@
       <c r="I17" s="135"/>
       <c r="J17" s="136"/>
       <c r="K17" s="137"/>
-      <c r="M17" s="294" t="s">
+      <c r="M17" s="299" t="s">
         <v>416</v>
       </c>
       <c r="N17" s="295"/>
@@ -9409,7 +9523,7 @@
       <c r="C18" s="133"/>
       <c r="E18" s="131"/>
       <c r="F18" s="134"/>
-      <c r="M18" s="294" t="s">
+      <c r="M18" s="299" t="s">
         <v>213</v>
       </c>
       <c r="N18" s="295"/>
@@ -9432,7 +9546,7 @@
       <c r="K19" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="M19" s="294" t="s">
+      <c r="M19" s="299" t="s">
         <v>290</v>
       </c>
       <c r="N19" s="295"/>
@@ -9453,7 +9567,7 @@
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
       <c r="K20" s="127"/>
-      <c r="M20" s="296" t="s">
+      <c r="M20" s="294" t="s">
         <v>423</v>
       </c>
       <c r="N20" s="295"/>
@@ -9470,7 +9584,7 @@
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
       <c r="K21" s="127"/>
-      <c r="M21" s="296" t="s">
+      <c r="M21" s="294" t="s">
         <v>424</v>
       </c>
       <c r="N21" s="295"/>
@@ -9490,21 +9604,21 @@
         <v>84</v>
       </c>
       <c r="K22" s="130"/>
-      <c r="M22" s="296"/>
+      <c r="M22" s="294"/>
       <c r="N22" s="295"/>
       <c r="O22" s="131"/>
       <c r="P22" s="132"/>
     </row>
     <row r="23" spans="3:16" ht="15.75" customHeight="1" thickBot="1">
-      <c r="H23" s="294" t="s">
+      <c r="H23" s="299" t="s">
         <v>405</v>
       </c>
-      <c r="I23" s="302"/>
+      <c r="I23" s="300"/>
       <c r="J23" s="140" t="s">
         <v>369</v>
       </c>
       <c r="K23" s="132"/>
-      <c r="M23" s="296"/>
+      <c r="M23" s="294"/>
       <c r="N23" s="295"/>
       <c r="O23" s="131"/>
       <c r="P23" s="132"/>
@@ -9518,11 +9632,11 @@
       <c r="F24" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="H24" s="294"/>
-      <c r="I24" s="302"/>
+      <c r="H24" s="299"/>
+      <c r="I24" s="300"/>
       <c r="J24" s="140"/>
       <c r="K24" s="132"/>
-      <c r="M24" s="296"/>
+      <c r="M24" s="294"/>
       <c r="N24" s="295"/>
       <c r="O24" s="131"/>
       <c r="P24" s="132"/>
@@ -9536,11 +9650,11 @@
       <c r="F25" s="143" t="s">
         <v>373</v>
       </c>
-      <c r="H25" s="294"/>
-      <c r="I25" s="302"/>
+      <c r="H25" s="299"/>
+      <c r="I25" s="300"/>
       <c r="J25" s="140"/>
       <c r="K25" s="132"/>
-      <c r="M25" s="296"/>
+      <c r="M25" s="294"/>
       <c r="N25" s="295"/>
       <c r="O25" s="131"/>
       <c r="P25" s="132"/>
@@ -9550,11 +9664,11 @@
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="127"/>
-      <c r="H26" s="297"/>
-      <c r="I26" s="298"/>
+      <c r="H26" s="301"/>
+      <c r="I26" s="302"/>
       <c r="J26" s="140"/>
       <c r="K26" s="132"/>
-      <c r="M26" s="296"/>
+      <c r="M26" s="294"/>
       <c r="N26" s="295"/>
       <c r="O26" s="131"/>
       <c r="P26" s="132"/>
@@ -9568,11 +9682,11 @@
         <v>84</v>
       </c>
       <c r="F27" s="130"/>
-      <c r="H27" s="297"/>
-      <c r="I27" s="298"/>
+      <c r="H27" s="301"/>
+      <c r="I27" s="302"/>
       <c r="J27" s="140"/>
       <c r="K27" s="132"/>
-      <c r="M27" s="296"/>
+      <c r="M27" s="294"/>
       <c r="N27" s="295"/>
       <c r="O27" s="131"/>
       <c r="P27" s="132"/>
@@ -9589,7 +9703,7 @@
       <c r="I28" s="135"/>
       <c r="J28" s="136"/>
       <c r="K28" s="137"/>
-      <c r="M28" s="296"/>
+      <c r="M28" s="294"/>
       <c r="N28" s="295"/>
       <c r="O28" s="131"/>
       <c r="P28" s="132"/>
@@ -9602,7 +9716,7 @@
         <v>388</v>
       </c>
       <c r="F29" s="132"/>
-      <c r="M29" s="296"/>
+      <c r="M29" s="294"/>
       <c r="N29" s="295"/>
       <c r="O29" s="131"/>
       <c r="P29" s="132"/>
@@ -9613,7 +9727,7 @@
       </c>
       <c r="E30" s="140"/>
       <c r="F30" s="132"/>
-      <c r="M30" s="296"/>
+      <c r="M30" s="294"/>
       <c r="N30" s="295"/>
       <c r="O30" s="131"/>
       <c r="P30" s="132"/>
@@ -9694,7 +9808,7 @@
       <c r="C37" s="133"/>
       <c r="E37" s="131"/>
       <c r="F37" s="134"/>
-      <c r="M37" s="294" t="s">
+      <c r="M37" s="299" t="s">
         <v>428</v>
       </c>
       <c r="N37" s="295"/>
@@ -9707,7 +9821,7 @@
       <c r="C38" s="133"/>
       <c r="E38" s="131"/>
       <c r="F38" s="134"/>
-      <c r="M38" s="296" t="s">
+      <c r="M38" s="294" t="s">
         <v>429</v>
       </c>
       <c r="N38" s="295"/>
@@ -9721,7 +9835,7 @@
       <c r="D39" s="135"/>
       <c r="E39" s="136"/>
       <c r="F39" s="139"/>
-      <c r="M39" s="296"/>
+      <c r="M39" s="294"/>
       <c r="N39" s="295"/>
       <c r="O39" s="131" t="s">
         <v>432</v>
@@ -9729,7 +9843,7 @@
       <c r="P39" s="132"/>
     </row>
     <row r="40" spans="3:16" ht="15.75" customHeight="1" thickBot="1">
-      <c r="M40" s="296"/>
+      <c r="M40" s="294"/>
       <c r="N40" s="295"/>
       <c r="O40" s="131" t="s">
         <v>433</v>
@@ -9745,7 +9859,7 @@
       <c r="F41" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="M41" s="296"/>
+      <c r="M41" s="294"/>
       <c r="N41" s="295"/>
       <c r="O41" s="131" t="s">
         <v>435</v>
@@ -9761,7 +9875,7 @@
       <c r="F42" s="143" t="s">
         <v>373</v>
       </c>
-      <c r="M42" s="296"/>
+      <c r="M42" s="294"/>
       <c r="N42" s="295"/>
       <c r="O42" s="131" t="s">
         <v>434</v>
@@ -9856,7 +9970,7 @@
         <v>397</v>
       </c>
       <c r="F49" s="134"/>
-      <c r="M49" s="294" t="s">
+      <c r="M49" s="299" t="s">
         <v>436</v>
       </c>
       <c r="N49" s="295"/>
@@ -9873,7 +9987,7 @@
         <v>334</v>
       </c>
       <c r="F50" s="134"/>
-      <c r="M50" s="296" t="s">
+      <c r="M50" s="294" t="s">
         <v>437</v>
       </c>
       <c r="N50" s="295"/>
@@ -9890,7 +10004,7 @@
         <v>369</v>
       </c>
       <c r="F51" s="134"/>
-      <c r="M51" s="296" t="s">
+      <c r="M51" s="294" t="s">
         <v>438</v>
       </c>
       <c r="N51" s="295"/>
@@ -9903,7 +10017,7 @@
         <v>456</v>
       </c>
       <c r="F52" s="134"/>
-      <c r="M52" s="296" t="s">
+      <c r="M52" s="294" t="s">
         <v>441</v>
       </c>
       <c r="N52" s="295"/>
@@ -9917,7 +10031,7 @@
         <v>457</v>
       </c>
       <c r="F53" s="137"/>
-      <c r="M53" s="296"/>
+      <c r="M53" s="294"/>
       <c r="N53" s="295"/>
       <c r="O53" s="131"/>
       <c r="P53" s="132"/>
@@ -9970,7 +10084,7 @@
       </c>
     </row>
     <row r="60" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M60" s="294" t="s">
+      <c r="M60" s="299" t="s">
         <v>442</v>
       </c>
       <c r="N60" s="295"/>
@@ -9982,7 +10096,7 @@
       </c>
     </row>
     <row r="61" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M61" s="296" t="s">
+      <c r="M61" s="294" t="s">
         <v>443</v>
       </c>
       <c r="N61" s="295"/>
@@ -9994,7 +10108,7 @@
       </c>
     </row>
     <row r="62" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M62" s="294" t="s">
+      <c r="M62" s="299" t="s">
         <v>448</v>
       </c>
       <c r="N62" s="295"/>
@@ -10006,13 +10120,13 @@
       </c>
     </row>
     <row r="63" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M63" s="296"/>
+      <c r="M63" s="294"/>
       <c r="N63" s="295"/>
       <c r="O63" s="131"/>
       <c r="P63" s="132"/>
     </row>
     <row r="64" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M64" s="296"/>
+      <c r="M64" s="294"/>
       <c r="N64" s="295"/>
       <c r="O64" s="131"/>
       <c r="P64" s="132"/>
@@ -10061,7 +10175,7 @@
       <c r="P70" s="130"/>
     </row>
     <row r="71" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M71" s="294" t="s">
+      <c r="M71" s="299" t="s">
         <v>449</v>
       </c>
       <c r="N71" s="295"/>
@@ -10071,7 +10185,7 @@
       <c r="P71" s="132"/>
     </row>
     <row r="72" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M72" s="294" t="s">
+      <c r="M72" s="299" t="s">
         <v>450</v>
       </c>
       <c r="N72" s="295"/>
@@ -10081,19 +10195,19 @@
       <c r="P72" s="132"/>
     </row>
     <row r="73" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M73" s="296"/>
+      <c r="M73" s="294"/>
       <c r="N73" s="295"/>
       <c r="O73" s="131"/>
       <c r="P73" s="132"/>
     </row>
     <row r="74" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M74" s="296"/>
+      <c r="M74" s="294"/>
       <c r="N74" s="295"/>
       <c r="O74" s="131"/>
       <c r="P74" s="132"/>
     </row>
     <row r="75" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M75" s="296"/>
+      <c r="M75" s="294"/>
       <c r="N75" s="295"/>
       <c r="O75" s="131"/>
       <c r="P75" s="132"/>
@@ -10142,7 +10256,7 @@
       <c r="P81" s="130"/>
     </row>
     <row r="82" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M82" s="294" t="s">
+      <c r="M82" s="299" t="s">
         <v>449</v>
       </c>
       <c r="N82" s="295"/>
@@ -10152,7 +10266,7 @@
       <c r="P82" s="132"/>
     </row>
     <row r="83" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M83" s="294" t="s">
+      <c r="M83" s="299" t="s">
         <v>452</v>
       </c>
       <c r="N83" s="295"/>
@@ -10162,19 +10276,19 @@
       <c r="P83" s="132"/>
     </row>
     <row r="84" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M84" s="296"/>
+      <c r="M84" s="294"/>
       <c r="N84" s="295"/>
       <c r="O84" s="131"/>
       <c r="P84" s="132"/>
     </row>
     <row r="85" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M85" s="296"/>
+      <c r="M85" s="294"/>
       <c r="N85" s="295"/>
       <c r="O85" s="131"/>
       <c r="P85" s="132"/>
     </row>
     <row r="86" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M86" s="296"/>
+      <c r="M86" s="294"/>
       <c r="N86" s="295"/>
       <c r="O86" s="131"/>
       <c r="P86" s="132"/>
@@ -10221,7 +10335,7 @@
       <c r="P92" s="130"/>
     </row>
     <row r="93" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M93" s="294" t="s">
+      <c r="M93" s="299" t="s">
         <v>216</v>
       </c>
       <c r="N93" s="295"/>
@@ -10231,7 +10345,7 @@
       <c r="P93" s="132"/>
     </row>
     <row r="94" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M94" s="296"/>
+      <c r="M94" s="294"/>
       <c r="N94" s="295"/>
       <c r="O94" s="140" t="s">
         <v>454</v>
@@ -10239,7 +10353,7 @@
       <c r="P94" s="132"/>
     </row>
     <row r="95" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M95" s="296"/>
+      <c r="M95" s="294"/>
       <c r="N95" s="295"/>
       <c r="O95" s="140" t="s">
         <v>455</v>
@@ -10247,13 +10361,13 @@
       <c r="P95" s="132"/>
     </row>
     <row r="96" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M96" s="296"/>
+      <c r="M96" s="294"/>
       <c r="N96" s="295"/>
       <c r="O96" s="131"/>
       <c r="P96" s="132"/>
     </row>
     <row r="97" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M97" s="296"/>
+      <c r="M97" s="294"/>
       <c r="N97" s="295"/>
       <c r="O97" s="131"/>
       <c r="P97" s="132"/>
@@ -10300,7 +10414,7 @@
       <c r="P103" s="130"/>
     </row>
     <row r="104" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M104" s="294" t="s">
+      <c r="M104" s="299" t="s">
         <v>465</v>
       </c>
       <c r="N104" s="295"/>
@@ -10310,7 +10424,7 @@
       <c r="P104" s="132"/>
     </row>
     <row r="105" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M105" s="294" t="s">
+      <c r="M105" s="299" t="s">
         <v>466</v>
       </c>
       <c r="N105" s="295"/>
@@ -10320,7 +10434,7 @@
       <c r="P105" s="132"/>
     </row>
     <row r="106" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M106" s="294" t="s">
+      <c r="M106" s="299" t="s">
         <v>467</v>
       </c>
       <c r="N106" s="295"/>
@@ -10330,7 +10444,7 @@
       <c r="P106" s="132"/>
     </row>
     <row r="107" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M107" s="296"/>
+      <c r="M107" s="294"/>
       <c r="N107" s="295"/>
       <c r="O107" s="140" t="s">
         <v>464</v>
@@ -10338,7 +10452,7 @@
       <c r="P107" s="132"/>
     </row>
     <row r="108" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M108" s="296"/>
+      <c r="M108" s="294"/>
       <c r="N108" s="295"/>
       <c r="O108" s="131"/>
       <c r="P108" s="132"/>
@@ -10387,7 +10501,7 @@
       <c r="P114" s="130"/>
     </row>
     <row r="115" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M115" s="294" t="s">
+      <c r="M115" s="299" t="s">
         <v>482</v>
       </c>
       <c r="N115" s="295"/>
@@ -10397,31 +10511,31 @@
       <c r="P115" s="132"/>
     </row>
     <row r="116" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M116" s="296"/>
+      <c r="M116" s="294"/>
       <c r="N116" s="295"/>
       <c r="O116" s="131"/>
       <c r="P116" s="132"/>
     </row>
     <row r="117" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M117" s="296"/>
+      <c r="M117" s="294"/>
       <c r="N117" s="295"/>
       <c r="O117" s="131"/>
       <c r="P117" s="132"/>
     </row>
     <row r="118" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M118" s="296"/>
+      <c r="M118" s="294"/>
       <c r="N118" s="295"/>
       <c r="O118" s="131"/>
       <c r="P118" s="132"/>
     </row>
     <row r="119" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M119" s="296"/>
+      <c r="M119" s="294"/>
       <c r="N119" s="295"/>
       <c r="O119" s="131"/>
       <c r="P119" s="132"/>
     </row>
     <row r="120" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M120" s="296"/>
+      <c r="M120" s="294"/>
       <c r="N120" s="295"/>
       <c r="O120" s="131"/>
       <c r="P120" s="132"/>
@@ -10434,6 +10548,62 @@
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="M83:N83"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="M72:N72"/>
+    <mergeCell ref="M73:N73"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="M82:N82"/>
+    <mergeCell ref="M61:N61"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="M63:N63"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M71:N71"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
     <mergeCell ref="M119:N119"/>
     <mergeCell ref="M120:N120"/>
     <mergeCell ref="D3:I3"/>
@@ -10450,62 +10620,6 @@
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="H26:I26"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M49:N49"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="M51:N51"/>
-    <mergeCell ref="M52:N52"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="M61:N61"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="M63:N63"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M71:N71"/>
-    <mergeCell ref="M72:N72"/>
-    <mergeCell ref="M73:N73"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="M82:N82"/>
-    <mergeCell ref="M83:N83"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="M104:N104"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
@@ -15602,10 +15716,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:U198"/>
+  <dimension ref="B2:U215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -16582,12 +16696,12 @@
     </row>
     <row r="41" spans="2:21" ht="20.25" customHeight="1">
       <c r="B41" s="242"/>
-      <c r="C41" s="218"/>
+      <c r="C41" s="229"/>
       <c r="D41" s="218"/>
       <c r="E41" s="231"/>
       <c r="F41" s="232"/>
       <c r="G41" s="217"/>
-      <c r="H41" s="231"/>
+      <c r="H41" s="244"/>
       <c r="I41" s="216"/>
       <c r="J41" s="217"/>
       <c r="K41" s="231"/>
@@ -16602,12 +16716,15 @@
       <c r="U41" s="309"/>
     </row>
     <row r="42" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B42" s="242"/>
+      <c r="B42" s="242" t="s">
+        <v>655</v>
+      </c>
+      <c r="C42" s="229"/>
       <c r="D42" s="218"/>
       <c r="E42" s="231"/>
       <c r="F42" s="232"/>
       <c r="G42" s="217"/>
-      <c r="H42" s="231"/>
+      <c r="H42" s="244"/>
       <c r="I42" s="216"/>
       <c r="J42" s="217"/>
       <c r="K42" s="231"/>
@@ -16622,15 +16739,17 @@
       <c r="U42" s="309"/>
     </row>
     <row r="43" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B43" s="242" t="s">
-        <v>479</v>
-      </c>
-      <c r="C43" s="218"/>
-      <c r="D43" s="218"/>
+      <c r="B43" s="242"/>
+      <c r="C43" s="229" t="s">
+        <v>656</v>
+      </c>
+      <c r="D43" s="218" t="s">
+        <v>643</v>
+      </c>
       <c r="E43" s="231"/>
       <c r="F43" s="232"/>
       <c r="G43" s="217"/>
-      <c r="H43" s="231"/>
+      <c r="H43" s="244"/>
       <c r="I43" s="216"/>
       <c r="J43" s="217"/>
       <c r="K43" s="231"/>
@@ -16647,13 +16766,15 @@
     <row r="44" spans="2:21" ht="20.25" customHeight="1">
       <c r="B44" s="242"/>
       <c r="C44" s="229" t="s">
-        <v>636</v>
-      </c>
-      <c r="D44" s="218"/>
+        <v>657</v>
+      </c>
+      <c r="D44" s="218" t="s">
+        <v>643</v>
+      </c>
       <c r="E44" s="231"/>
       <c r="F44" s="232"/>
       <c r="G44" s="217"/>
-      <c r="H44" s="231"/>
+      <c r="H44" s="244"/>
       <c r="I44" s="216"/>
       <c r="J44" s="217"/>
       <c r="K44" s="231"/>
@@ -16669,11 +16790,16 @@
     </row>
     <row r="45" spans="2:21" ht="20.25" customHeight="1">
       <c r="B45" s="242"/>
-      <c r="D45" s="218"/>
+      <c r="C45" s="229" t="s">
+        <v>658</v>
+      </c>
+      <c r="D45" s="218" t="s">
+        <v>643</v>
+      </c>
       <c r="E45" s="231"/>
       <c r="F45" s="232"/>
       <c r="G45" s="217"/>
-      <c r="H45" s="231"/>
+      <c r="H45" s="244"/>
       <c r="I45" s="216"/>
       <c r="J45" s="217"/>
       <c r="K45" s="231"/>
@@ -16688,15 +16814,17 @@
       <c r="U45" s="309"/>
     </row>
     <row r="46" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B46" s="242" t="s">
-        <v>427</v>
-      </c>
-      <c r="C46" s="218"/>
-      <c r="D46" s="218"/>
+      <c r="B46" s="242"/>
+      <c r="C46" s="229" t="s">
+        <v>659</v>
+      </c>
+      <c r="D46" s="218" t="s">
+        <v>643</v>
+      </c>
       <c r="E46" s="231"/>
       <c r="F46" s="232"/>
       <c r="G46" s="217"/>
-      <c r="H46" s="231"/>
+      <c r="H46" s="244"/>
       <c r="I46" s="216"/>
       <c r="J46" s="217"/>
       <c r="K46" s="231"/>
@@ -16711,15 +16839,13 @@
       <c r="U46" s="309"/>
     </row>
     <row r="47" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B47" s="218"/>
-      <c r="C47" s="229" t="s">
-        <v>636</v>
-      </c>
+      <c r="B47" s="242"/>
+      <c r="C47" s="229"/>
       <c r="D47" s="218"/>
       <c r="E47" s="231"/>
       <c r="F47" s="232"/>
       <c r="G47" s="217"/>
-      <c r="H47" s="231"/>
+      <c r="H47" s="244"/>
       <c r="I47" s="216"/>
       <c r="J47" s="217"/>
       <c r="K47" s="231"/>
@@ -16734,13 +16860,15 @@
       <c r="U47" s="309"/>
     </row>
     <row r="48" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B48" s="218"/>
-      <c r="C48" s="218"/>
+      <c r="B48" s="242" t="s">
+        <v>662</v>
+      </c>
+      <c r="C48" s="229"/>
       <c r="D48" s="218"/>
       <c r="E48" s="231"/>
       <c r="F48" s="232"/>
       <c r="G48" s="217"/>
-      <c r="H48" s="231"/>
+      <c r="H48" s="244"/>
       <c r="I48" s="216"/>
       <c r="J48" s="217"/>
       <c r="K48" s="231"/>
@@ -16755,9 +16883,15 @@
       <c r="U48" s="309"/>
     </row>
     <row r="49" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B49" s="218"/>
-      <c r="C49" s="218"/>
-      <c r="D49" s="218"/>
+      <c r="B49" s="242" t="s">
+        <v>663</v>
+      </c>
+      <c r="C49" s="218" t="s">
+        <v>660</v>
+      </c>
+      <c r="D49" s="218" t="s">
+        <v>653</v>
+      </c>
       <c r="E49" s="231"/>
       <c r="F49" s="232"/>
       <c r="G49" s="217"/>
@@ -16776,9 +16910,13 @@
       <c r="U49" s="309"/>
     </row>
     <row r="50" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B50" s="218"/>
-      <c r="C50" s="218"/>
-      <c r="D50" s="218"/>
+      <c r="B50" s="242"/>
+      <c r="C50" s="70" t="s">
+        <v>661</v>
+      </c>
+      <c r="D50" s="218" t="s">
+        <v>653</v>
+      </c>
       <c r="E50" s="231"/>
       <c r="F50" s="232"/>
       <c r="G50" s="217"/>
@@ -16797,7 +16935,9 @@
       <c r="U50" s="309"/>
     </row>
     <row r="51" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B51" s="218"/>
+      <c r="B51" s="242" t="s">
+        <v>664</v>
+      </c>
       <c r="C51" s="218"/>
       <c r="D51" s="218"/>
       <c r="E51" s="231"/>
@@ -16818,9 +16958,13 @@
       <c r="U51" s="309"/>
     </row>
     <row r="52" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B52" s="218"/>
-      <c r="C52" s="218"/>
-      <c r="D52" s="218"/>
+      <c r="B52" s="242"/>
+      <c r="C52" s="229" t="s">
+        <v>665</v>
+      </c>
+      <c r="D52" s="218" t="s">
+        <v>653</v>
+      </c>
       <c r="E52" s="231"/>
       <c r="F52" s="232"/>
       <c r="G52" s="217"/>
@@ -16839,9 +16983,13 @@
       <c r="U52" s="309"/>
     </row>
     <row r="53" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B53" s="218"/>
-      <c r="C53" s="218"/>
-      <c r="D53" s="218"/>
+      <c r="B53" s="242"/>
+      <c r="C53" s="229" t="s">
+        <v>666</v>
+      </c>
+      <c r="D53" s="218" t="s">
+        <v>653</v>
+      </c>
       <c r="E53" s="231"/>
       <c r="F53" s="232"/>
       <c r="G53" s="217"/>
@@ -16860,9 +17008,13 @@
       <c r="U53" s="309"/>
     </row>
     <row r="54" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B54" s="218"/>
-      <c r="C54" s="218"/>
-      <c r="D54" s="218"/>
+      <c r="B54" s="242"/>
+      <c r="C54" s="229" t="s">
+        <v>667</v>
+      </c>
+      <c r="D54" s="218" t="s">
+        <v>653</v>
+      </c>
       <c r="E54" s="231"/>
       <c r="F54" s="232"/>
       <c r="G54" s="217"/>
@@ -16881,8 +17033,8 @@
       <c r="U54" s="309"/>
     </row>
     <row r="55" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B55" s="218"/>
-      <c r="C55" s="218"/>
+      <c r="B55" s="242"/>
+      <c r="C55" s="229"/>
       <c r="D55" s="218"/>
       <c r="E55" s="231"/>
       <c r="F55" s="232"/>
@@ -16902,8 +17054,10 @@
       <c r="U55" s="309"/>
     </row>
     <row r="56" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B56" s="218"/>
-      <c r="C56" s="218"/>
+      <c r="B56" s="242" t="s">
+        <v>668</v>
+      </c>
+      <c r="C56" s="229"/>
       <c r="D56" s="218"/>
       <c r="E56" s="231"/>
       <c r="F56" s="232"/>
@@ -16923,9 +17077,13 @@
       <c r="U56" s="309"/>
     </row>
     <row r="57" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B57" s="218"/>
-      <c r="C57" s="218"/>
-      <c r="D57" s="218"/>
+      <c r="B57" s="242"/>
+      <c r="C57" s="229" t="s">
+        <v>669</v>
+      </c>
+      <c r="D57" s="229" t="s">
+        <v>648</v>
+      </c>
       <c r="E57" s="231"/>
       <c r="F57" s="232"/>
       <c r="G57" s="217"/>
@@ -16944,9 +17102,13 @@
       <c r="U57" s="309"/>
     </row>
     <row r="58" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B58" s="218"/>
-      <c r="C58" s="218"/>
-      <c r="D58" s="218"/>
+      <c r="B58" s="242"/>
+      <c r="C58" s="229" t="s">
+        <v>670</v>
+      </c>
+      <c r="D58" s="229" t="s">
+        <v>648</v>
+      </c>
       <c r="E58" s="231"/>
       <c r="F58" s="232"/>
       <c r="G58" s="217"/>
@@ -16965,9 +17127,13 @@
       <c r="U58" s="309"/>
     </row>
     <row r="59" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B59" s="218"/>
-      <c r="C59" s="218"/>
-      <c r="D59" s="218"/>
+      <c r="B59" s="242"/>
+      <c r="C59" s="229" t="s">
+        <v>671</v>
+      </c>
+      <c r="D59" s="229" t="s">
+        <v>648</v>
+      </c>
       <c r="E59" s="231"/>
       <c r="F59" s="232"/>
       <c r="G59" s="217"/>
@@ -16986,9 +17152,13 @@
       <c r="U59" s="309"/>
     </row>
     <row r="60" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B60" s="218"/>
-      <c r="C60" s="218"/>
-      <c r="D60" s="218"/>
+      <c r="B60" s="242"/>
+      <c r="C60" s="229" t="s">
+        <v>672</v>
+      </c>
+      <c r="D60" s="229" t="s">
+        <v>648</v>
+      </c>
       <c r="E60" s="231"/>
       <c r="F60" s="232"/>
       <c r="G60" s="217"/>
@@ -17007,8 +17177,8 @@
       <c r="U60" s="309"/>
     </row>
     <row r="61" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B61" s="218"/>
-      <c r="C61" s="218"/>
+      <c r="B61" s="242"/>
+      <c r="C61" s="229"/>
       <c r="D61" s="218"/>
       <c r="E61" s="231"/>
       <c r="F61" s="232"/>
@@ -17028,8 +17198,7 @@
       <c r="U61" s="309"/>
     </row>
     <row r="62" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B62" s="218"/>
-      <c r="C62" s="218"/>
+      <c r="B62" s="242"/>
       <c r="D62" s="218"/>
       <c r="E62" s="231"/>
       <c r="F62" s="232"/>
@@ -17049,7 +17218,9 @@
       <c r="U62" s="309"/>
     </row>
     <row r="63" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B63" s="218"/>
+      <c r="B63" s="242" t="s">
+        <v>427</v>
+      </c>
       <c r="C63" s="218"/>
       <c r="D63" s="218"/>
       <c r="E63" s="231"/>
@@ -17071,7 +17242,9 @@
     </row>
     <row r="64" spans="2:21" ht="20.25" customHeight="1">
       <c r="B64" s="218"/>
-      <c r="C64" s="218"/>
+      <c r="C64" s="229" t="s">
+        <v>636</v>
+      </c>
       <c r="D64" s="218"/>
       <c r="E64" s="231"/>
       <c r="F64" s="232"/>
@@ -19656,18 +19829,18 @@
       <c r="B187" s="218"/>
       <c r="C187" s="218"/>
       <c r="D187" s="218"/>
-      <c r="E187" s="219"/>
-      <c r="F187" s="220"/>
-      <c r="G187" s="221"/>
-      <c r="H187" s="219"/>
-      <c r="I187" s="218"/>
-      <c r="J187" s="221"/>
-      <c r="K187" s="219"/>
-      <c r="L187" s="218"/>
-      <c r="M187" s="221"/>
-      <c r="N187" s="219"/>
-      <c r="O187" s="218"/>
-      <c r="P187" s="221"/>
+      <c r="E187" s="231"/>
+      <c r="F187" s="232"/>
+      <c r="G187" s="217"/>
+      <c r="H187" s="231"/>
+      <c r="I187" s="216"/>
+      <c r="J187" s="217"/>
+      <c r="K187" s="231"/>
+      <c r="L187" s="216"/>
+      <c r="M187" s="217"/>
+      <c r="N187" s="231"/>
+      <c r="O187" s="216"/>
+      <c r="P187" s="217"/>
       <c r="R187" s="307"/>
       <c r="S187" s="308"/>
       <c r="T187" s="308"/>
@@ -19677,18 +19850,18 @@
       <c r="B188" s="218"/>
       <c r="C188" s="218"/>
       <c r="D188" s="218"/>
-      <c r="E188" s="222"/>
-      <c r="F188" s="218"/>
-      <c r="G188" s="221"/>
-      <c r="H188" s="222"/>
-      <c r="I188" s="218"/>
-      <c r="J188" s="221"/>
-      <c r="K188" s="222"/>
-      <c r="L188" s="218"/>
-      <c r="M188" s="221"/>
-      <c r="N188" s="222"/>
-      <c r="O188" s="218"/>
-      <c r="P188" s="221"/>
+      <c r="E188" s="231"/>
+      <c r="F188" s="232"/>
+      <c r="G188" s="217"/>
+      <c r="H188" s="231"/>
+      <c r="I188" s="216"/>
+      <c r="J188" s="217"/>
+      <c r="K188" s="231"/>
+      <c r="L188" s="216"/>
+      <c r="M188" s="217"/>
+      <c r="N188" s="231"/>
+      <c r="O188" s="216"/>
+      <c r="P188" s="217"/>
       <c r="R188" s="307"/>
       <c r="S188" s="308"/>
       <c r="T188" s="308"/>
@@ -19698,18 +19871,18 @@
       <c r="B189" s="218"/>
       <c r="C189" s="218"/>
       <c r="D189" s="218"/>
-      <c r="E189" s="222"/>
-      <c r="F189" s="218"/>
-      <c r="G189" s="221"/>
-      <c r="H189" s="222"/>
-      <c r="I189" s="218"/>
-      <c r="J189" s="221"/>
-      <c r="K189" s="222"/>
-      <c r="L189" s="218"/>
-      <c r="M189" s="221"/>
-      <c r="N189" s="222"/>
-      <c r="O189" s="218"/>
-      <c r="P189" s="221"/>
+      <c r="E189" s="231"/>
+      <c r="F189" s="232"/>
+      <c r="G189" s="217"/>
+      <c r="H189" s="231"/>
+      <c r="I189" s="216"/>
+      <c r="J189" s="217"/>
+      <c r="K189" s="231"/>
+      <c r="L189" s="216"/>
+      <c r="M189" s="217"/>
+      <c r="N189" s="231"/>
+      <c r="O189" s="216"/>
+      <c r="P189" s="217"/>
       <c r="R189" s="307"/>
       <c r="S189" s="308"/>
       <c r="T189" s="308"/>
@@ -19719,18 +19892,18 @@
       <c r="B190" s="218"/>
       <c r="C190" s="218"/>
       <c r="D190" s="218"/>
-      <c r="E190" s="219"/>
-      <c r="F190" s="223"/>
-      <c r="G190" s="224"/>
-      <c r="H190" s="219"/>
-      <c r="I190" s="223"/>
-      <c r="J190" s="224"/>
-      <c r="K190" s="219"/>
-      <c r="L190" s="223"/>
-      <c r="M190" s="224"/>
-      <c r="N190" s="219"/>
-      <c r="O190" s="223"/>
-      <c r="P190" s="224"/>
+      <c r="E190" s="231"/>
+      <c r="F190" s="232"/>
+      <c r="G190" s="217"/>
+      <c r="H190" s="231"/>
+      <c r="I190" s="216"/>
+      <c r="J190" s="217"/>
+      <c r="K190" s="231"/>
+      <c r="L190" s="216"/>
+      <c r="M190" s="217"/>
+      <c r="N190" s="231"/>
+      <c r="O190" s="216"/>
+      <c r="P190" s="217"/>
       <c r="R190" s="307"/>
       <c r="S190" s="308"/>
       <c r="T190" s="308"/>
@@ -19740,39 +19913,39 @@
       <c r="B191" s="218"/>
       <c r="C191" s="218"/>
       <c r="D191" s="218"/>
-      <c r="E191" s="222"/>
-      <c r="F191" s="223"/>
-      <c r="G191" s="224"/>
-      <c r="H191" s="222"/>
-      <c r="I191" s="223"/>
-      <c r="J191" s="224"/>
-      <c r="K191" s="222"/>
-      <c r="L191" s="223"/>
-      <c r="M191" s="224"/>
-      <c r="N191" s="222"/>
-      <c r="O191" s="223"/>
-      <c r="P191" s="224"/>
+      <c r="E191" s="231"/>
+      <c r="F191" s="232"/>
+      <c r="G191" s="217"/>
+      <c r="H191" s="231"/>
+      <c r="I191" s="216"/>
+      <c r="J191" s="217"/>
+      <c r="K191" s="231"/>
+      <c r="L191" s="216"/>
+      <c r="M191" s="217"/>
+      <c r="N191" s="231"/>
+      <c r="O191" s="216"/>
+      <c r="P191" s="217"/>
       <c r="R191" s="307"/>
       <c r="S191" s="308"/>
       <c r="T191" s="308"/>
       <c r="U191" s="309"/>
     </row>
     <row r="192" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B192" s="229"/>
+      <c r="B192" s="218"/>
       <c r="C192" s="218"/>
       <c r="D192" s="218"/>
-      <c r="E192" s="222"/>
-      <c r="F192" s="223"/>
-      <c r="G192" s="224"/>
-      <c r="H192" s="222"/>
-      <c r="I192" s="223"/>
-      <c r="J192" s="224"/>
-      <c r="K192" s="222"/>
-      <c r="L192" s="223"/>
-      <c r="M192" s="224"/>
-      <c r="N192" s="222"/>
-      <c r="O192" s="223"/>
-      <c r="P192" s="224"/>
+      <c r="E192" s="231"/>
+      <c r="F192" s="232"/>
+      <c r="G192" s="217"/>
+      <c r="H192" s="231"/>
+      <c r="I192" s="216"/>
+      <c r="J192" s="217"/>
+      <c r="K192" s="231"/>
+      <c r="L192" s="216"/>
+      <c r="M192" s="217"/>
+      <c r="N192" s="231"/>
+      <c r="O192" s="216"/>
+      <c r="P192" s="217"/>
       <c r="R192" s="307"/>
       <c r="S192" s="308"/>
       <c r="T192" s="308"/>
@@ -19782,18 +19955,18 @@
       <c r="B193" s="218"/>
       <c r="C193" s="218"/>
       <c r="D193" s="218"/>
-      <c r="E193" s="219"/>
-      <c r="F193" s="223"/>
-      <c r="G193" s="224"/>
-      <c r="H193" s="219"/>
-      <c r="I193" s="223"/>
-      <c r="J193" s="224"/>
-      <c r="K193" s="219"/>
-      <c r="L193" s="223"/>
-      <c r="M193" s="224"/>
-      <c r="N193" s="219"/>
-      <c r="O193" s="223"/>
-      <c r="P193" s="224"/>
+      <c r="E193" s="231"/>
+      <c r="F193" s="232"/>
+      <c r="G193" s="217"/>
+      <c r="H193" s="231"/>
+      <c r="I193" s="216"/>
+      <c r="J193" s="217"/>
+      <c r="K193" s="231"/>
+      <c r="L193" s="216"/>
+      <c r="M193" s="217"/>
+      <c r="N193" s="231"/>
+      <c r="O193" s="216"/>
+      <c r="P193" s="217"/>
       <c r="R193" s="307"/>
       <c r="S193" s="308"/>
       <c r="T193" s="308"/>
@@ -19803,18 +19976,18 @@
       <c r="B194" s="218"/>
       <c r="C194" s="218"/>
       <c r="D194" s="218"/>
-      <c r="E194" s="222"/>
-      <c r="F194" s="223"/>
-      <c r="G194" s="224"/>
-      <c r="H194" s="222"/>
-      <c r="I194" s="223"/>
-      <c r="J194" s="224"/>
-      <c r="K194" s="222"/>
-      <c r="L194" s="223"/>
-      <c r="M194" s="224"/>
-      <c r="N194" s="222"/>
-      <c r="O194" s="223"/>
-      <c r="P194" s="224"/>
+      <c r="E194" s="231"/>
+      <c r="F194" s="232"/>
+      <c r="G194" s="217"/>
+      <c r="H194" s="231"/>
+      <c r="I194" s="216"/>
+      <c r="J194" s="217"/>
+      <c r="K194" s="231"/>
+      <c r="L194" s="216"/>
+      <c r="M194" s="217"/>
+      <c r="N194" s="231"/>
+      <c r="O194" s="216"/>
+      <c r="P194" s="217"/>
       <c r="R194" s="307"/>
       <c r="S194" s="308"/>
       <c r="T194" s="308"/>
@@ -19824,18 +19997,18 @@
       <c r="B195" s="218"/>
       <c r="C195" s="218"/>
       <c r="D195" s="218"/>
-      <c r="E195" s="222"/>
-      <c r="F195" s="223"/>
-      <c r="G195" s="224"/>
-      <c r="H195" s="222"/>
-      <c r="I195" s="223"/>
-      <c r="J195" s="224"/>
-      <c r="K195" s="222"/>
-      <c r="L195" s="223"/>
-      <c r="M195" s="224"/>
-      <c r="N195" s="222"/>
-      <c r="O195" s="223"/>
-      <c r="P195" s="224"/>
+      <c r="E195" s="231"/>
+      <c r="F195" s="232"/>
+      <c r="G195" s="217"/>
+      <c r="H195" s="231"/>
+      <c r="I195" s="216"/>
+      <c r="J195" s="217"/>
+      <c r="K195" s="231"/>
+      <c r="L195" s="216"/>
+      <c r="M195" s="217"/>
+      <c r="N195" s="231"/>
+      <c r="O195" s="216"/>
+      <c r="P195" s="217"/>
       <c r="R195" s="307"/>
       <c r="S195" s="308"/>
       <c r="T195" s="308"/>
@@ -19845,95 +20018,472 @@
       <c r="B196" s="218"/>
       <c r="C196" s="218"/>
       <c r="D196" s="218"/>
-      <c r="E196" s="219"/>
-      <c r="F196" s="223"/>
-      <c r="G196" s="224"/>
-      <c r="H196" s="219"/>
-      <c r="I196" s="223"/>
-      <c r="J196" s="224"/>
-      <c r="K196" s="219"/>
-      <c r="L196" s="223"/>
-      <c r="M196" s="224"/>
-      <c r="N196" s="219"/>
-      <c r="O196" s="223"/>
-      <c r="P196" s="224"/>
+      <c r="E196" s="231"/>
+      <c r="F196" s="232"/>
+      <c r="G196" s="217"/>
+      <c r="H196" s="231"/>
+      <c r="I196" s="216"/>
+      <c r="J196" s="217"/>
+      <c r="K196" s="231"/>
+      <c r="L196" s="216"/>
+      <c r="M196" s="217"/>
+      <c r="N196" s="231"/>
+      <c r="O196" s="216"/>
+      <c r="P196" s="217"/>
       <c r="R196" s="307"/>
       <c r="S196" s="308"/>
       <c r="T196" s="308"/>
       <c r="U196" s="309"/>
     </row>
-    <row r="197" spans="2:21" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B197" s="225"/>
-      <c r="C197" s="226"/>
-      <c r="D197" s="227"/>
-      <c r="E197" s="230"/>
-      <c r="F197" s="226"/>
-      <c r="G197" s="228"/>
-      <c r="H197" s="230"/>
-      <c r="I197" s="226"/>
-      <c r="J197" s="228"/>
-      <c r="K197" s="230"/>
-      <c r="L197" s="226"/>
-      <c r="M197" s="228"/>
-      <c r="N197" s="230"/>
-      <c r="O197" s="226"/>
-      <c r="P197" s="228"/>
-      <c r="R197" s="310"/>
-      <c r="S197" s="311"/>
-      <c r="T197" s="311"/>
-      <c r="U197" s="312"/>
-    </row>
-    <row r="198" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B198" s="186"/>
-      <c r="C198" s="186"/>
-      <c r="D198" s="186"/>
-      <c r="E198" s="186"/>
-      <c r="F198" s="186"/>
-      <c r="G198" s="186"/>
-      <c r="H198" s="186"/>
-      <c r="I198" s="186"/>
-      <c r="J198" s="186"/>
-      <c r="K198" s="186"/>
-      <c r="L198" s="186"/>
-      <c r="M198" s="186"/>
-      <c r="N198" s="186"/>
-      <c r="O198" s="186"/>
-      <c r="P198" s="186"/>
-      <c r="Q198" s="186"/>
+    <row r="197" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B197" s="218"/>
+      <c r="C197" s="218"/>
+      <c r="D197" s="218"/>
+      <c r="E197" s="231"/>
+      <c r="F197" s="232"/>
+      <c r="G197" s="217"/>
+      <c r="H197" s="231"/>
+      <c r="I197" s="216"/>
+      <c r="J197" s="217"/>
+      <c r="K197" s="231"/>
+      <c r="L197" s="216"/>
+      <c r="M197" s="217"/>
+      <c r="N197" s="231"/>
+      <c r="O197" s="216"/>
+      <c r="P197" s="217"/>
+      <c r="R197" s="307"/>
+      <c r="S197" s="308"/>
+      <c r="T197" s="308"/>
+      <c r="U197" s="309"/>
+    </row>
+    <row r="198" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B198" s="218"/>
+      <c r="C198" s="218"/>
+      <c r="D198" s="218"/>
+      <c r="E198" s="231"/>
+      <c r="F198" s="232"/>
+      <c r="G198" s="217"/>
+      <c r="H198" s="231"/>
+      <c r="I198" s="216"/>
+      <c r="J198" s="217"/>
+      <c r="K198" s="231"/>
+      <c r="L198" s="216"/>
+      <c r="M198" s="217"/>
+      <c r="N198" s="231"/>
+      <c r="O198" s="216"/>
+      <c r="P198" s="217"/>
+      <c r="R198" s="307"/>
+      <c r="S198" s="308"/>
+      <c r="T198" s="308"/>
+      <c r="U198" s="309"/>
+    </row>
+    <row r="199" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B199" s="218"/>
+      <c r="C199" s="218"/>
+      <c r="D199" s="218"/>
+      <c r="E199" s="231"/>
+      <c r="F199" s="232"/>
+      <c r="G199" s="217"/>
+      <c r="H199" s="231"/>
+      <c r="I199" s="216"/>
+      <c r="J199" s="217"/>
+      <c r="K199" s="231"/>
+      <c r="L199" s="216"/>
+      <c r="M199" s="217"/>
+      <c r="N199" s="231"/>
+      <c r="O199" s="216"/>
+      <c r="P199" s="217"/>
+      <c r="R199" s="307"/>
+      <c r="S199" s="308"/>
+      <c r="T199" s="308"/>
+      <c r="U199" s="309"/>
+    </row>
+    <row r="200" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B200" s="218"/>
+      <c r="C200" s="218"/>
+      <c r="D200" s="218"/>
+      <c r="E200" s="231"/>
+      <c r="F200" s="232"/>
+      <c r="G200" s="217"/>
+      <c r="H200" s="231"/>
+      <c r="I200" s="216"/>
+      <c r="J200" s="217"/>
+      <c r="K200" s="231"/>
+      <c r="L200" s="216"/>
+      <c r="M200" s="217"/>
+      <c r="N200" s="231"/>
+      <c r="O200" s="216"/>
+      <c r="P200" s="217"/>
+      <c r="R200" s="307"/>
+      <c r="S200" s="308"/>
+      <c r="T200" s="308"/>
+      <c r="U200" s="309"/>
+    </row>
+    <row r="201" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B201" s="218"/>
+      <c r="C201" s="218"/>
+      <c r="D201" s="218"/>
+      <c r="E201" s="231"/>
+      <c r="F201" s="232"/>
+      <c r="G201" s="217"/>
+      <c r="H201" s="231"/>
+      <c r="I201" s="216"/>
+      <c r="J201" s="217"/>
+      <c r="K201" s="231"/>
+      <c r="L201" s="216"/>
+      <c r="M201" s="217"/>
+      <c r="N201" s="231"/>
+      <c r="O201" s="216"/>
+      <c r="P201" s="217"/>
+      <c r="R201" s="307"/>
+      <c r="S201" s="308"/>
+      <c r="T201" s="308"/>
+      <c r="U201" s="309"/>
+    </row>
+    <row r="202" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B202" s="218"/>
+      <c r="C202" s="218"/>
+      <c r="D202" s="218"/>
+      <c r="E202" s="231"/>
+      <c r="F202" s="232"/>
+      <c r="G202" s="217"/>
+      <c r="H202" s="231"/>
+      <c r="I202" s="216"/>
+      <c r="J202" s="217"/>
+      <c r="K202" s="231"/>
+      <c r="L202" s="216"/>
+      <c r="M202" s="217"/>
+      <c r="N202" s="231"/>
+      <c r="O202" s="216"/>
+      <c r="P202" s="217"/>
+      <c r="R202" s="307"/>
+      <c r="S202" s="308"/>
+      <c r="T202" s="308"/>
+      <c r="U202" s="309"/>
+    </row>
+    <row r="203" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B203" s="218"/>
+      <c r="C203" s="218"/>
+      <c r="D203" s="218"/>
+      <c r="E203" s="231"/>
+      <c r="F203" s="232"/>
+      <c r="G203" s="217"/>
+      <c r="H203" s="231"/>
+      <c r="I203" s="216"/>
+      <c r="J203" s="217"/>
+      <c r="K203" s="231"/>
+      <c r="L203" s="216"/>
+      <c r="M203" s="217"/>
+      <c r="N203" s="231"/>
+      <c r="O203" s="216"/>
+      <c r="P203" s="217"/>
+      <c r="R203" s="307"/>
+      <c r="S203" s="308"/>
+      <c r="T203" s="308"/>
+      <c r="U203" s="309"/>
+    </row>
+    <row r="204" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B204" s="218"/>
+      <c r="C204" s="218"/>
+      <c r="D204" s="218"/>
+      <c r="E204" s="219"/>
+      <c r="F204" s="220"/>
+      <c r="G204" s="221"/>
+      <c r="H204" s="219"/>
+      <c r="I204" s="218"/>
+      <c r="J204" s="221"/>
+      <c r="K204" s="219"/>
+      <c r="L204" s="218"/>
+      <c r="M204" s="221"/>
+      <c r="N204" s="219"/>
+      <c r="O204" s="218"/>
+      <c r="P204" s="221"/>
+      <c r="R204" s="307"/>
+      <c r="S204" s="308"/>
+      <c r="T204" s="308"/>
+      <c r="U204" s="309"/>
+    </row>
+    <row r="205" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B205" s="218"/>
+      <c r="C205" s="218"/>
+      <c r="D205" s="218"/>
+      <c r="E205" s="222"/>
+      <c r="F205" s="218"/>
+      <c r="G205" s="221"/>
+      <c r="H205" s="222"/>
+      <c r="I205" s="218"/>
+      <c r="J205" s="221"/>
+      <c r="K205" s="222"/>
+      <c r="L205" s="218"/>
+      <c r="M205" s="221"/>
+      <c r="N205" s="222"/>
+      <c r="O205" s="218"/>
+      <c r="P205" s="221"/>
+      <c r="R205" s="307"/>
+      <c r="S205" s="308"/>
+      <c r="T205" s="308"/>
+      <c r="U205" s="309"/>
+    </row>
+    <row r="206" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B206" s="218"/>
+      <c r="C206" s="218"/>
+      <c r="D206" s="218"/>
+      <c r="E206" s="222"/>
+      <c r="F206" s="218"/>
+      <c r="G206" s="221"/>
+      <c r="H206" s="222"/>
+      <c r="I206" s="218"/>
+      <c r="J206" s="221"/>
+      <c r="K206" s="222"/>
+      <c r="L206" s="218"/>
+      <c r="M206" s="221"/>
+      <c r="N206" s="222"/>
+      <c r="O206" s="218"/>
+      <c r="P206" s="221"/>
+      <c r="R206" s="307"/>
+      <c r="S206" s="308"/>
+      <c r="T206" s="308"/>
+      <c r="U206" s="309"/>
+    </row>
+    <row r="207" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B207" s="218"/>
+      <c r="C207" s="218"/>
+      <c r="D207" s="218"/>
+      <c r="E207" s="219"/>
+      <c r="F207" s="223"/>
+      <c r="G207" s="224"/>
+      <c r="H207" s="219"/>
+      <c r="I207" s="223"/>
+      <c r="J207" s="224"/>
+      <c r="K207" s="219"/>
+      <c r="L207" s="223"/>
+      <c r="M207" s="224"/>
+      <c r="N207" s="219"/>
+      <c r="O207" s="223"/>
+      <c r="P207" s="224"/>
+      <c r="R207" s="307"/>
+      <c r="S207" s="308"/>
+      <c r="T207" s="308"/>
+      <c r="U207" s="309"/>
+    </row>
+    <row r="208" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B208" s="218"/>
+      <c r="C208" s="218"/>
+      <c r="D208" s="218"/>
+      <c r="E208" s="222"/>
+      <c r="F208" s="223"/>
+      <c r="G208" s="224"/>
+      <c r="H208" s="222"/>
+      <c r="I208" s="223"/>
+      <c r="J208" s="224"/>
+      <c r="K208" s="222"/>
+      <c r="L208" s="223"/>
+      <c r="M208" s="224"/>
+      <c r="N208" s="222"/>
+      <c r="O208" s="223"/>
+      <c r="P208" s="224"/>
+      <c r="R208" s="307"/>
+      <c r="S208" s="308"/>
+      <c r="T208" s="308"/>
+      <c r="U208" s="309"/>
+    </row>
+    <row r="209" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B209" s="229"/>
+      <c r="C209" s="218"/>
+      <c r="D209" s="218"/>
+      <c r="E209" s="222"/>
+      <c r="F209" s="223"/>
+      <c r="G209" s="224"/>
+      <c r="H209" s="222"/>
+      <c r="I209" s="223"/>
+      <c r="J209" s="224"/>
+      <c r="K209" s="222"/>
+      <c r="L209" s="223"/>
+      <c r="M209" s="224"/>
+      <c r="N209" s="222"/>
+      <c r="O209" s="223"/>
+      <c r="P209" s="224"/>
+      <c r="R209" s="307"/>
+      <c r="S209" s="308"/>
+      <c r="T209" s="308"/>
+      <c r="U209" s="309"/>
+    </row>
+    <row r="210" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B210" s="218"/>
+      <c r="C210" s="218"/>
+      <c r="D210" s="218"/>
+      <c r="E210" s="219"/>
+      <c r="F210" s="223"/>
+      <c r="G210" s="224"/>
+      <c r="H210" s="219"/>
+      <c r="I210" s="223"/>
+      <c r="J210" s="224"/>
+      <c r="K210" s="219"/>
+      <c r="L210" s="223"/>
+      <c r="M210" s="224"/>
+      <c r="N210" s="219"/>
+      <c r="O210" s="223"/>
+      <c r="P210" s="224"/>
+      <c r="R210" s="307"/>
+      <c r="S210" s="308"/>
+      <c r="T210" s="308"/>
+      <c r="U210" s="309"/>
+    </row>
+    <row r="211" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B211" s="218"/>
+      <c r="C211" s="218"/>
+      <c r="D211" s="218"/>
+      <c r="E211" s="222"/>
+      <c r="F211" s="223"/>
+      <c r="G211" s="224"/>
+      <c r="H211" s="222"/>
+      <c r="I211" s="223"/>
+      <c r="J211" s="224"/>
+      <c r="K211" s="222"/>
+      <c r="L211" s="223"/>
+      <c r="M211" s="224"/>
+      <c r="N211" s="222"/>
+      <c r="O211" s="223"/>
+      <c r="P211" s="224"/>
+      <c r="R211" s="307"/>
+      <c r="S211" s="308"/>
+      <c r="T211" s="308"/>
+      <c r="U211" s="309"/>
+    </row>
+    <row r="212" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B212" s="218"/>
+      <c r="C212" s="218"/>
+      <c r="D212" s="218"/>
+      <c r="E212" s="222"/>
+      <c r="F212" s="223"/>
+      <c r="G212" s="224"/>
+      <c r="H212" s="222"/>
+      <c r="I212" s="223"/>
+      <c r="J212" s="224"/>
+      <c r="K212" s="222"/>
+      <c r="L212" s="223"/>
+      <c r="M212" s="224"/>
+      <c r="N212" s="222"/>
+      <c r="O212" s="223"/>
+      <c r="P212" s="224"/>
+      <c r="R212" s="307"/>
+      <c r="S212" s="308"/>
+      <c r="T212" s="308"/>
+      <c r="U212" s="309"/>
+    </row>
+    <row r="213" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B213" s="218"/>
+      <c r="C213" s="218"/>
+      <c r="D213" s="218"/>
+      <c r="E213" s="219"/>
+      <c r="F213" s="223"/>
+      <c r="G213" s="224"/>
+      <c r="H213" s="219"/>
+      <c r="I213" s="223"/>
+      <c r="J213" s="224"/>
+      <c r="K213" s="219"/>
+      <c r="L213" s="223"/>
+      <c r="M213" s="224"/>
+      <c r="N213" s="219"/>
+      <c r="O213" s="223"/>
+      <c r="P213" s="224"/>
+      <c r="R213" s="307"/>
+      <c r="S213" s="308"/>
+      <c r="T213" s="308"/>
+      <c r="U213" s="309"/>
+    </row>
+    <row r="214" spans="2:21" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B214" s="225"/>
+      <c r="C214" s="226"/>
+      <c r="D214" s="227"/>
+      <c r="E214" s="230"/>
+      <c r="F214" s="226"/>
+      <c r="G214" s="228"/>
+      <c r="H214" s="230"/>
+      <c r="I214" s="226"/>
+      <c r="J214" s="228"/>
+      <c r="K214" s="230"/>
+      <c r="L214" s="226"/>
+      <c r="M214" s="228"/>
+      <c r="N214" s="230"/>
+      <c r="O214" s="226"/>
+      <c r="P214" s="228"/>
+      <c r="R214" s="310"/>
+      <c r="S214" s="311"/>
+      <c r="T214" s="311"/>
+      <c r="U214" s="312"/>
+    </row>
+    <row r="215" spans="2:21" ht="15.75" customHeight="1">
+      <c r="B215" s="186"/>
+      <c r="C215" s="186"/>
+      <c r="D215" s="186"/>
+      <c r="E215" s="186"/>
+      <c r="F215" s="186"/>
+      <c r="G215" s="186"/>
+      <c r="H215" s="186"/>
+      <c r="I215" s="186"/>
+      <c r="J215" s="186"/>
+      <c r="K215" s="186"/>
+      <c r="L215" s="186"/>
+      <c r="M215" s="186"/>
+      <c r="N215" s="186"/>
+      <c r="O215" s="186"/>
+      <c r="P215" s="186"/>
+      <c r="Q215" s="186"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="H3:P3"/>
-    <mergeCell ref="R6:U197"/>
+    <mergeCell ref="R6:U214"/>
   </mergeCells>
-  <conditionalFormatting sqref="B12:D27 C28:C38 B28:B196 D38 C40 C43:C44 C47:C203 D41:D196">
-    <cfRule type="expression" dxfId="5" priority="3">
+  <conditionalFormatting sqref="B12:D27 C28:C38 B28:B213 D38 C40:C48 D51 C51:C61 C64:C220 D59:D213">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>IF((B12&lt;&gt;"")*AND(F12&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>IF((C35&lt;&gt;"")*AND(G38&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39 C41">
-    <cfRule type="expression" dxfId="3" priority="5">
+  <conditionalFormatting sqref="C39 C49">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>IF((C39&lt;&gt;"")*AND(G40&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="expression" dxfId="2" priority="14">
-      <formula>IF((C46&lt;&gt;"")*AND(G45&lt;&gt;""),1,0)</formula>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="6" priority="18">
+      <formula>IF((C63&lt;&gt;"")*AND(G62&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:D37">
-    <cfRule type="expression" dxfId="1" priority="10">
+    <cfRule type="expression" dxfId="5" priority="14">
       <formula>IF((C28&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39:D40">
+  <conditionalFormatting sqref="D39:D42 D47:D48">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>IF((D39&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D43:D46">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>IF((D43&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52:D56">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>IF((D52&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49:D50">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>IF((D49&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D57:D58">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>IF((D39&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
+      <formula>IF((D57&lt;&gt;"")*AND(H57&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
add : modifications orientation
</commit_message>
<xml_diff>
--- a/doc/chiffrier_sim_vie.xlsx
+++ b/doc/chiffrier_sim_vie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travail\sim_vie\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C994FE-BE65-4586-9275-53CF16CB40CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2A7237-7C6B-4C8E-86B5-F79748EEAA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4088,20 +4088,93 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -4130,84 +4203,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4218,17 +4227,8 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -4267,37 +4267,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="0" shrinkToFit="0"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <alignment wrapText="0" shrinkToFit="0"/>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -7606,16 +7576,16 @@
       <c r="W10" s="29"/>
     </row>
     <row r="11" spans="1:107" thickBot="1">
-      <c r="G11" s="281" t="s">
+      <c r="G11" s="261" t="s">
         <v>324</v>
       </c>
-      <c r="H11" s="282"/>
-      <c r="I11" s="282"/>
-      <c r="J11" s="282"/>
-      <c r="K11" s="282"/>
-      <c r="L11" s="282"/>
-      <c r="M11" s="282"/>
-      <c r="N11" s="283"/>
+      <c r="H11" s="262"/>
+      <c r="I11" s="262"/>
+      <c r="J11" s="262"/>
+      <c r="K11" s="262"/>
+      <c r="L11" s="262"/>
+      <c r="M11" s="262"/>
+      <c r="N11" s="263"/>
       <c r="O11" s="48"/>
       <c r="P11" s="39"/>
       <c r="Q11" s="39"/>
@@ -7653,66 +7623,66 @@
       <c r="AW11" s="47"/>
       <c r="AX11" s="113"/>
       <c r="AY11" s="115"/>
-      <c r="BD11" s="281" t="s">
+      <c r="BD11" s="261" t="s">
         <v>324</v>
       </c>
-      <c r="BE11" s="282"/>
-      <c r="BF11" s="282"/>
-      <c r="BG11" s="282"/>
-      <c r="BH11" s="282"/>
-      <c r="BI11" s="282"/>
-      <c r="BJ11" s="282"/>
-      <c r="BK11" s="283"/>
-      <c r="BP11" s="281" t="s">
+      <c r="BE11" s="262"/>
+      <c r="BF11" s="262"/>
+      <c r="BG11" s="262"/>
+      <c r="BH11" s="262"/>
+      <c r="BI11" s="262"/>
+      <c r="BJ11" s="262"/>
+      <c r="BK11" s="263"/>
+      <c r="BP11" s="261" t="s">
         <v>324</v>
       </c>
-      <c r="BQ11" s="282"/>
-      <c r="BR11" s="282"/>
-      <c r="BS11" s="282"/>
-      <c r="BT11" s="282"/>
-      <c r="BU11" s="282"/>
-      <c r="BV11" s="282"/>
-      <c r="BW11" s="283"/>
-      <c r="CA11" s="281" t="s">
+      <c r="BQ11" s="262"/>
+      <c r="BR11" s="262"/>
+      <c r="BS11" s="262"/>
+      <c r="BT11" s="262"/>
+      <c r="BU11" s="262"/>
+      <c r="BV11" s="262"/>
+      <c r="BW11" s="263"/>
+      <c r="CA11" s="261" t="s">
         <v>324</v>
       </c>
-      <c r="CB11" s="282"/>
-      <c r="CC11" s="282"/>
-      <c r="CD11" s="282"/>
-      <c r="CE11" s="282"/>
-      <c r="CF11" s="282"/>
-      <c r="CG11" s="282"/>
-      <c r="CH11" s="283"/>
-      <c r="CL11" s="281" t="s">
+      <c r="CB11" s="262"/>
+      <c r="CC11" s="262"/>
+      <c r="CD11" s="262"/>
+      <c r="CE11" s="262"/>
+      <c r="CF11" s="262"/>
+      <c r="CG11" s="262"/>
+      <c r="CH11" s="263"/>
+      <c r="CL11" s="261" t="s">
         <v>324</v>
       </c>
-      <c r="CM11" s="282"/>
-      <c r="CN11" s="282"/>
-      <c r="CO11" s="282"/>
-      <c r="CP11" s="282"/>
-      <c r="CQ11" s="282"/>
-      <c r="CR11" s="282"/>
-      <c r="CS11" s="283"/>
-      <c r="CV11" s="281" t="s">
+      <c r="CM11" s="262"/>
+      <c r="CN11" s="262"/>
+      <c r="CO11" s="262"/>
+      <c r="CP11" s="262"/>
+      <c r="CQ11" s="262"/>
+      <c r="CR11" s="262"/>
+      <c r="CS11" s="263"/>
+      <c r="CV11" s="261" t="s">
         <v>324</v>
       </c>
-      <c r="CW11" s="282"/>
-      <c r="CX11" s="282"/>
-      <c r="CY11" s="282"/>
-      <c r="CZ11" s="282"/>
-      <c r="DA11" s="282"/>
-      <c r="DB11" s="282"/>
-      <c r="DC11" s="283"/>
+      <c r="CW11" s="262"/>
+      <c r="CX11" s="262"/>
+      <c r="CY11" s="262"/>
+      <c r="CZ11" s="262"/>
+      <c r="DA11" s="262"/>
+      <c r="DB11" s="262"/>
+      <c r="DC11" s="263"/>
     </row>
     <row r="12" spans="1:107" thickBot="1">
-      <c r="G12" s="284"/>
-      <c r="H12" s="285"/>
-      <c r="I12" s="285"/>
-      <c r="J12" s="285"/>
-      <c r="K12" s="285"/>
-      <c r="L12" s="285"/>
-      <c r="M12" s="285"/>
-      <c r="N12" s="286"/>
+      <c r="G12" s="264"/>
+      <c r="H12" s="265"/>
+      <c r="I12" s="265"/>
+      <c r="J12" s="265"/>
+      <c r="K12" s="265"/>
+      <c r="L12" s="265"/>
+      <c r="M12" s="265"/>
+      <c r="N12" s="266"/>
       <c r="O12" s="40"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
@@ -7723,49 +7693,49 @@
       <c r="V12" s="29"/>
       <c r="W12" s="29"/>
       <c r="AX12" s="42"/>
-      <c r="AY12" s="290" t="s">
+      <c r="AY12" s="258" t="s">
         <v>323</v>
       </c>
-      <c r="BD12" s="284"/>
-      <c r="BE12" s="285"/>
-      <c r="BF12" s="285"/>
-      <c r="BG12" s="285"/>
-      <c r="BH12" s="285"/>
-      <c r="BI12" s="285"/>
-      <c r="BJ12" s="285"/>
-      <c r="BK12" s="286"/>
-      <c r="BP12" s="284"/>
-      <c r="BQ12" s="285"/>
-      <c r="BR12" s="285"/>
-      <c r="BS12" s="285"/>
-      <c r="BT12" s="285"/>
-      <c r="BU12" s="285"/>
-      <c r="BV12" s="285"/>
-      <c r="BW12" s="286"/>
-      <c r="CA12" s="284"/>
-      <c r="CB12" s="285"/>
-      <c r="CC12" s="285"/>
-      <c r="CD12" s="285"/>
-      <c r="CE12" s="285"/>
-      <c r="CF12" s="285"/>
-      <c r="CG12" s="285"/>
-      <c r="CH12" s="286"/>
-      <c r="CL12" s="284"/>
-      <c r="CM12" s="285"/>
-      <c r="CN12" s="285"/>
-      <c r="CO12" s="285"/>
-      <c r="CP12" s="285"/>
-      <c r="CQ12" s="285"/>
-      <c r="CR12" s="285"/>
-      <c r="CS12" s="286"/>
-      <c r="CV12" s="284"/>
-      <c r="CW12" s="285"/>
-      <c r="CX12" s="285"/>
-      <c r="CY12" s="285"/>
-      <c r="CZ12" s="285"/>
-      <c r="DA12" s="285"/>
-      <c r="DB12" s="285"/>
-      <c r="DC12" s="286"/>
+      <c r="BD12" s="264"/>
+      <c r="BE12" s="265"/>
+      <c r="BF12" s="265"/>
+      <c r="BG12" s="265"/>
+      <c r="BH12" s="265"/>
+      <c r="BI12" s="265"/>
+      <c r="BJ12" s="265"/>
+      <c r="BK12" s="266"/>
+      <c r="BP12" s="264"/>
+      <c r="BQ12" s="265"/>
+      <c r="BR12" s="265"/>
+      <c r="BS12" s="265"/>
+      <c r="BT12" s="265"/>
+      <c r="BU12" s="265"/>
+      <c r="BV12" s="265"/>
+      <c r="BW12" s="266"/>
+      <c r="CA12" s="264"/>
+      <c r="CB12" s="265"/>
+      <c r="CC12" s="265"/>
+      <c r="CD12" s="265"/>
+      <c r="CE12" s="265"/>
+      <c r="CF12" s="265"/>
+      <c r="CG12" s="265"/>
+      <c r="CH12" s="266"/>
+      <c r="CL12" s="264"/>
+      <c r="CM12" s="265"/>
+      <c r="CN12" s="265"/>
+      <c r="CO12" s="265"/>
+      <c r="CP12" s="265"/>
+      <c r="CQ12" s="265"/>
+      <c r="CR12" s="265"/>
+      <c r="CS12" s="266"/>
+      <c r="CV12" s="264"/>
+      <c r="CW12" s="265"/>
+      <c r="CX12" s="265"/>
+      <c r="CY12" s="265"/>
+      <c r="CZ12" s="265"/>
+      <c r="DA12" s="265"/>
+      <c r="DB12" s="265"/>
+      <c r="DC12" s="266"/>
     </row>
     <row r="13" spans="1:107" thickBot="1">
       <c r="G13" s="40"/>
@@ -7784,7 +7754,7 @@
       <c r="V13" s="29"/>
       <c r="W13" s="29"/>
       <c r="AX13" s="42"/>
-      <c r="AY13" s="291"/>
+      <c r="AY13" s="259"/>
       <c r="BD13" s="40"/>
       <c r="BG13" s="29"/>
       <c r="BH13" s="29"/>
@@ -7809,16 +7779,16 @@
       <c r="DC13" s="42"/>
     </row>
     <row r="14" spans="1:107" thickBot="1">
-      <c r="G14" s="287" t="s">
+      <c r="G14" s="267" t="s">
         <v>325</v>
       </c>
-      <c r="H14" s="288"/>
-      <c r="I14" s="288"/>
-      <c r="J14" s="288"/>
-      <c r="K14" s="288"/>
-      <c r="L14" s="288"/>
-      <c r="M14" s="288"/>
-      <c r="N14" s="289"/>
+      <c r="H14" s="268"/>
+      <c r="I14" s="268"/>
+      <c r="J14" s="268"/>
+      <c r="K14" s="268"/>
+      <c r="L14" s="268"/>
+      <c r="M14" s="268"/>
+      <c r="N14" s="269"/>
       <c r="O14" s="40"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="29"/>
@@ -7829,57 +7799,57 @@
       <c r="V14" s="29"/>
       <c r="W14" s="29"/>
       <c r="AX14" s="42"/>
-      <c r="AY14" s="291"/>
-      <c r="BD14" s="287" t="s">
+      <c r="AY14" s="259"/>
+      <c r="BD14" s="267" t="s">
         <v>338</v>
       </c>
-      <c r="BE14" s="288"/>
-      <c r="BF14" s="288"/>
-      <c r="BG14" s="288"/>
-      <c r="BH14" s="288"/>
-      <c r="BI14" s="288"/>
-      <c r="BJ14" s="288"/>
-      <c r="BK14" s="289"/>
-      <c r="BP14" s="287" t="s">
+      <c r="BE14" s="268"/>
+      <c r="BF14" s="268"/>
+      <c r="BG14" s="268"/>
+      <c r="BH14" s="268"/>
+      <c r="BI14" s="268"/>
+      <c r="BJ14" s="268"/>
+      <c r="BK14" s="269"/>
+      <c r="BP14" s="267" t="s">
         <v>327</v>
       </c>
-      <c r="BQ14" s="288"/>
-      <c r="BR14" s="288"/>
-      <c r="BS14" s="288"/>
-      <c r="BT14" s="288"/>
-      <c r="BU14" s="288"/>
-      <c r="BV14" s="288"/>
-      <c r="BW14" s="289"/>
-      <c r="CA14" s="287" t="s">
+      <c r="BQ14" s="268"/>
+      <c r="BR14" s="268"/>
+      <c r="BS14" s="268"/>
+      <c r="BT14" s="268"/>
+      <c r="BU14" s="268"/>
+      <c r="BV14" s="268"/>
+      <c r="BW14" s="269"/>
+      <c r="CA14" s="267" t="s">
         <v>326</v>
       </c>
-      <c r="CB14" s="288"/>
-      <c r="CC14" s="288"/>
-      <c r="CD14" s="288"/>
-      <c r="CE14" s="288"/>
-      <c r="CF14" s="288"/>
-      <c r="CG14" s="288"/>
-      <c r="CH14" s="289"/>
-      <c r="CL14" s="287" t="s">
+      <c r="CB14" s="268"/>
+      <c r="CC14" s="268"/>
+      <c r="CD14" s="268"/>
+      <c r="CE14" s="268"/>
+      <c r="CF14" s="268"/>
+      <c r="CG14" s="268"/>
+      <c r="CH14" s="269"/>
+      <c r="CL14" s="267" t="s">
         <v>329</v>
       </c>
-      <c r="CM14" s="288"/>
-      <c r="CN14" s="288"/>
-      <c r="CO14" s="288"/>
-      <c r="CP14" s="288"/>
-      <c r="CQ14" s="288"/>
-      <c r="CR14" s="288"/>
-      <c r="CS14" s="289"/>
-      <c r="CV14" s="287" t="s">
+      <c r="CM14" s="268"/>
+      <c r="CN14" s="268"/>
+      <c r="CO14" s="268"/>
+      <c r="CP14" s="268"/>
+      <c r="CQ14" s="268"/>
+      <c r="CR14" s="268"/>
+      <c r="CS14" s="269"/>
+      <c r="CV14" s="267" t="s">
         <v>328</v>
       </c>
-      <c r="CW14" s="288"/>
-      <c r="CX14" s="288"/>
-      <c r="CY14" s="288"/>
-      <c r="CZ14" s="288"/>
-      <c r="DA14" s="288"/>
-      <c r="DB14" s="288"/>
-      <c r="DC14" s="289"/>
+      <c r="CW14" s="268"/>
+      <c r="CX14" s="268"/>
+      <c r="CY14" s="268"/>
+      <c r="CZ14" s="268"/>
+      <c r="DA14" s="268"/>
+      <c r="DB14" s="268"/>
+      <c r="DC14" s="269"/>
     </row>
     <row r="15" spans="1:107" thickBot="1">
       <c r="G15" s="117"/>
@@ -7900,7 +7870,7 @@
       <c r="V15" s="29"/>
       <c r="W15" s="29"/>
       <c r="AX15" s="42"/>
-      <c r="AY15" s="291"/>
+      <c r="AY15" s="259"/>
       <c r="BD15" s="117"/>
       <c r="BE15" s="116"/>
       <c r="BF15" s="114"/>
@@ -7961,7 +7931,7 @@
       <c r="V16" s="29"/>
       <c r="W16" s="29"/>
       <c r="AX16" s="42"/>
-      <c r="AY16" s="291"/>
+      <c r="AY16" s="259"/>
       <c r="BD16" s="40"/>
       <c r="BE16" s="29"/>
       <c r="BF16" s="29"/>
@@ -8013,16 +7983,16 @@
       <c r="M17" s="29"/>
       <c r="N17" s="29"/>
       <c r="O17" s="40"/>
-      <c r="P17" s="293"/>
+      <c r="P17" s="270"/>
       <c r="Q17" s="246"/>
       <c r="R17" s="246"/>
       <c r="S17" s="29"/>
-      <c r="T17" s="293"/>
+      <c r="T17" s="270"/>
       <c r="U17" s="246"/>
       <c r="V17" s="246"/>
       <c r="W17" s="246"/>
       <c r="AX17" s="42"/>
-      <c r="AY17" s="291"/>
+      <c r="AY17" s="259"/>
       <c r="BD17" s="40"/>
       <c r="BE17" s="29"/>
       <c r="BF17" s="29"/>
@@ -8040,14 +8010,14 @@
       <c r="BV17" s="29"/>
       <c r="BW17" s="46"/>
       <c r="CA17" s="40"/>
-      <c r="CB17" s="255" t="s">
+      <c r="CB17" s="271" t="s">
         <v>349</v>
       </c>
-      <c r="CC17" s="258"/>
-      <c r="CD17" s="258"/>
-      <c r="CE17" s="258"/>
-      <c r="CF17" s="258"/>
-      <c r="CG17" s="259"/>
+      <c r="CC17" s="256"/>
+      <c r="CD17" s="256"/>
+      <c r="CE17" s="256"/>
+      <c r="CF17" s="256"/>
+      <c r="CG17" s="257"/>
       <c r="CH17" s="46"/>
       <c r="CL17" s="40"/>
       <c r="CM17" s="29"/>
@@ -8070,96 +8040,96 @@
       <c r="G18" s="41"/>
       <c r="O18" s="41"/>
       <c r="AX18" s="42"/>
-      <c r="AY18" s="291"/>
+      <c r="AY18" s="259"/>
       <c r="BD18" s="41"/>
-      <c r="BE18" s="269" t="s">
+      <c r="BE18" s="255" t="s">
         <v>335</v>
       </c>
-      <c r="BF18" s="258"/>
-      <c r="BG18" s="258"/>
-      <c r="BH18" s="258"/>
-      <c r="BI18" s="258"/>
-      <c r="BJ18" s="259"/>
+      <c r="BF18" s="256"/>
+      <c r="BG18" s="256"/>
+      <c r="BH18" s="256"/>
+      <c r="BI18" s="256"/>
+      <c r="BJ18" s="257"/>
       <c r="BK18" s="42"/>
       <c r="BP18" s="41"/>
-      <c r="BQ18" s="269" t="s">
+      <c r="BQ18" s="255" t="s">
         <v>331</v>
       </c>
-      <c r="BR18" s="258"/>
-      <c r="BS18" s="258"/>
-      <c r="BT18" s="258"/>
-      <c r="BU18" s="258"/>
-      <c r="BV18" s="259"/>
+      <c r="BR18" s="256"/>
+      <c r="BS18" s="256"/>
+      <c r="BT18" s="256"/>
+      <c r="BU18" s="256"/>
+      <c r="BV18" s="257"/>
       <c r="BW18" s="42"/>
       <c r="CA18" s="41"/>
-      <c r="CB18" s="270" t="s">
+      <c r="CB18" s="272" t="s">
         <v>342</v>
       </c>
-      <c r="CC18" s="271"/>
-      <c r="CD18" s="269"/>
-      <c r="CE18" s="259"/>
-      <c r="CF18" s="270" t="s">
+      <c r="CC18" s="273"/>
+      <c r="CD18" s="255"/>
+      <c r="CE18" s="257"/>
+      <c r="CF18" s="272" t="s">
         <v>341</v>
       </c>
-      <c r="CG18" s="271"/>
+      <c r="CG18" s="273"/>
       <c r="CH18" s="42"/>
       <c r="CL18" s="41"/>
-      <c r="CM18" s="255" t="s">
+      <c r="CM18" s="271" t="s">
         <v>354</v>
       </c>
-      <c r="CN18" s="258"/>
-      <c r="CO18" s="258"/>
-      <c r="CP18" s="258"/>
-      <c r="CQ18" s="258"/>
-      <c r="CR18" s="259"/>
+      <c r="CN18" s="256"/>
+      <c r="CO18" s="256"/>
+      <c r="CP18" s="256"/>
+      <c r="CQ18" s="256"/>
+      <c r="CR18" s="257"/>
       <c r="CS18" s="42"/>
       <c r="CV18" s="41"/>
-      <c r="CW18" s="255" t="s">
+      <c r="CW18" s="271" t="s">
         <v>359</v>
       </c>
-      <c r="CX18" s="258"/>
-      <c r="CY18" s="258"/>
-      <c r="CZ18" s="258"/>
-      <c r="DA18" s="258"/>
-      <c r="DB18" s="259"/>
+      <c r="CX18" s="256"/>
+      <c r="CY18" s="256"/>
+      <c r="CZ18" s="256"/>
+      <c r="DA18" s="256"/>
+      <c r="DB18" s="257"/>
       <c r="DC18" s="42"/>
     </row>
     <row r="19" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G19" s="41"/>
       <c r="O19" s="41"/>
       <c r="AX19" s="42"/>
-      <c r="AY19" s="291"/>
+      <c r="AY19" s="259"/>
       <c r="BD19" s="41"/>
-      <c r="BE19" s="269" t="s">
+      <c r="BE19" s="255" t="s">
         <v>336</v>
       </c>
-      <c r="BF19" s="258"/>
-      <c r="BG19" s="258"/>
-      <c r="BH19" s="258"/>
-      <c r="BI19" s="258"/>
-      <c r="BJ19" s="259"/>
+      <c r="BF19" s="256"/>
+      <c r="BG19" s="256"/>
+      <c r="BH19" s="256"/>
+      <c r="BI19" s="256"/>
+      <c r="BJ19" s="257"/>
       <c r="BK19" s="42"/>
       <c r="BP19" s="41"/>
-      <c r="BQ19" s="269" t="s">
+      <c r="BQ19" s="255" t="s">
         <v>330</v>
       </c>
-      <c r="BR19" s="258"/>
-      <c r="BS19" s="258"/>
-      <c r="BT19" s="258"/>
-      <c r="BU19" s="258"/>
-      <c r="BV19" s="259"/>
+      <c r="BR19" s="256"/>
+      <c r="BS19" s="256"/>
+      <c r="BT19" s="256"/>
+      <c r="BU19" s="256"/>
+      <c r="BV19" s="257"/>
       <c r="BW19" s="42"/>
       <c r="CA19" s="41"/>
       <c r="CH19" s="42"/>
       <c r="CL19" s="41"/>
-      <c r="CM19" s="255" t="s">
+      <c r="CM19" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CN19" s="258"/>
-      <c r="CO19" s="258"/>
-      <c r="CP19" s="258"/>
-      <c r="CQ19" s="258"/>
-      <c r="CR19" s="259"/>
+      <c r="CN19" s="256"/>
+      <c r="CO19" s="256"/>
+      <c r="CP19" s="256"/>
+      <c r="CQ19" s="256"/>
+      <c r="CR19" s="257"/>
       <c r="CS19" s="42"/>
       <c r="CV19" s="41"/>
       <c r="DC19" s="42"/>
@@ -8168,114 +8138,114 @@
       <c r="G20" s="41"/>
       <c r="O20" s="41"/>
       <c r="AX20" s="42"/>
-      <c r="AY20" s="291"/>
+      <c r="AY20" s="259"/>
       <c r="BD20" s="41"/>
       <c r="BK20" s="42"/>
       <c r="BP20" s="41"/>
       <c r="BW20" s="42"/>
       <c r="CA20" s="41"/>
-      <c r="CB20" s="255" t="s">
+      <c r="CB20" s="271" t="s">
         <v>350</v>
       </c>
-      <c r="CC20" s="258"/>
-      <c r="CD20" s="258"/>
-      <c r="CE20" s="258"/>
-      <c r="CF20" s="258"/>
-      <c r="CG20" s="259"/>
+      <c r="CC20" s="256"/>
+      <c r="CD20" s="256"/>
+      <c r="CE20" s="256"/>
+      <c r="CF20" s="256"/>
+      <c r="CG20" s="257"/>
       <c r="CH20" s="42"/>
       <c r="CL20" s="41"/>
       <c r="CS20" s="42"/>
       <c r="CV20" s="41"/>
-      <c r="CW20" s="255" t="s">
+      <c r="CW20" s="271" t="s">
         <v>360</v>
       </c>
-      <c r="CX20" s="258"/>
-      <c r="CY20" s="258"/>
-      <c r="CZ20" s="258"/>
-      <c r="DA20" s="258"/>
-      <c r="DB20" s="259"/>
+      <c r="CX20" s="256"/>
+      <c r="CY20" s="256"/>
+      <c r="CZ20" s="256"/>
+      <c r="DA20" s="256"/>
+      <c r="DB20" s="257"/>
       <c r="DC20" s="42"/>
     </row>
     <row r="21" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G21" s="41"/>
       <c r="O21" s="41"/>
       <c r="AX21" s="42"/>
-      <c r="AY21" s="291"/>
+      <c r="AY21" s="259"/>
       <c r="BD21" s="41"/>
-      <c r="BE21" s="269" t="s">
+      <c r="BE21" s="255" t="s">
         <v>337</v>
       </c>
-      <c r="BF21" s="258"/>
-      <c r="BG21" s="258"/>
-      <c r="BH21" s="258"/>
-      <c r="BI21" s="258"/>
-      <c r="BJ21" s="259"/>
+      <c r="BF21" s="256"/>
+      <c r="BG21" s="256"/>
+      <c r="BH21" s="256"/>
+      <c r="BI21" s="256"/>
+      <c r="BJ21" s="257"/>
       <c r="BK21" s="42"/>
       <c r="BP21" s="41"/>
-      <c r="BQ21" s="269" t="s">
+      <c r="BQ21" s="255" t="s">
         <v>332</v>
       </c>
-      <c r="BR21" s="258"/>
-      <c r="BS21" s="258"/>
-      <c r="BT21" s="258"/>
-      <c r="BU21" s="258"/>
-      <c r="BV21" s="259"/>
+      <c r="BR21" s="256"/>
+      <c r="BS21" s="256"/>
+      <c r="BT21" s="256"/>
+      <c r="BU21" s="256"/>
+      <c r="BV21" s="257"/>
       <c r="BW21" s="42"/>
       <c r="CA21" s="41"/>
-      <c r="CB21" s="255" t="s">
+      <c r="CB21" s="271" t="s">
         <v>336</v>
       </c>
-      <c r="CC21" s="258"/>
-      <c r="CD21" s="258"/>
-      <c r="CE21" s="258"/>
-      <c r="CF21" s="258"/>
-      <c r="CG21" s="259"/>
+      <c r="CC21" s="256"/>
+      <c r="CD21" s="256"/>
+      <c r="CE21" s="256"/>
+      <c r="CF21" s="256"/>
+      <c r="CG21" s="257"/>
       <c r="CH21" s="42"/>
       <c r="CL21" s="41"/>
-      <c r="CM21" s="255" t="s">
+      <c r="CM21" s="271" t="s">
         <v>356</v>
       </c>
-      <c r="CN21" s="258"/>
-      <c r="CO21" s="258"/>
-      <c r="CP21" s="258"/>
-      <c r="CQ21" s="258"/>
-      <c r="CR21" s="259"/>
+      <c r="CN21" s="256"/>
+      <c r="CO21" s="256"/>
+      <c r="CP21" s="256"/>
+      <c r="CQ21" s="256"/>
+      <c r="CR21" s="257"/>
       <c r="CS21" s="42"/>
       <c r="CV21" s="41"/>
-      <c r="CW21" s="255" t="s">
+      <c r="CW21" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CX21" s="258"/>
-      <c r="CY21" s="258"/>
-      <c r="CZ21" s="258"/>
-      <c r="DA21" s="258"/>
-      <c r="DB21" s="259"/>
+      <c r="CX21" s="256"/>
+      <c r="CY21" s="256"/>
+      <c r="CZ21" s="256"/>
+      <c r="DA21" s="256"/>
+      <c r="DB21" s="257"/>
       <c r="DC21" s="42"/>
     </row>
     <row r="22" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G22" s="41"/>
       <c r="O22" s="41"/>
       <c r="AX22" s="42"/>
-      <c r="AY22" s="291"/>
+      <c r="AY22" s="259"/>
       <c r="BD22" s="41"/>
-      <c r="BE22" s="269" t="s">
+      <c r="BE22" s="255" t="s">
         <v>336</v>
       </c>
-      <c r="BF22" s="258"/>
-      <c r="BG22" s="258"/>
-      <c r="BH22" s="258"/>
-      <c r="BI22" s="258"/>
-      <c r="BJ22" s="259"/>
+      <c r="BF22" s="256"/>
+      <c r="BG22" s="256"/>
+      <c r="BH22" s="256"/>
+      <c r="BI22" s="256"/>
+      <c r="BJ22" s="257"/>
       <c r="BK22" s="42"/>
       <c r="BP22" s="41"/>
-      <c r="BQ22" s="269" t="s">
+      <c r="BQ22" s="255" t="s">
         <v>330</v>
       </c>
-      <c r="BR22" s="258"/>
-      <c r="BS22" s="258"/>
-      <c r="BT22" s="258"/>
-      <c r="BU22" s="258"/>
-      <c r="BV22" s="259"/>
+      <c r="BR22" s="256"/>
+      <c r="BS22" s="256"/>
+      <c r="BT22" s="256"/>
+      <c r="BU22" s="256"/>
+      <c r="BV22" s="257"/>
       <c r="BW22" s="42"/>
       <c r="CA22" s="41"/>
       <c r="CH22" s="42"/>
@@ -8288,7 +8258,7 @@
       <c r="G23" s="41"/>
       <c r="O23" s="41"/>
       <c r="AX23" s="42"/>
-      <c r="AY23" s="291"/>
+      <c r="AY23" s="259"/>
       <c r="BD23" s="41"/>
       <c r="BK23" s="42"/>
       <c r="BP23" s="41"/>
@@ -8297,57 +8267,57 @@
       <c r="CB23" s="29"/>
       <c r="CC23" s="29"/>
       <c r="CD23" s="29"/>
-      <c r="CE23" s="278" t="s">
+      <c r="CE23" s="282" t="s">
         <v>348</v>
       </c>
-      <c r="CF23" s="279"/>
-      <c r="CG23" s="279"/>
-      <c r="CH23" s="280"/>
+      <c r="CF23" s="283"/>
+      <c r="CG23" s="283"/>
+      <c r="CH23" s="284"/>
       <c r="CL23" s="41"/>
-      <c r="CM23" s="255" t="s">
+      <c r="CM23" s="271" t="s">
         <v>357</v>
       </c>
-      <c r="CN23" s="258"/>
-      <c r="CO23" s="258"/>
-      <c r="CP23" s="258"/>
-      <c r="CQ23" s="258"/>
-      <c r="CR23" s="259"/>
+      <c r="CN23" s="256"/>
+      <c r="CO23" s="256"/>
+      <c r="CP23" s="256"/>
+      <c r="CQ23" s="256"/>
+      <c r="CR23" s="257"/>
       <c r="CS23" s="42"/>
       <c r="CV23" s="41"/>
-      <c r="CW23" s="255" t="s">
+      <c r="CW23" s="271" t="s">
         <v>361</v>
       </c>
-      <c r="CX23" s="258"/>
-      <c r="CY23" s="258"/>
-      <c r="CZ23" s="258"/>
-      <c r="DA23" s="258"/>
-      <c r="DB23" s="259"/>
+      <c r="CX23" s="256"/>
+      <c r="CY23" s="256"/>
+      <c r="CZ23" s="256"/>
+      <c r="DA23" s="256"/>
+      <c r="DB23" s="257"/>
       <c r="DC23" s="42"/>
     </row>
     <row r="24" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G24" s="41"/>
       <c r="O24" s="41"/>
       <c r="AX24" s="42"/>
-      <c r="AY24" s="291"/>
+      <c r="AY24" s="259"/>
       <c r="BD24" s="41"/>
-      <c r="BE24" s="269" t="s">
+      <c r="BE24" s="255" t="s">
         <v>339</v>
       </c>
-      <c r="BF24" s="258"/>
-      <c r="BG24" s="258"/>
-      <c r="BH24" s="258"/>
-      <c r="BI24" s="258"/>
-      <c r="BJ24" s="259"/>
+      <c r="BF24" s="256"/>
+      <c r="BG24" s="256"/>
+      <c r="BH24" s="256"/>
+      <c r="BI24" s="256"/>
+      <c r="BJ24" s="257"/>
       <c r="BK24" s="42"/>
       <c r="BP24" s="41"/>
-      <c r="BQ24" s="269" t="s">
+      <c r="BQ24" s="255" t="s">
         <v>333</v>
       </c>
-      <c r="BR24" s="258"/>
-      <c r="BS24" s="258"/>
-      <c r="BT24" s="258"/>
-      <c r="BU24" s="258"/>
-      <c r="BV24" s="259"/>
+      <c r="BR24" s="256"/>
+      <c r="BS24" s="256"/>
+      <c r="BT24" s="256"/>
+      <c r="BU24" s="256"/>
+      <c r="BV24" s="257"/>
       <c r="BW24" s="42"/>
       <c r="CA24" s="40"/>
       <c r="CB24" s="29"/>
@@ -8358,60 +8328,60 @@
       <c r="CG24" s="29"/>
       <c r="CH24" s="46"/>
       <c r="CL24" s="41"/>
-      <c r="CM24" s="255" t="s">
+      <c r="CM24" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CN24" s="258"/>
-      <c r="CO24" s="258"/>
-      <c r="CP24" s="258"/>
-      <c r="CQ24" s="258"/>
-      <c r="CR24" s="259"/>
+      <c r="CN24" s="256"/>
+      <c r="CO24" s="256"/>
+      <c r="CP24" s="256"/>
+      <c r="CQ24" s="256"/>
+      <c r="CR24" s="257"/>
       <c r="CS24" s="42"/>
       <c r="CV24" s="41"/>
-      <c r="CW24" s="255" t="s">
+      <c r="CW24" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CX24" s="258"/>
-      <c r="CY24" s="258"/>
-      <c r="CZ24" s="258"/>
-      <c r="DA24" s="258"/>
-      <c r="DB24" s="259"/>
+      <c r="CX24" s="256"/>
+      <c r="CY24" s="256"/>
+      <c r="CZ24" s="256"/>
+      <c r="DA24" s="256"/>
+      <c r="DB24" s="257"/>
       <c r="DC24" s="42"/>
     </row>
     <row r="25" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G25" s="41"/>
       <c r="O25" s="41"/>
       <c r="AX25" s="42"/>
-      <c r="AY25" s="291"/>
+      <c r="AY25" s="259"/>
       <c r="BD25" s="41"/>
-      <c r="BE25" s="269" t="s">
+      <c r="BE25" s="255" t="s">
         <v>336</v>
       </c>
-      <c r="BF25" s="258"/>
-      <c r="BG25" s="258"/>
-      <c r="BH25" s="258"/>
-      <c r="BI25" s="258"/>
-      <c r="BJ25" s="259"/>
+      <c r="BF25" s="256"/>
+      <c r="BG25" s="256"/>
+      <c r="BH25" s="256"/>
+      <c r="BI25" s="256"/>
+      <c r="BJ25" s="257"/>
       <c r="BK25" s="42"/>
       <c r="BP25" s="41"/>
-      <c r="BQ25" s="269" t="s">
+      <c r="BQ25" s="255" t="s">
         <v>330</v>
       </c>
-      <c r="BR25" s="258"/>
-      <c r="BS25" s="258"/>
-      <c r="BT25" s="258"/>
-      <c r="BU25" s="258"/>
-      <c r="BV25" s="259"/>
+      <c r="BR25" s="256"/>
+      <c r="BS25" s="256"/>
+      <c r="BT25" s="256"/>
+      <c r="BU25" s="256"/>
+      <c r="BV25" s="257"/>
       <c r="BW25" s="42"/>
       <c r="CA25" s="41"/>
-      <c r="CB25" s="255" t="s">
+      <c r="CB25" s="271" t="s">
         <v>343</v>
       </c>
-      <c r="CC25" s="256"/>
-      <c r="CD25" s="256"/>
-      <c r="CE25" s="256"/>
-      <c r="CF25" s="256"/>
-      <c r="CG25" s="257"/>
+      <c r="CC25" s="280"/>
+      <c r="CD25" s="280"/>
+      <c r="CE25" s="280"/>
+      <c r="CF25" s="280"/>
+      <c r="CG25" s="281"/>
       <c r="CH25" s="42"/>
       <c r="CL25" s="41"/>
       <c r="CS25" s="42"/>
@@ -8422,128 +8392,128 @@
       <c r="G26" s="41"/>
       <c r="O26" s="41"/>
       <c r="AX26" s="42"/>
-      <c r="AY26" s="291"/>
+      <c r="AY26" s="259"/>
       <c r="BD26" s="41"/>
       <c r="BK26" s="42"/>
       <c r="BP26" s="41"/>
       <c r="BW26" s="42"/>
       <c r="CA26" s="41"/>
-      <c r="CB26" s="270" t="s">
+      <c r="CB26" s="272" t="s">
         <v>342</v>
       </c>
-      <c r="CC26" s="271"/>
-      <c r="CD26" s="269"/>
-      <c r="CE26" s="259"/>
-      <c r="CF26" s="270" t="s">
+      <c r="CC26" s="273"/>
+      <c r="CD26" s="255"/>
+      <c r="CE26" s="257"/>
+      <c r="CF26" s="272" t="s">
         <v>341</v>
       </c>
-      <c r="CG26" s="271"/>
+      <c r="CG26" s="273"/>
       <c r="CH26" s="42"/>
       <c r="CL26" s="41"/>
-      <c r="CM26" s="269" t="s">
+      <c r="CM26" s="255" t="s">
         <v>331</v>
       </c>
-      <c r="CN26" s="258"/>
-      <c r="CO26" s="258"/>
-      <c r="CP26" s="258"/>
-      <c r="CQ26" s="258"/>
-      <c r="CR26" s="259"/>
+      <c r="CN26" s="256"/>
+      <c r="CO26" s="256"/>
+      <c r="CP26" s="256"/>
+      <c r="CQ26" s="256"/>
+      <c r="CR26" s="257"/>
       <c r="CS26" s="42"/>
       <c r="CV26" s="41"/>
-      <c r="CW26" s="255" t="s">
+      <c r="CW26" s="271" t="s">
         <v>362</v>
       </c>
-      <c r="CX26" s="258"/>
-      <c r="CY26" s="258"/>
-      <c r="CZ26" s="258"/>
-      <c r="DA26" s="258"/>
-      <c r="DB26" s="259"/>
+      <c r="CX26" s="256"/>
+      <c r="CY26" s="256"/>
+      <c r="CZ26" s="256"/>
+      <c r="DA26" s="256"/>
+      <c r="DB26" s="257"/>
       <c r="DC26" s="42"/>
     </row>
     <row r="27" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G27" s="41"/>
       <c r="O27" s="41"/>
       <c r="AX27" s="42"/>
-      <c r="AY27" s="291"/>
+      <c r="AY27" s="259"/>
       <c r="BD27" s="41"/>
-      <c r="BE27" s="269" t="s">
+      <c r="BE27" s="255" t="s">
         <v>340</v>
       </c>
-      <c r="BF27" s="258"/>
-      <c r="BG27" s="258"/>
-      <c r="BH27" s="258"/>
-      <c r="BI27" s="258"/>
-      <c r="BJ27" s="259"/>
+      <c r="BF27" s="256"/>
+      <c r="BG27" s="256"/>
+      <c r="BH27" s="256"/>
+      <c r="BI27" s="256"/>
+      <c r="BJ27" s="257"/>
       <c r="BK27" s="42"/>
       <c r="BP27" s="41"/>
-      <c r="BQ27" s="269" t="s">
+      <c r="BQ27" s="255" t="s">
         <v>334</v>
       </c>
-      <c r="BR27" s="258"/>
-      <c r="BS27" s="258"/>
-      <c r="BT27" s="258"/>
-      <c r="BU27" s="258"/>
-      <c r="BV27" s="259"/>
+      <c r="BR27" s="256"/>
+      <c r="BS27" s="256"/>
+      <c r="BT27" s="256"/>
+      <c r="BU27" s="256"/>
+      <c r="BV27" s="257"/>
       <c r="BW27" s="42"/>
       <c r="CA27" s="41"/>
       <c r="CH27" s="42"/>
       <c r="CL27" s="41"/>
-      <c r="CM27" s="255" t="s">
+      <c r="CM27" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CN27" s="258"/>
-      <c r="CO27" s="258"/>
-      <c r="CP27" s="258"/>
-      <c r="CQ27" s="258"/>
-      <c r="CR27" s="259"/>
+      <c r="CN27" s="256"/>
+      <c r="CO27" s="256"/>
+      <c r="CP27" s="256"/>
+      <c r="CQ27" s="256"/>
+      <c r="CR27" s="257"/>
       <c r="CS27" s="42"/>
       <c r="CV27" s="41"/>
-      <c r="CW27" s="255" t="s">
+      <c r="CW27" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CX27" s="258"/>
-      <c r="CY27" s="258"/>
-      <c r="CZ27" s="258"/>
-      <c r="DA27" s="258"/>
-      <c r="DB27" s="259"/>
+      <c r="CX27" s="256"/>
+      <c r="CY27" s="256"/>
+      <c r="CZ27" s="256"/>
+      <c r="DA27" s="256"/>
+      <c r="DB27" s="257"/>
       <c r="DC27" s="42"/>
     </row>
     <row r="28" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G28" s="41"/>
       <c r="O28" s="41"/>
       <c r="AX28" s="42"/>
-      <c r="AY28" s="291"/>
+      <c r="AY28" s="259"/>
       <c r="BD28" s="119"/>
-      <c r="BE28" s="270" t="s">
+      <c r="BE28" s="272" t="s">
         <v>342</v>
       </c>
-      <c r="BF28" s="271"/>
-      <c r="BG28" s="269"/>
-      <c r="BH28" s="259"/>
-      <c r="BI28" s="270" t="s">
+      <c r="BF28" s="273"/>
+      <c r="BG28" s="255"/>
+      <c r="BH28" s="257"/>
+      <c r="BI28" s="272" t="s">
         <v>341</v>
       </c>
-      <c r="BJ28" s="271"/>
+      <c r="BJ28" s="273"/>
       <c r="BK28" s="42"/>
       <c r="BP28" s="41"/>
-      <c r="BQ28" s="269" t="s">
+      <c r="BQ28" s="255" t="s">
         <v>330</v>
       </c>
-      <c r="BR28" s="258"/>
-      <c r="BS28" s="258"/>
-      <c r="BT28" s="258"/>
-      <c r="BU28" s="258"/>
-      <c r="BV28" s="259"/>
+      <c r="BR28" s="256"/>
+      <c r="BS28" s="256"/>
+      <c r="BT28" s="256"/>
+      <c r="BU28" s="256"/>
+      <c r="BV28" s="257"/>
       <c r="BW28" s="42"/>
       <c r="CA28" s="41"/>
-      <c r="CB28" s="255" t="s">
+      <c r="CB28" s="271" t="s">
         <v>344</v>
       </c>
-      <c r="CC28" s="256"/>
-      <c r="CD28" s="256"/>
-      <c r="CE28" s="256"/>
-      <c r="CF28" s="256"/>
-      <c r="CG28" s="257"/>
+      <c r="CC28" s="280"/>
+      <c r="CD28" s="280"/>
+      <c r="CE28" s="280"/>
+      <c r="CF28" s="280"/>
+      <c r="CG28" s="281"/>
       <c r="CH28" s="42"/>
       <c r="CL28" s="41"/>
       <c r="CS28" s="42"/>
@@ -8554,49 +8524,49 @@
       <c r="G29" s="41"/>
       <c r="O29" s="41"/>
       <c r="AX29" s="42"/>
-      <c r="AY29" s="291"/>
+      <c r="AY29" s="259"/>
       <c r="BD29" s="41"/>
       <c r="BK29" s="42"/>
       <c r="BP29" s="41"/>
       <c r="BW29" s="42"/>
       <c r="CA29" s="41"/>
-      <c r="CB29" s="270" t="s">
+      <c r="CB29" s="272" t="s">
         <v>342</v>
       </c>
-      <c r="CC29" s="271"/>
-      <c r="CD29" s="269"/>
-      <c r="CE29" s="259"/>
-      <c r="CF29" s="270" t="s">
+      <c r="CC29" s="273"/>
+      <c r="CD29" s="255"/>
+      <c r="CE29" s="257"/>
+      <c r="CF29" s="272" t="s">
         <v>341</v>
       </c>
-      <c r="CG29" s="271"/>
+      <c r="CG29" s="273"/>
       <c r="CH29" s="42"/>
       <c r="CL29" s="41"/>
-      <c r="CM29" s="269" t="s">
+      <c r="CM29" s="255" t="s">
         <v>332</v>
       </c>
-      <c r="CN29" s="258"/>
-      <c r="CO29" s="258"/>
-      <c r="CP29" s="258"/>
-      <c r="CQ29" s="258"/>
-      <c r="CR29" s="259"/>
+      <c r="CN29" s="256"/>
+      <c r="CO29" s="256"/>
+      <c r="CP29" s="256"/>
+      <c r="CQ29" s="256"/>
+      <c r="CR29" s="257"/>
       <c r="CS29" s="42"/>
       <c r="CV29" s="41"/>
-      <c r="CW29" s="255" t="s">
+      <c r="CW29" s="271" t="s">
         <v>363</v>
       </c>
-      <c r="CX29" s="258"/>
-      <c r="CY29" s="258"/>
-      <c r="CZ29" s="258"/>
-      <c r="DA29" s="258"/>
-      <c r="DB29" s="259"/>
+      <c r="CX29" s="256"/>
+      <c r="CY29" s="256"/>
+      <c r="CZ29" s="256"/>
+      <c r="DA29" s="256"/>
+      <c r="DB29" s="257"/>
       <c r="DC29" s="42"/>
     </row>
     <row r="30" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G30" s="41"/>
       <c r="O30" s="41"/>
       <c r="AX30" s="42"/>
-      <c r="AY30" s="291"/>
+      <c r="AY30" s="259"/>
       <c r="BD30" s="41"/>
       <c r="BK30" s="42"/>
       <c r="BP30" s="41"/>
@@ -8604,44 +8574,44 @@
       <c r="CA30" s="41"/>
       <c r="CH30" s="42"/>
       <c r="CL30" s="41"/>
-      <c r="CM30" s="255" t="s">
+      <c r="CM30" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CN30" s="258"/>
-      <c r="CO30" s="258"/>
-      <c r="CP30" s="258"/>
-      <c r="CQ30" s="258"/>
-      <c r="CR30" s="259"/>
+      <c r="CN30" s="256"/>
+      <c r="CO30" s="256"/>
+      <c r="CP30" s="256"/>
+      <c r="CQ30" s="256"/>
+      <c r="CR30" s="257"/>
       <c r="CS30" s="42"/>
       <c r="CV30" s="41"/>
-      <c r="CW30" s="255" t="s">
+      <c r="CW30" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CX30" s="256"/>
-      <c r="CY30" s="256"/>
-      <c r="CZ30" s="256"/>
-      <c r="DA30" s="256"/>
-      <c r="DB30" s="257"/>
+      <c r="CX30" s="280"/>
+      <c r="CY30" s="280"/>
+      <c r="CZ30" s="280"/>
+      <c r="DA30" s="280"/>
+      <c r="DB30" s="281"/>
       <c r="DC30" s="42"/>
     </row>
     <row r="31" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G31" s="41"/>
       <c r="O31" s="41"/>
       <c r="AX31" s="42"/>
-      <c r="AY31" s="291"/>
+      <c r="AY31" s="259"/>
       <c r="BD31" s="41"/>
       <c r="BK31" s="42"/>
       <c r="BP31" s="41"/>
       <c r="BW31" s="42"/>
       <c r="CA31" s="41"/>
-      <c r="CB31" s="255" t="s">
+      <c r="CB31" s="271" t="s">
         <v>345</v>
       </c>
-      <c r="CC31" s="256"/>
-      <c r="CD31" s="256"/>
-      <c r="CE31" s="256"/>
-      <c r="CF31" s="256"/>
-      <c r="CG31" s="257"/>
+      <c r="CC31" s="280"/>
+      <c r="CD31" s="280"/>
+      <c r="CE31" s="280"/>
+      <c r="CF31" s="280"/>
+      <c r="CG31" s="281"/>
       <c r="CH31" s="42"/>
       <c r="CL31" s="41"/>
       <c r="CS31" s="42"/>
@@ -8652,122 +8622,122 @@
       <c r="G32" s="41"/>
       <c r="O32" s="41"/>
       <c r="AX32" s="42"/>
-      <c r="AY32" s="291"/>
+      <c r="AY32" s="259"/>
       <c r="BD32" s="41"/>
-      <c r="BE32" s="272" t="s">
+      <c r="BE32" s="274" t="s">
         <v>277</v>
       </c>
-      <c r="BF32" s="273"/>
-      <c r="BG32" s="273"/>
-      <c r="BH32" s="273"/>
-      <c r="BI32" s="273"/>
-      <c r="BJ32" s="274"/>
+      <c r="BF32" s="275"/>
+      <c r="BG32" s="275"/>
+      <c r="BH32" s="275"/>
+      <c r="BI32" s="275"/>
+      <c r="BJ32" s="276"/>
       <c r="BK32" s="42"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="272" t="s">
+      <c r="BQ32" s="274" t="s">
         <v>352</v>
       </c>
-      <c r="BR32" s="273"/>
-      <c r="BS32" s="273"/>
-      <c r="BT32" s="273"/>
-      <c r="BU32" s="273"/>
-      <c r="BV32" s="274"/>
+      <c r="BR32" s="275"/>
+      <c r="BS32" s="275"/>
+      <c r="BT32" s="275"/>
+      <c r="BU32" s="275"/>
+      <c r="BV32" s="276"/>
       <c r="BW32" s="42"/>
       <c r="CA32" s="41"/>
-      <c r="CB32" s="270" t="s">
+      <c r="CB32" s="272" t="s">
         <v>342</v>
       </c>
-      <c r="CC32" s="271"/>
-      <c r="CD32" s="269"/>
-      <c r="CE32" s="259"/>
-      <c r="CF32" s="270" t="s">
+      <c r="CC32" s="273"/>
+      <c r="CD32" s="255"/>
+      <c r="CE32" s="257"/>
+      <c r="CF32" s="272" t="s">
         <v>341</v>
       </c>
-      <c r="CG32" s="271"/>
+      <c r="CG32" s="273"/>
       <c r="CH32" s="42"/>
       <c r="CL32" s="41"/>
-      <c r="CM32" s="269" t="s">
+      <c r="CM32" s="255" t="s">
         <v>333</v>
       </c>
-      <c r="CN32" s="258"/>
-      <c r="CO32" s="258"/>
-      <c r="CP32" s="258"/>
-      <c r="CQ32" s="258"/>
-      <c r="CR32" s="259"/>
+      <c r="CN32" s="256"/>
+      <c r="CO32" s="256"/>
+      <c r="CP32" s="256"/>
+      <c r="CQ32" s="256"/>
+      <c r="CR32" s="257"/>
       <c r="CS32" s="42"/>
       <c r="CV32" s="41"/>
-      <c r="CW32" s="255" t="s">
+      <c r="CW32" s="271" t="s">
         <v>364</v>
       </c>
-      <c r="CX32" s="258"/>
-      <c r="CY32" s="258"/>
-      <c r="CZ32" s="258"/>
-      <c r="DA32" s="258"/>
-      <c r="DB32" s="259"/>
+      <c r="CX32" s="256"/>
+      <c r="CY32" s="256"/>
+      <c r="CZ32" s="256"/>
+      <c r="DA32" s="256"/>
+      <c r="DB32" s="257"/>
       <c r="DC32" s="42"/>
     </row>
     <row r="33" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G33" s="41"/>
       <c r="O33" s="41"/>
       <c r="AX33" s="42"/>
-      <c r="AY33" s="291"/>
+      <c r="AY33" s="259"/>
       <c r="BD33" s="41"/>
-      <c r="BE33" s="275"/>
-      <c r="BF33" s="276"/>
-      <c r="BG33" s="276"/>
-      <c r="BH33" s="276"/>
-      <c r="BI33" s="276"/>
-      <c r="BJ33" s="277"/>
+      <c r="BE33" s="277"/>
+      <c r="BF33" s="278"/>
+      <c r="BG33" s="278"/>
+      <c r="BH33" s="278"/>
+      <c r="BI33" s="278"/>
+      <c r="BJ33" s="279"/>
       <c r="BK33" s="42"/>
       <c r="BP33" s="41"/>
-      <c r="BQ33" s="275"/>
-      <c r="BR33" s="276"/>
-      <c r="BS33" s="276"/>
-      <c r="BT33" s="276"/>
-      <c r="BU33" s="276"/>
-      <c r="BV33" s="277"/>
+      <c r="BQ33" s="277"/>
+      <c r="BR33" s="278"/>
+      <c r="BS33" s="278"/>
+      <c r="BT33" s="278"/>
+      <c r="BU33" s="278"/>
+      <c r="BV33" s="279"/>
       <c r="BW33" s="42"/>
       <c r="CA33" s="41"/>
       <c r="CH33" s="42"/>
       <c r="CL33" s="41"/>
-      <c r="CM33" s="255" t="s">
+      <c r="CM33" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CN33" s="256"/>
-      <c r="CO33" s="256"/>
-      <c r="CP33" s="256"/>
-      <c r="CQ33" s="256"/>
-      <c r="CR33" s="257"/>
+      <c r="CN33" s="280"/>
+      <c r="CO33" s="280"/>
+      <c r="CP33" s="280"/>
+      <c r="CQ33" s="280"/>
+      <c r="CR33" s="281"/>
       <c r="CS33" s="42"/>
       <c r="CV33" s="41"/>
-      <c r="CW33" s="255" t="s">
+      <c r="CW33" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CX33" s="256"/>
-      <c r="CY33" s="256"/>
-      <c r="CZ33" s="256"/>
-      <c r="DA33" s="256"/>
-      <c r="DB33" s="257"/>
+      <c r="CX33" s="280"/>
+      <c r="CY33" s="280"/>
+      <c r="CZ33" s="280"/>
+      <c r="DA33" s="280"/>
+      <c r="DB33" s="281"/>
       <c r="DC33" s="42"/>
     </row>
     <row r="34" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G34" s="41"/>
       <c r="O34" s="41"/>
       <c r="AX34" s="42"/>
-      <c r="AY34" s="291"/>
+      <c r="AY34" s="259"/>
       <c r="BD34" s="41"/>
       <c r="BK34" s="42"/>
       <c r="BP34" s="41"/>
       <c r="BW34" s="42"/>
       <c r="CA34" s="41"/>
-      <c r="CB34" s="255" t="s">
+      <c r="CB34" s="271" t="s">
         <v>346</v>
       </c>
-      <c r="CC34" s="256"/>
-      <c r="CD34" s="256"/>
-      <c r="CE34" s="256"/>
-      <c r="CF34" s="256"/>
-      <c r="CG34" s="257"/>
+      <c r="CC34" s="280"/>
+      <c r="CD34" s="280"/>
+      <c r="CE34" s="280"/>
+      <c r="CF34" s="280"/>
+      <c r="CG34" s="281"/>
       <c r="CH34" s="42"/>
       <c r="CL34" s="41"/>
       <c r="CS34" s="42"/>
@@ -8778,95 +8748,95 @@
       <c r="G35" s="41"/>
       <c r="O35" s="41"/>
       <c r="AX35" s="42"/>
-      <c r="AY35" s="291"/>
+      <c r="AY35" s="259"/>
       <c r="BD35" s="41"/>
       <c r="BK35" s="42"/>
       <c r="BP35" s="41"/>
-      <c r="BQ35" s="255" t="s">
+      <c r="BQ35" s="271" t="s">
         <v>351</v>
       </c>
-      <c r="BR35" s="258"/>
-      <c r="BS35" s="258"/>
-      <c r="BT35" s="258"/>
-      <c r="BU35" s="258"/>
-      <c r="BV35" s="259"/>
+      <c r="BR35" s="256"/>
+      <c r="BS35" s="256"/>
+      <c r="BT35" s="256"/>
+      <c r="BU35" s="256"/>
+      <c r="BV35" s="257"/>
       <c r="BW35" s="42"/>
       <c r="CA35" s="41"/>
-      <c r="CB35" s="270" t="s">
+      <c r="CB35" s="272" t="s">
         <v>342</v>
       </c>
-      <c r="CC35" s="271"/>
-      <c r="CD35" s="269"/>
-      <c r="CE35" s="259"/>
-      <c r="CF35" s="270" t="s">
+      <c r="CC35" s="273"/>
+      <c r="CD35" s="255"/>
+      <c r="CE35" s="257"/>
+      <c r="CF35" s="272" t="s">
         <v>341</v>
       </c>
-      <c r="CG35" s="271"/>
+      <c r="CG35" s="273"/>
       <c r="CH35" s="42"/>
       <c r="CL35" s="41"/>
-      <c r="CM35" s="255" t="s">
+      <c r="CM35" s="271" t="s">
         <v>358</v>
       </c>
-      <c r="CN35" s="258"/>
-      <c r="CO35" s="258"/>
-      <c r="CP35" s="258"/>
-      <c r="CQ35" s="258"/>
-      <c r="CR35" s="259"/>
+      <c r="CN35" s="256"/>
+      <c r="CO35" s="256"/>
+      <c r="CP35" s="256"/>
+      <c r="CQ35" s="256"/>
+      <c r="CR35" s="257"/>
       <c r="CS35" s="42"/>
       <c r="CV35" s="41"/>
-      <c r="CW35" s="255" t="s">
+      <c r="CW35" s="271" t="s">
         <v>365</v>
       </c>
-      <c r="CX35" s="258"/>
-      <c r="CY35" s="258"/>
-      <c r="CZ35" s="258"/>
-      <c r="DA35" s="258"/>
-      <c r="DB35" s="259"/>
+      <c r="CX35" s="256"/>
+      <c r="CY35" s="256"/>
+      <c r="CZ35" s="256"/>
+      <c r="DA35" s="256"/>
+      <c r="DB35" s="257"/>
       <c r="DC35" s="42"/>
     </row>
     <row r="36" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G36" s="41"/>
       <c r="O36" s="41"/>
       <c r="AX36" s="42"/>
-      <c r="AY36" s="291"/>
+      <c r="AY36" s="259"/>
       <c r="BD36" s="41"/>
       <c r="BK36" s="42"/>
       <c r="BP36" s="41"/>
-      <c r="BQ36" s="255" t="s">
+      <c r="BQ36" s="271" t="s">
         <v>353</v>
       </c>
-      <c r="BR36" s="258"/>
-      <c r="BS36" s="258"/>
-      <c r="BT36" s="258"/>
-      <c r="BU36" s="258"/>
-      <c r="BV36" s="259"/>
+      <c r="BR36" s="256"/>
+      <c r="BS36" s="256"/>
+      <c r="BT36" s="256"/>
+      <c r="BU36" s="256"/>
+      <c r="BV36" s="257"/>
       <c r="BW36" s="42"/>
       <c r="CA36" s="41"/>
       <c r="CH36" s="42"/>
       <c r="CL36" s="41"/>
-      <c r="CM36" s="255" t="s">
+      <c r="CM36" s="271" t="s">
         <v>355</v>
       </c>
-      <c r="CN36" s="256"/>
-      <c r="CO36" s="256"/>
-      <c r="CP36" s="256"/>
-      <c r="CQ36" s="256"/>
-      <c r="CR36" s="257"/>
+      <c r="CN36" s="280"/>
+      <c r="CO36" s="280"/>
+      <c r="CP36" s="280"/>
+      <c r="CQ36" s="280"/>
+      <c r="CR36" s="281"/>
       <c r="CS36" s="42"/>
       <c r="CV36" s="41"/>
-      <c r="CW36" s="260"/>
-      <c r="CX36" s="261"/>
-      <c r="CY36" s="261"/>
-      <c r="CZ36" s="261"/>
-      <c r="DA36" s="261"/>
-      <c r="DB36" s="262"/>
+      <c r="CW36" s="285"/>
+      <c r="CX36" s="286"/>
+      <c r="CY36" s="286"/>
+      <c r="CZ36" s="286"/>
+      <c r="DA36" s="286"/>
+      <c r="DB36" s="287"/>
       <c r="DC36" s="42"/>
     </row>
     <row r="37" spans="7:107" ht="15.75" customHeight="1">
       <c r="G37" s="41"/>
       <c r="O37" s="41"/>
       <c r="AX37" s="42"/>
-      <c r="AY37" s="291"/>
+      <c r="AY37" s="259"/>
       <c r="BD37" s="41"/>
       <c r="BK37" s="42"/>
       <c r="BP37" s="41"/>
@@ -8876,19 +8846,19 @@
       <c r="CL37" s="41"/>
       <c r="CS37" s="42"/>
       <c r="CV37" s="41"/>
-      <c r="CW37" s="263"/>
-      <c r="CX37" s="264"/>
-      <c r="CY37" s="264"/>
-      <c r="CZ37" s="264"/>
-      <c r="DA37" s="264"/>
-      <c r="DB37" s="265"/>
+      <c r="CW37" s="288"/>
+      <c r="CX37" s="289"/>
+      <c r="CY37" s="289"/>
+      <c r="CZ37" s="289"/>
+      <c r="DA37" s="289"/>
+      <c r="DB37" s="290"/>
       <c r="DC37" s="42"/>
     </row>
     <row r="38" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G38" s="41"/>
       <c r="O38" s="41"/>
       <c r="AX38" s="42"/>
-      <c r="AY38" s="291"/>
+      <c r="AY38" s="259"/>
       <c r="BD38" s="41"/>
       <c r="BK38" s="42"/>
       <c r="BP38" s="41"/>
@@ -8898,70 +8868,70 @@
       <c r="CL38" s="41"/>
       <c r="CS38" s="42"/>
       <c r="CV38" s="41"/>
-      <c r="CW38" s="263"/>
-      <c r="CX38" s="264"/>
-      <c r="CY38" s="264"/>
-      <c r="CZ38" s="264"/>
-      <c r="DA38" s="264"/>
-      <c r="DB38" s="265"/>
+      <c r="CW38" s="288"/>
+      <c r="CX38" s="289"/>
+      <c r="CY38" s="289"/>
+      <c r="CZ38" s="289"/>
+      <c r="DA38" s="289"/>
+      <c r="DB38" s="290"/>
       <c r="DC38" s="42"/>
     </row>
     <row r="39" spans="7:107" ht="15.75" customHeight="1">
       <c r="G39" s="41"/>
       <c r="O39" s="41"/>
       <c r="AX39" s="42"/>
-      <c r="AY39" s="291"/>
+      <c r="AY39" s="259"/>
       <c r="BD39" s="41"/>
       <c r="BK39" s="42"/>
       <c r="BP39" s="41"/>
       <c r="BW39" s="42"/>
       <c r="CA39" s="41"/>
-      <c r="CB39" s="272" t="s">
+      <c r="CB39" s="274" t="s">
         <v>347</v>
       </c>
-      <c r="CC39" s="273"/>
-      <c r="CD39" s="273"/>
-      <c r="CE39" s="273"/>
-      <c r="CF39" s="273"/>
-      <c r="CG39" s="274"/>
+      <c r="CC39" s="275"/>
+      <c r="CD39" s="275"/>
+      <c r="CE39" s="275"/>
+      <c r="CF39" s="275"/>
+      <c r="CG39" s="276"/>
       <c r="CH39" s="42"/>
       <c r="CL39" s="41"/>
       <c r="CS39" s="42"/>
       <c r="CV39" s="41"/>
-      <c r="CW39" s="263"/>
-      <c r="CX39" s="264"/>
-      <c r="CY39" s="264"/>
-      <c r="CZ39" s="264"/>
-      <c r="DA39" s="264"/>
-      <c r="DB39" s="265"/>
+      <c r="CW39" s="288"/>
+      <c r="CX39" s="289"/>
+      <c r="CY39" s="289"/>
+      <c r="CZ39" s="289"/>
+      <c r="DA39" s="289"/>
+      <c r="DB39" s="290"/>
       <c r="DC39" s="42"/>
     </row>
     <row r="40" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G40" s="41"/>
       <c r="O40" s="41"/>
       <c r="AX40" s="42"/>
-      <c r="AY40" s="292"/>
+      <c r="AY40" s="260"/>
       <c r="BD40" s="41"/>
       <c r="BK40" s="42"/>
       <c r="BP40" s="41"/>
       <c r="BW40" s="42"/>
       <c r="CA40" s="41"/>
-      <c r="CB40" s="275"/>
-      <c r="CC40" s="276"/>
-      <c r="CD40" s="276"/>
-      <c r="CE40" s="276"/>
-      <c r="CF40" s="276"/>
-      <c r="CG40" s="277"/>
+      <c r="CB40" s="277"/>
+      <c r="CC40" s="278"/>
+      <c r="CD40" s="278"/>
+      <c r="CE40" s="278"/>
+      <c r="CF40" s="278"/>
+      <c r="CG40" s="279"/>
       <c r="CH40" s="42"/>
       <c r="CL40" s="41"/>
       <c r="CS40" s="42"/>
       <c r="CV40" s="41"/>
-      <c r="CW40" s="266"/>
-      <c r="CX40" s="267"/>
-      <c r="CY40" s="267"/>
-      <c r="CZ40" s="267"/>
-      <c r="DA40" s="267"/>
-      <c r="DB40" s="268"/>
+      <c r="CW40" s="291"/>
+      <c r="CX40" s="292"/>
+      <c r="CY40" s="292"/>
+      <c r="CZ40" s="292"/>
+      <c r="DA40" s="292"/>
+      <c r="DB40" s="293"/>
       <c r="DC40" s="42"/>
     </row>
     <row r="41" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
@@ -9024,43 +8994,43 @@
       <c r="M42" s="44"/>
       <c r="N42" s="44"/>
       <c r="O42" s="115"/>
-      <c r="P42" s="269" t="s">
+      <c r="P42" s="255" t="s">
         <v>323</v>
       </c>
-      <c r="Q42" s="258"/>
-      <c r="R42" s="258"/>
-      <c r="S42" s="258"/>
-      <c r="T42" s="258"/>
-      <c r="U42" s="258"/>
-      <c r="V42" s="258"/>
-      <c r="W42" s="258"/>
-      <c r="X42" s="258"/>
-      <c r="Y42" s="258"/>
-      <c r="Z42" s="258"/>
-      <c r="AA42" s="258"/>
-      <c r="AB42" s="258"/>
-      <c r="AC42" s="258"/>
-      <c r="AD42" s="258"/>
-      <c r="AE42" s="258"/>
-      <c r="AF42" s="258"/>
-      <c r="AG42" s="258"/>
-      <c r="AH42" s="258"/>
-      <c r="AI42" s="258"/>
-      <c r="AJ42" s="258"/>
-      <c r="AK42" s="258"/>
-      <c r="AL42" s="258"/>
-      <c r="AM42" s="258"/>
-      <c r="AN42" s="258"/>
-      <c r="AO42" s="258"/>
-      <c r="AP42" s="258"/>
-      <c r="AQ42" s="258"/>
-      <c r="AR42" s="258"/>
-      <c r="AS42" s="258"/>
-      <c r="AT42" s="258"/>
-      <c r="AU42" s="258"/>
-      <c r="AV42" s="258"/>
-      <c r="AW42" s="258"/>
-      <c r="AX42" s="259"/>
+      <c r="Q42" s="256"/>
+      <c r="R42" s="256"/>
+      <c r="S42" s="256"/>
+      <c r="T42" s="256"/>
+      <c r="U42" s="256"/>
+      <c r="V42" s="256"/>
+      <c r="W42" s="256"/>
+      <c r="X42" s="256"/>
+      <c r="Y42" s="256"/>
+      <c r="Z42" s="256"/>
+      <c r="AA42" s="256"/>
+      <c r="AB42" s="256"/>
+      <c r="AC42" s="256"/>
+      <c r="AD42" s="256"/>
+      <c r="AE42" s="256"/>
+      <c r="AF42" s="256"/>
+      <c r="AG42" s="256"/>
+      <c r="AH42" s="256"/>
+      <c r="AI42" s="256"/>
+      <c r="AJ42" s="256"/>
+      <c r="AK42" s="256"/>
+      <c r="AL42" s="256"/>
+      <c r="AM42" s="256"/>
+      <c r="AN42" s="256"/>
+      <c r="AO42" s="256"/>
+      <c r="AP42" s="256"/>
+      <c r="AQ42" s="256"/>
+      <c r="AR42" s="256"/>
+      <c r="AS42" s="256"/>
+      <c r="AT42" s="256"/>
+      <c r="AU42" s="256"/>
+      <c r="AV42" s="256"/>
+      <c r="AW42" s="256"/>
+      <c r="AX42" s="257"/>
       <c r="AY42" s="115"/>
       <c r="BD42" s="43"/>
       <c r="BE42" s="44"/>
@@ -9105,78 +9075,6 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="P42:AX42"/>
-    <mergeCell ref="AY12:AY40"/>
-    <mergeCell ref="G11:N12"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="T17:W17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="BD11:BK12"/>
-    <mergeCell ref="BD14:BK14"/>
-    <mergeCell ref="BP11:BW12"/>
-    <mergeCell ref="BP14:BW14"/>
-    <mergeCell ref="CA11:CH12"/>
-    <mergeCell ref="CA14:CH14"/>
-    <mergeCell ref="CL11:CS12"/>
-    <mergeCell ref="CL14:CS14"/>
-    <mergeCell ref="CV11:DC12"/>
-    <mergeCell ref="CV14:DC14"/>
-    <mergeCell ref="BQ24:BV24"/>
-    <mergeCell ref="CM18:CR18"/>
-    <mergeCell ref="CM19:CR19"/>
-    <mergeCell ref="CM21:CR21"/>
-    <mergeCell ref="CM24:CR24"/>
-    <mergeCell ref="CM23:CR23"/>
-    <mergeCell ref="BE19:BJ19"/>
-    <mergeCell ref="BE18:BJ18"/>
-    <mergeCell ref="BE21:BJ21"/>
-    <mergeCell ref="BE22:BJ22"/>
-    <mergeCell ref="BQ19:BV19"/>
-    <mergeCell ref="BQ18:BV18"/>
-    <mergeCell ref="BQ21:BV21"/>
-    <mergeCell ref="BQ22:BV22"/>
-    <mergeCell ref="BE24:BJ24"/>
-    <mergeCell ref="BE25:BJ25"/>
-    <mergeCell ref="BE27:BJ27"/>
-    <mergeCell ref="BE28:BF28"/>
-    <mergeCell ref="BI28:BJ28"/>
-    <mergeCell ref="BG28:BH28"/>
-    <mergeCell ref="BE32:BJ33"/>
-    <mergeCell ref="CF29:CG29"/>
-    <mergeCell ref="CD29:CE29"/>
-    <mergeCell ref="CB29:CC29"/>
-    <mergeCell ref="CB28:CG28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="CB39:CG40"/>
-    <mergeCell ref="CB17:CG17"/>
-    <mergeCell ref="CB18:CC18"/>
-    <mergeCell ref="CD18:CE18"/>
-    <mergeCell ref="CF18:CG18"/>
-    <mergeCell ref="CB20:CG20"/>
-    <mergeCell ref="CF26:CG26"/>
-    <mergeCell ref="CD26:CE26"/>
-    <mergeCell ref="CB26:CC26"/>
-    <mergeCell ref="CB25:CG25"/>
-    <mergeCell ref="CE23:CH23"/>
-    <mergeCell ref="CB21:CG21"/>
-    <mergeCell ref="BQ36:BV36"/>
-    <mergeCell ref="CB31:CG31"/>
-    <mergeCell ref="CB32:CC32"/>
-    <mergeCell ref="CD32:CE32"/>
-    <mergeCell ref="CF32:CG32"/>
-    <mergeCell ref="CB34:CG34"/>
-    <mergeCell ref="CB35:CC35"/>
-    <mergeCell ref="CD35:CE35"/>
-    <mergeCell ref="CF35:CG35"/>
-    <mergeCell ref="BQ32:BV33"/>
-    <mergeCell ref="BQ25:BV25"/>
-    <mergeCell ref="BQ27:BV27"/>
-    <mergeCell ref="CM32:CR32"/>
-    <mergeCell ref="CM33:CR33"/>
-    <mergeCell ref="CM35:CR35"/>
-    <mergeCell ref="CM27:CR27"/>
-    <mergeCell ref="CM26:CR26"/>
-    <mergeCell ref="BQ35:BV35"/>
     <mergeCell ref="CM36:CR36"/>
     <mergeCell ref="CW18:DB18"/>
     <mergeCell ref="CW20:DB20"/>
@@ -9193,6 +9091,78 @@
     <mergeCell ref="CW36:DB40"/>
     <mergeCell ref="CM29:CR29"/>
     <mergeCell ref="CM30:CR30"/>
+    <mergeCell ref="BQ25:BV25"/>
+    <mergeCell ref="BQ27:BV27"/>
+    <mergeCell ref="CM32:CR32"/>
+    <mergeCell ref="CM33:CR33"/>
+    <mergeCell ref="CM35:CR35"/>
+    <mergeCell ref="CM27:CR27"/>
+    <mergeCell ref="CM26:CR26"/>
+    <mergeCell ref="BQ35:BV35"/>
+    <mergeCell ref="BQ36:BV36"/>
+    <mergeCell ref="CB31:CG31"/>
+    <mergeCell ref="CB32:CC32"/>
+    <mergeCell ref="CD32:CE32"/>
+    <mergeCell ref="CF32:CG32"/>
+    <mergeCell ref="CB34:CG34"/>
+    <mergeCell ref="CB35:CC35"/>
+    <mergeCell ref="CD35:CE35"/>
+    <mergeCell ref="CF35:CG35"/>
+    <mergeCell ref="BQ32:BV33"/>
+    <mergeCell ref="CB39:CG40"/>
+    <mergeCell ref="CB17:CG17"/>
+    <mergeCell ref="CB18:CC18"/>
+    <mergeCell ref="CD18:CE18"/>
+    <mergeCell ref="CF18:CG18"/>
+    <mergeCell ref="CB20:CG20"/>
+    <mergeCell ref="CF26:CG26"/>
+    <mergeCell ref="CD26:CE26"/>
+    <mergeCell ref="CB26:CC26"/>
+    <mergeCell ref="CB25:CG25"/>
+    <mergeCell ref="CE23:CH23"/>
+    <mergeCell ref="CB21:CG21"/>
+    <mergeCell ref="BE32:BJ33"/>
+    <mergeCell ref="CF29:CG29"/>
+    <mergeCell ref="CD29:CE29"/>
+    <mergeCell ref="CB29:CC29"/>
+    <mergeCell ref="CB28:CG28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="BE24:BJ24"/>
+    <mergeCell ref="BE25:BJ25"/>
+    <mergeCell ref="BE27:BJ27"/>
+    <mergeCell ref="BE28:BF28"/>
+    <mergeCell ref="BI28:BJ28"/>
+    <mergeCell ref="BG28:BH28"/>
+    <mergeCell ref="BE19:BJ19"/>
+    <mergeCell ref="BE18:BJ18"/>
+    <mergeCell ref="BE21:BJ21"/>
+    <mergeCell ref="BE22:BJ22"/>
+    <mergeCell ref="BQ19:BV19"/>
+    <mergeCell ref="BQ18:BV18"/>
+    <mergeCell ref="BQ21:BV21"/>
+    <mergeCell ref="BQ22:BV22"/>
+    <mergeCell ref="CL11:CS12"/>
+    <mergeCell ref="CL14:CS14"/>
+    <mergeCell ref="CV11:DC12"/>
+    <mergeCell ref="CV14:DC14"/>
+    <mergeCell ref="BQ24:BV24"/>
+    <mergeCell ref="CM18:CR18"/>
+    <mergeCell ref="CM19:CR19"/>
+    <mergeCell ref="CM21:CR21"/>
+    <mergeCell ref="CM24:CR24"/>
+    <mergeCell ref="CM23:CR23"/>
+    <mergeCell ref="BD11:BK12"/>
+    <mergeCell ref="BD14:BK14"/>
+    <mergeCell ref="BP11:BW12"/>
+    <mergeCell ref="BP14:BW14"/>
+    <mergeCell ref="CA11:CH12"/>
+    <mergeCell ref="CA14:CH14"/>
+    <mergeCell ref="P42:AX42"/>
+    <mergeCell ref="AY12:AY40"/>
+    <mergeCell ref="G11:N12"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="T17:W17"/>
+    <mergeCell ref="P17:R17"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9251,14 +9221,14 @@
         <v>476</v>
       </c>
       <c r="C3" s="28"/>
-      <c r="D3" s="296" t="s">
+      <c r="D3" s="299" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="297"/>
-      <c r="F3" s="297"/>
-      <c r="G3" s="297"/>
-      <c r="H3" s="297"/>
-      <c r="I3" s="298"/>
+      <c r="E3" s="300"/>
+      <c r="F3" s="300"/>
+      <c r="G3" s="300"/>
+      <c r="H3" s="300"/>
+      <c r="I3" s="301"/>
     </row>
     <row r="4" spans="1:16" ht="21" customHeight="1">
       <c r="A4" s="156" t="s">
@@ -9397,15 +9367,15 @@
         <v>375</v>
       </c>
       <c r="F12" s="132"/>
-      <c r="H12" s="299" t="s">
+      <c r="H12" s="294" t="s">
         <v>400</v>
       </c>
-      <c r="I12" s="300"/>
+      <c r="I12" s="302"/>
       <c r="J12" s="140" t="s">
         <v>404</v>
       </c>
       <c r="K12" s="132"/>
-      <c r="M12" s="299" t="s">
+      <c r="M12" s="294" t="s">
         <v>415</v>
       </c>
       <c r="N12" s="295"/>
@@ -9422,15 +9392,15 @@
         <v>368</v>
       </c>
       <c r="F13" s="132"/>
-      <c r="H13" s="299" t="s">
+      <c r="H13" s="294" t="s">
         <v>401</v>
       </c>
-      <c r="I13" s="300"/>
+      <c r="I13" s="302"/>
       <c r="J13" s="140" t="s">
         <v>403</v>
       </c>
       <c r="K13" s="132"/>
-      <c r="M13" s="299" t="s">
+      <c r="M13" s="294" t="s">
         <v>216</v>
       </c>
       <c r="N13" s="295"/>
@@ -9445,15 +9415,15 @@
       </c>
       <c r="E14" s="131"/>
       <c r="F14" s="132"/>
-      <c r="H14" s="299" t="s">
+      <c r="H14" s="294" t="s">
         <v>402</v>
       </c>
-      <c r="I14" s="300"/>
+      <c r="I14" s="302"/>
       <c r="J14" s="140" t="s">
         <v>369</v>
       </c>
       <c r="K14" s="132"/>
-      <c r="M14" s="299" t="s">
+      <c r="M14" s="294" t="s">
         <v>215</v>
       </c>
       <c r="N14" s="295"/>
@@ -9468,11 +9438,11 @@
       </c>
       <c r="E15" s="140"/>
       <c r="F15" s="132"/>
-      <c r="H15" s="301"/>
-      <c r="I15" s="302"/>
+      <c r="H15" s="297"/>
+      <c r="I15" s="298"/>
       <c r="J15" s="140"/>
       <c r="K15" s="132"/>
-      <c r="M15" s="299" t="s">
+      <c r="M15" s="294" t="s">
         <v>211</v>
       </c>
       <c r="N15" s="295"/>
@@ -9487,11 +9457,11 @@
       </c>
       <c r="E16" s="131"/>
       <c r="F16" s="134"/>
-      <c r="H16" s="301"/>
-      <c r="I16" s="302"/>
+      <c r="H16" s="297"/>
+      <c r="I16" s="298"/>
       <c r="J16" s="140"/>
       <c r="K16" s="132"/>
-      <c r="M16" s="299" t="s">
+      <c r="M16" s="294" t="s">
         <v>212</v>
       </c>
       <c r="N16" s="295"/>
@@ -9510,7 +9480,7 @@
       <c r="I17" s="135"/>
       <c r="J17" s="136"/>
       <c r="K17" s="137"/>
-      <c r="M17" s="299" t="s">
+      <c r="M17" s="294" t="s">
         <v>416</v>
       </c>
       <c r="N17" s="295"/>
@@ -9523,7 +9493,7 @@
       <c r="C18" s="133"/>
       <c r="E18" s="131"/>
       <c r="F18" s="134"/>
-      <c r="M18" s="299" t="s">
+      <c r="M18" s="294" t="s">
         <v>213</v>
       </c>
       <c r="N18" s="295"/>
@@ -9546,7 +9516,7 @@
       <c r="K19" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="M19" s="299" t="s">
+      <c r="M19" s="294" t="s">
         <v>290</v>
       </c>
       <c r="N19" s="295"/>
@@ -9567,7 +9537,7 @@
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
       <c r="K20" s="127"/>
-      <c r="M20" s="294" t="s">
+      <c r="M20" s="296" t="s">
         <v>423</v>
       </c>
       <c r="N20" s="295"/>
@@ -9584,7 +9554,7 @@
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
       <c r="K21" s="127"/>
-      <c r="M21" s="294" t="s">
+      <c r="M21" s="296" t="s">
         <v>424</v>
       </c>
       <c r="N21" s="295"/>
@@ -9604,21 +9574,21 @@
         <v>84</v>
       </c>
       <c r="K22" s="130"/>
-      <c r="M22" s="294"/>
+      <c r="M22" s="296"/>
       <c r="N22" s="295"/>
       <c r="O22" s="131"/>
       <c r="P22" s="132"/>
     </row>
     <row r="23" spans="3:16" ht="15.75" customHeight="1" thickBot="1">
-      <c r="H23" s="299" t="s">
+      <c r="H23" s="294" t="s">
         <v>405</v>
       </c>
-      <c r="I23" s="300"/>
+      <c r="I23" s="302"/>
       <c r="J23" s="140" t="s">
         <v>369</v>
       </c>
       <c r="K23" s="132"/>
-      <c r="M23" s="294"/>
+      <c r="M23" s="296"/>
       <c r="N23" s="295"/>
       <c r="O23" s="131"/>
       <c r="P23" s="132"/>
@@ -9632,11 +9602,11 @@
       <c r="F24" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="H24" s="299"/>
-      <c r="I24" s="300"/>
+      <c r="H24" s="294"/>
+      <c r="I24" s="302"/>
       <c r="J24" s="140"/>
       <c r="K24" s="132"/>
-      <c r="M24" s="294"/>
+      <c r="M24" s="296"/>
       <c r="N24" s="295"/>
       <c r="O24" s="131"/>
       <c r="P24" s="132"/>
@@ -9650,11 +9620,11 @@
       <c r="F25" s="143" t="s">
         <v>373</v>
       </c>
-      <c r="H25" s="299"/>
-      <c r="I25" s="300"/>
+      <c r="H25" s="294"/>
+      <c r="I25" s="302"/>
       <c r="J25" s="140"/>
       <c r="K25" s="132"/>
-      <c r="M25" s="294"/>
+      <c r="M25" s="296"/>
       <c r="N25" s="295"/>
       <c r="O25" s="131"/>
       <c r="P25" s="132"/>
@@ -9664,11 +9634,11 @@
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="127"/>
-      <c r="H26" s="301"/>
-      <c r="I26" s="302"/>
+      <c r="H26" s="297"/>
+      <c r="I26" s="298"/>
       <c r="J26" s="140"/>
       <c r="K26" s="132"/>
-      <c r="M26" s="294"/>
+      <c r="M26" s="296"/>
       <c r="N26" s="295"/>
       <c r="O26" s="131"/>
       <c r="P26" s="132"/>
@@ -9682,11 +9652,11 @@
         <v>84</v>
       </c>
       <c r="F27" s="130"/>
-      <c r="H27" s="301"/>
-      <c r="I27" s="302"/>
+      <c r="H27" s="297"/>
+      <c r="I27" s="298"/>
       <c r="J27" s="140"/>
       <c r="K27" s="132"/>
-      <c r="M27" s="294"/>
+      <c r="M27" s="296"/>
       <c r="N27" s="295"/>
       <c r="O27" s="131"/>
       <c r="P27" s="132"/>
@@ -9703,7 +9673,7 @@
       <c r="I28" s="135"/>
       <c r="J28" s="136"/>
       <c r="K28" s="137"/>
-      <c r="M28" s="294"/>
+      <c r="M28" s="296"/>
       <c r="N28" s="295"/>
       <c r="O28" s="131"/>
       <c r="P28" s="132"/>
@@ -9716,7 +9686,7 @@
         <v>388</v>
       </c>
       <c r="F29" s="132"/>
-      <c r="M29" s="294"/>
+      <c r="M29" s="296"/>
       <c r="N29" s="295"/>
       <c r="O29" s="131"/>
       <c r="P29" s="132"/>
@@ -9727,7 +9697,7 @@
       </c>
       <c r="E30" s="140"/>
       <c r="F30" s="132"/>
-      <c r="M30" s="294"/>
+      <c r="M30" s="296"/>
       <c r="N30" s="295"/>
       <c r="O30" s="131"/>
       <c r="P30" s="132"/>
@@ -9808,7 +9778,7 @@
       <c r="C37" s="133"/>
       <c r="E37" s="131"/>
       <c r="F37" s="134"/>
-      <c r="M37" s="299" t="s">
+      <c r="M37" s="294" t="s">
         <v>428</v>
       </c>
       <c r="N37" s="295"/>
@@ -9821,7 +9791,7 @@
       <c r="C38" s="133"/>
       <c r="E38" s="131"/>
       <c r="F38" s="134"/>
-      <c r="M38" s="294" t="s">
+      <c r="M38" s="296" t="s">
         <v>429</v>
       </c>
       <c r="N38" s="295"/>
@@ -9835,7 +9805,7 @@
       <c r="D39" s="135"/>
       <c r="E39" s="136"/>
       <c r="F39" s="139"/>
-      <c r="M39" s="294"/>
+      <c r="M39" s="296"/>
       <c r="N39" s="295"/>
       <c r="O39" s="131" t="s">
         <v>432</v>
@@ -9843,7 +9813,7 @@
       <c r="P39" s="132"/>
     </row>
     <row r="40" spans="3:16" ht="15.75" customHeight="1" thickBot="1">
-      <c r="M40" s="294"/>
+      <c r="M40" s="296"/>
       <c r="N40" s="295"/>
       <c r="O40" s="131" t="s">
         <v>433</v>
@@ -9859,7 +9829,7 @@
       <c r="F41" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="M41" s="294"/>
+      <c r="M41" s="296"/>
       <c r="N41" s="295"/>
       <c r="O41" s="131" t="s">
         <v>435</v>
@@ -9875,7 +9845,7 @@
       <c r="F42" s="143" t="s">
         <v>373</v>
       </c>
-      <c r="M42" s="294"/>
+      <c r="M42" s="296"/>
       <c r="N42" s="295"/>
       <c r="O42" s="131" t="s">
         <v>434</v>
@@ -9970,7 +9940,7 @@
         <v>397</v>
       </c>
       <c r="F49" s="134"/>
-      <c r="M49" s="299" t="s">
+      <c r="M49" s="294" t="s">
         <v>436</v>
       </c>
       <c r="N49" s="295"/>
@@ -9987,7 +9957,7 @@
         <v>334</v>
       </c>
       <c r="F50" s="134"/>
-      <c r="M50" s="294" t="s">
+      <c r="M50" s="296" t="s">
         <v>437</v>
       </c>
       <c r="N50" s="295"/>
@@ -10004,7 +9974,7 @@
         <v>369</v>
       </c>
       <c r="F51" s="134"/>
-      <c r="M51" s="294" t="s">
+      <c r="M51" s="296" t="s">
         <v>438</v>
       </c>
       <c r="N51" s="295"/>
@@ -10017,7 +9987,7 @@
         <v>456</v>
       </c>
       <c r="F52" s="134"/>
-      <c r="M52" s="294" t="s">
+      <c r="M52" s="296" t="s">
         <v>441</v>
       </c>
       <c r="N52" s="295"/>
@@ -10031,7 +10001,7 @@
         <v>457</v>
       </c>
       <c r="F53" s="137"/>
-      <c r="M53" s="294"/>
+      <c r="M53" s="296"/>
       <c r="N53" s="295"/>
       <c r="O53" s="131"/>
       <c r="P53" s="132"/>
@@ -10084,7 +10054,7 @@
       </c>
     </row>
     <row r="60" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M60" s="299" t="s">
+      <c r="M60" s="294" t="s">
         <v>442</v>
       </c>
       <c r="N60" s="295"/>
@@ -10096,7 +10066,7 @@
       </c>
     </row>
     <row r="61" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M61" s="294" t="s">
+      <c r="M61" s="296" t="s">
         <v>443</v>
       </c>
       <c r="N61" s="295"/>
@@ -10108,7 +10078,7 @@
       </c>
     </row>
     <row r="62" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M62" s="299" t="s">
+      <c r="M62" s="294" t="s">
         <v>448</v>
       </c>
       <c r="N62" s="295"/>
@@ -10120,13 +10090,13 @@
       </c>
     </row>
     <row r="63" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M63" s="294"/>
+      <c r="M63" s="296"/>
       <c r="N63" s="295"/>
       <c r="O63" s="131"/>
       <c r="P63" s="132"/>
     </row>
     <row r="64" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M64" s="294"/>
+      <c r="M64" s="296"/>
       <c r="N64" s="295"/>
       <c r="O64" s="131"/>
       <c r="P64" s="132"/>
@@ -10175,7 +10145,7 @@
       <c r="P70" s="130"/>
     </row>
     <row r="71" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M71" s="299" t="s">
+      <c r="M71" s="294" t="s">
         <v>449</v>
       </c>
       <c r="N71" s="295"/>
@@ -10185,7 +10155,7 @@
       <c r="P71" s="132"/>
     </row>
     <row r="72" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M72" s="299" t="s">
+      <c r="M72" s="294" t="s">
         <v>450</v>
       </c>
       <c r="N72" s="295"/>
@@ -10195,19 +10165,19 @@
       <c r="P72" s="132"/>
     </row>
     <row r="73" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M73" s="294"/>
+      <c r="M73" s="296"/>
       <c r="N73" s="295"/>
       <c r="O73" s="131"/>
       <c r="P73" s="132"/>
     </row>
     <row r="74" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M74" s="294"/>
+      <c r="M74" s="296"/>
       <c r="N74" s="295"/>
       <c r="O74" s="131"/>
       <c r="P74" s="132"/>
     </row>
     <row r="75" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M75" s="294"/>
+      <c r="M75" s="296"/>
       <c r="N75" s="295"/>
       <c r="O75" s="131"/>
       <c r="P75" s="132"/>
@@ -10256,7 +10226,7 @@
       <c r="P81" s="130"/>
     </row>
     <row r="82" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M82" s="299" t="s">
+      <c r="M82" s="294" t="s">
         <v>449</v>
       </c>
       <c r="N82" s="295"/>
@@ -10266,7 +10236,7 @@
       <c r="P82" s="132"/>
     </row>
     <row r="83" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M83" s="299" t="s">
+      <c r="M83" s="294" t="s">
         <v>452</v>
       </c>
       <c r="N83" s="295"/>
@@ -10276,19 +10246,19 @@
       <c r="P83" s="132"/>
     </row>
     <row r="84" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M84" s="294"/>
+      <c r="M84" s="296"/>
       <c r="N84" s="295"/>
       <c r="O84" s="131"/>
       <c r="P84" s="132"/>
     </row>
     <row r="85" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M85" s="294"/>
+      <c r="M85" s="296"/>
       <c r="N85" s="295"/>
       <c r="O85" s="131"/>
       <c r="P85" s="132"/>
     </row>
     <row r="86" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M86" s="294"/>
+      <c r="M86" s="296"/>
       <c r="N86" s="295"/>
       <c r="O86" s="131"/>
       <c r="P86" s="132"/>
@@ -10335,7 +10305,7 @@
       <c r="P92" s="130"/>
     </row>
     <row r="93" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M93" s="299" t="s">
+      <c r="M93" s="294" t="s">
         <v>216</v>
       </c>
       <c r="N93" s="295"/>
@@ -10345,7 +10315,7 @@
       <c r="P93" s="132"/>
     </row>
     <row r="94" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M94" s="294"/>
+      <c r="M94" s="296"/>
       <c r="N94" s="295"/>
       <c r="O94" s="140" t="s">
         <v>454</v>
@@ -10353,7 +10323,7 @@
       <c r="P94" s="132"/>
     </row>
     <row r="95" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M95" s="294"/>
+      <c r="M95" s="296"/>
       <c r="N95" s="295"/>
       <c r="O95" s="140" t="s">
         <v>455</v>
@@ -10361,13 +10331,13 @@
       <c r="P95" s="132"/>
     </row>
     <row r="96" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M96" s="294"/>
+      <c r="M96" s="296"/>
       <c r="N96" s="295"/>
       <c r="O96" s="131"/>
       <c r="P96" s="132"/>
     </row>
     <row r="97" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M97" s="294"/>
+      <c r="M97" s="296"/>
       <c r="N97" s="295"/>
       <c r="O97" s="131"/>
       <c r="P97" s="132"/>
@@ -10414,7 +10384,7 @@
       <c r="P103" s="130"/>
     </row>
     <row r="104" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M104" s="299" t="s">
+      <c r="M104" s="294" t="s">
         <v>465</v>
       </c>
       <c r="N104" s="295"/>
@@ -10424,7 +10394,7 @@
       <c r="P104" s="132"/>
     </row>
     <row r="105" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M105" s="299" t="s">
+      <c r="M105" s="294" t="s">
         <v>466</v>
       </c>
       <c r="N105" s="295"/>
@@ -10434,7 +10404,7 @@
       <c r="P105" s="132"/>
     </row>
     <row r="106" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M106" s="299" t="s">
+      <c r="M106" s="294" t="s">
         <v>467</v>
       </c>
       <c r="N106" s="295"/>
@@ -10444,7 +10414,7 @@
       <c r="P106" s="132"/>
     </row>
     <row r="107" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M107" s="294"/>
+      <c r="M107" s="296"/>
       <c r="N107" s="295"/>
       <c r="O107" s="140" t="s">
         <v>464</v>
@@ -10452,7 +10422,7 @@
       <c r="P107" s="132"/>
     </row>
     <row r="108" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M108" s="294"/>
+      <c r="M108" s="296"/>
       <c r="N108" s="295"/>
       <c r="O108" s="131"/>
       <c r="P108" s="132"/>
@@ -10501,7 +10471,7 @@
       <c r="P114" s="130"/>
     </row>
     <row r="115" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M115" s="299" t="s">
+      <c r="M115" s="294" t="s">
         <v>482</v>
       </c>
       <c r="N115" s="295"/>
@@ -10511,31 +10481,31 @@
       <c r="P115" s="132"/>
     </row>
     <row r="116" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M116" s="294"/>
+      <c r="M116" s="296"/>
       <c r="N116" s="295"/>
       <c r="O116" s="131"/>
       <c r="P116" s="132"/>
     </row>
     <row r="117" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M117" s="294"/>
+      <c r="M117" s="296"/>
       <c r="N117" s="295"/>
       <c r="O117" s="131"/>
       <c r="P117" s="132"/>
     </row>
     <row r="118" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M118" s="294"/>
+      <c r="M118" s="296"/>
       <c r="N118" s="295"/>
       <c r="O118" s="131"/>
       <c r="P118" s="132"/>
     </row>
     <row r="119" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M119" s="294"/>
+      <c r="M119" s="296"/>
       <c r="N119" s="295"/>
       <c r="O119" s="131"/>
       <c r="P119" s="132"/>
     </row>
     <row r="120" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M120" s="294"/>
+      <c r="M120" s="296"/>
       <c r="N120" s="295"/>
       <c r="O120" s="131"/>
       <c r="P120" s="132"/>
@@ -10548,46 +10518,22 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="M104:N104"/>
-    <mergeCell ref="M83:N83"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="M72:N72"/>
-    <mergeCell ref="M73:N73"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="M82:N82"/>
-    <mergeCell ref="M61:N61"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="M63:N63"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M71:N71"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="M51:N51"/>
-    <mergeCell ref="M52:N52"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M49:N49"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M119:N119"/>
+    <mergeCell ref="M120:N120"/>
+    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="M115:N115"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="M117:N117"/>
+    <mergeCell ref="M118:N118"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
     <mergeCell ref="M37:N37"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="M12:N12"/>
@@ -10604,22 +10550,46 @@
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="M22:N22"/>
     <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M119:N119"/>
-    <mergeCell ref="M120:N120"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="M115:N115"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="M117:N117"/>
-    <mergeCell ref="M118:N118"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="M61:N61"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="M63:N63"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M71:N71"/>
+    <mergeCell ref="M72:N72"/>
+    <mergeCell ref="M73:N73"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="M82:N82"/>
+    <mergeCell ref="M83:N83"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="M104:N104"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
@@ -15718,8 +15688,8 @@
   </sheetPr>
   <dimension ref="B2:U215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -20436,52 +20406,42 @@
     <mergeCell ref="H3:P3"/>
     <mergeCell ref="R6:U214"/>
   </mergeCells>
-  <conditionalFormatting sqref="B12:D27 C28:C38 B28:B213 D38 C40:C48 D51 C51:C61 C64:C220 D59:D213">
-    <cfRule type="expression" dxfId="9" priority="7">
+  <conditionalFormatting sqref="B12:D27 C28:C38 B28:B213 D38 C40:C48 D51 C51:C61 C64:C220">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>IF((B12&lt;&gt;"")*AND(F12&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>IF((C35&lt;&gt;"")*AND(G38&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39 C49">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>IF((C39&lt;&gt;"")*AND(G40&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="6" priority="18">
+    <cfRule type="expression" dxfId="4" priority="18">
       <formula>IF((C63&lt;&gt;"")*AND(G62&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:D37">
-    <cfRule type="expression" dxfId="5" priority="14">
+    <cfRule type="expression" dxfId="3" priority="14">
       <formula>IF((C28&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39:D42 D47:D48">
-    <cfRule type="expression" dxfId="4" priority="5">
+  <conditionalFormatting sqref="D39:D50">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>IF((D39&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43:D46">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>IF((D43&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D52:D56">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>IF((D52&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D49:D50">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>IF((D49&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57:D58">
+  <conditionalFormatting sqref="D57:D213">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF((D57&lt;&gt;"")*AND(H57&lt;&gt;""),1,0)</formula>
     </cfRule>

</xml_diff>

<commit_message>
add : maj chiffrier
</commit_message>
<xml_diff>
--- a/doc/chiffrier_sim_vie.xlsx
+++ b/doc/chiffrier_sim_vie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travail\sim_vie\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C938235-D468-49FF-9EEE-CE94D788650B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBAA21F-039C-4941-B9F7-1F09133F2A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Méthodes SCRUM" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="683">
   <si>
     <t>Chiffrier de documentation de projets</t>
   </si>
@@ -2148,9 +2148,6 @@
     <t>Implémenter rôle du système nerveux (envoyer message aux ganglions)</t>
   </si>
   <si>
-    <t>…</t>
-  </si>
-  <si>
     <t>SPRINT 2</t>
   </si>
   <si>
@@ -2272,6 +2269,24 @@
   </si>
   <si>
     <t>Ajout d'état : en train de se reproduire (enum)</t>
+  </si>
+  <si>
+    <t>La méthode n'est pas au bon endroit</t>
+  </si>
+  <si>
+    <t>N'est pas implémenté dans les actions</t>
+  </si>
+  <si>
+    <t>Connecter les états à l'action manger (setTimeOut)</t>
+  </si>
+  <si>
+    <t>Connecter les états à l'action se reproduire (setTimeOut)</t>
+  </si>
+  <si>
+    <t>Problèmes à régler :</t>
+  </si>
+  <si>
+    <t>Replacer la logique de reproduction dans les classes responsables (modèle, créature, vue, contrôleur)</t>
   </si>
 </sst>
 </file>
@@ -3543,7 +3558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="314">
+  <cellXfs count="315">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4103,14 +4118,110 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -4121,110 +4232,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4233,18 +4260,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4278,6 +4293,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7606,16 +7622,16 @@
       <c r="W10" s="29"/>
     </row>
     <row r="11" spans="1:107" thickBot="1">
-      <c r="G11" s="261" t="s">
+      <c r="G11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="H11" s="262"/>
-      <c r="I11" s="262"/>
-      <c r="J11" s="262"/>
-      <c r="K11" s="262"/>
-      <c r="L11" s="262"/>
-      <c r="M11" s="262"/>
-      <c r="N11" s="263"/>
+      <c r="H11" s="282"/>
+      <c r="I11" s="282"/>
+      <c r="J11" s="282"/>
+      <c r="K11" s="282"/>
+      <c r="L11" s="282"/>
+      <c r="M11" s="282"/>
+      <c r="N11" s="283"/>
       <c r="O11" s="48"/>
       <c r="P11" s="39"/>
       <c r="Q11" s="39"/>
@@ -7653,66 +7669,66 @@
       <c r="AW11" s="47"/>
       <c r="AX11" s="113"/>
       <c r="AY11" s="115"/>
-      <c r="BD11" s="261" t="s">
+      <c r="BD11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="BE11" s="262"/>
-      <c r="BF11" s="262"/>
-      <c r="BG11" s="262"/>
-      <c r="BH11" s="262"/>
-      <c r="BI11" s="262"/>
-      <c r="BJ11" s="262"/>
-      <c r="BK11" s="263"/>
-      <c r="BP11" s="261" t="s">
+      <c r="BE11" s="282"/>
+      <c r="BF11" s="282"/>
+      <c r="BG11" s="282"/>
+      <c r="BH11" s="282"/>
+      <c r="BI11" s="282"/>
+      <c r="BJ11" s="282"/>
+      <c r="BK11" s="283"/>
+      <c r="BP11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="BQ11" s="262"/>
-      <c r="BR11" s="262"/>
-      <c r="BS11" s="262"/>
-      <c r="BT11" s="262"/>
-      <c r="BU11" s="262"/>
-      <c r="BV11" s="262"/>
-      <c r="BW11" s="263"/>
-      <c r="CA11" s="261" t="s">
+      <c r="BQ11" s="282"/>
+      <c r="BR11" s="282"/>
+      <c r="BS11" s="282"/>
+      <c r="BT11" s="282"/>
+      <c r="BU11" s="282"/>
+      <c r="BV11" s="282"/>
+      <c r="BW11" s="283"/>
+      <c r="CA11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="CB11" s="262"/>
-      <c r="CC11" s="262"/>
-      <c r="CD11" s="262"/>
-      <c r="CE11" s="262"/>
-      <c r="CF11" s="262"/>
-      <c r="CG11" s="262"/>
-      <c r="CH11" s="263"/>
-      <c r="CL11" s="261" t="s">
+      <c r="CB11" s="282"/>
+      <c r="CC11" s="282"/>
+      <c r="CD11" s="282"/>
+      <c r="CE11" s="282"/>
+      <c r="CF11" s="282"/>
+      <c r="CG11" s="282"/>
+      <c r="CH11" s="283"/>
+      <c r="CL11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="CM11" s="262"/>
-      <c r="CN11" s="262"/>
-      <c r="CO11" s="262"/>
-      <c r="CP11" s="262"/>
-      <c r="CQ11" s="262"/>
-      <c r="CR11" s="262"/>
-      <c r="CS11" s="263"/>
-      <c r="CV11" s="261" t="s">
+      <c r="CM11" s="282"/>
+      <c r="CN11" s="282"/>
+      <c r="CO11" s="282"/>
+      <c r="CP11" s="282"/>
+      <c r="CQ11" s="282"/>
+      <c r="CR11" s="282"/>
+      <c r="CS11" s="283"/>
+      <c r="CV11" s="281" t="s">
         <v>324</v>
       </c>
-      <c r="CW11" s="262"/>
-      <c r="CX11" s="262"/>
-      <c r="CY11" s="262"/>
-      <c r="CZ11" s="262"/>
-      <c r="DA11" s="262"/>
-      <c r="DB11" s="262"/>
-      <c r="DC11" s="263"/>
+      <c r="CW11" s="282"/>
+      <c r="CX11" s="282"/>
+      <c r="CY11" s="282"/>
+      <c r="CZ11" s="282"/>
+      <c r="DA11" s="282"/>
+      <c r="DB11" s="282"/>
+      <c r="DC11" s="283"/>
     </row>
     <row r="12" spans="1:107" thickBot="1">
-      <c r="G12" s="264"/>
-      <c r="H12" s="265"/>
-      <c r="I12" s="265"/>
-      <c r="J12" s="265"/>
-      <c r="K12" s="265"/>
-      <c r="L12" s="265"/>
-      <c r="M12" s="265"/>
-      <c r="N12" s="266"/>
+      <c r="G12" s="284"/>
+      <c r="H12" s="285"/>
+      <c r="I12" s="285"/>
+      <c r="J12" s="285"/>
+      <c r="K12" s="285"/>
+      <c r="L12" s="285"/>
+      <c r="M12" s="285"/>
+      <c r="N12" s="286"/>
       <c r="O12" s="40"/>
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
@@ -7723,49 +7739,49 @@
       <c r="V12" s="29"/>
       <c r="W12" s="29"/>
       <c r="AX12" s="42"/>
-      <c r="AY12" s="258" t="s">
+      <c r="AY12" s="290" t="s">
         <v>323</v>
       </c>
-      <c r="BD12" s="264"/>
-      <c r="BE12" s="265"/>
-      <c r="BF12" s="265"/>
-      <c r="BG12" s="265"/>
-      <c r="BH12" s="265"/>
-      <c r="BI12" s="265"/>
-      <c r="BJ12" s="265"/>
-      <c r="BK12" s="266"/>
-      <c r="BP12" s="264"/>
-      <c r="BQ12" s="265"/>
-      <c r="BR12" s="265"/>
-      <c r="BS12" s="265"/>
-      <c r="BT12" s="265"/>
-      <c r="BU12" s="265"/>
-      <c r="BV12" s="265"/>
-      <c r="BW12" s="266"/>
-      <c r="CA12" s="264"/>
-      <c r="CB12" s="265"/>
-      <c r="CC12" s="265"/>
-      <c r="CD12" s="265"/>
-      <c r="CE12" s="265"/>
-      <c r="CF12" s="265"/>
-      <c r="CG12" s="265"/>
-      <c r="CH12" s="266"/>
-      <c r="CL12" s="264"/>
-      <c r="CM12" s="265"/>
-      <c r="CN12" s="265"/>
-      <c r="CO12" s="265"/>
-      <c r="CP12" s="265"/>
-      <c r="CQ12" s="265"/>
-      <c r="CR12" s="265"/>
-      <c r="CS12" s="266"/>
-      <c r="CV12" s="264"/>
-      <c r="CW12" s="265"/>
-      <c r="CX12" s="265"/>
-      <c r="CY12" s="265"/>
-      <c r="CZ12" s="265"/>
-      <c r="DA12" s="265"/>
-      <c r="DB12" s="265"/>
-      <c r="DC12" s="266"/>
+      <c r="BD12" s="284"/>
+      <c r="BE12" s="285"/>
+      <c r="BF12" s="285"/>
+      <c r="BG12" s="285"/>
+      <c r="BH12" s="285"/>
+      <c r="BI12" s="285"/>
+      <c r="BJ12" s="285"/>
+      <c r="BK12" s="286"/>
+      <c r="BP12" s="284"/>
+      <c r="BQ12" s="285"/>
+      <c r="BR12" s="285"/>
+      <c r="BS12" s="285"/>
+      <c r="BT12" s="285"/>
+      <c r="BU12" s="285"/>
+      <c r="BV12" s="285"/>
+      <c r="BW12" s="286"/>
+      <c r="CA12" s="284"/>
+      <c r="CB12" s="285"/>
+      <c r="CC12" s="285"/>
+      <c r="CD12" s="285"/>
+      <c r="CE12" s="285"/>
+      <c r="CF12" s="285"/>
+      <c r="CG12" s="285"/>
+      <c r="CH12" s="286"/>
+      <c r="CL12" s="284"/>
+      <c r="CM12" s="285"/>
+      <c r="CN12" s="285"/>
+      <c r="CO12" s="285"/>
+      <c r="CP12" s="285"/>
+      <c r="CQ12" s="285"/>
+      <c r="CR12" s="285"/>
+      <c r="CS12" s="286"/>
+      <c r="CV12" s="284"/>
+      <c r="CW12" s="285"/>
+      <c r="CX12" s="285"/>
+      <c r="CY12" s="285"/>
+      <c r="CZ12" s="285"/>
+      <c r="DA12" s="285"/>
+      <c r="DB12" s="285"/>
+      <c r="DC12" s="286"/>
     </row>
     <row r="13" spans="1:107" thickBot="1">
       <c r="G13" s="40"/>
@@ -7784,7 +7800,7 @@
       <c r="V13" s="29"/>
       <c r="W13" s="29"/>
       <c r="AX13" s="42"/>
-      <c r="AY13" s="259"/>
+      <c r="AY13" s="291"/>
       <c r="BD13" s="40"/>
       <c r="BG13" s="29"/>
       <c r="BH13" s="29"/>
@@ -7809,16 +7825,16 @@
       <c r="DC13" s="42"/>
     </row>
     <row r="14" spans="1:107" thickBot="1">
-      <c r="G14" s="267" t="s">
+      <c r="G14" s="287" t="s">
         <v>325</v>
       </c>
-      <c r="H14" s="268"/>
-      <c r="I14" s="268"/>
-      <c r="J14" s="268"/>
-      <c r="K14" s="268"/>
-      <c r="L14" s="268"/>
-      <c r="M14" s="268"/>
-      <c r="N14" s="269"/>
+      <c r="H14" s="288"/>
+      <c r="I14" s="288"/>
+      <c r="J14" s="288"/>
+      <c r="K14" s="288"/>
+      <c r="L14" s="288"/>
+      <c r="M14" s="288"/>
+      <c r="N14" s="289"/>
       <c r="O14" s="40"/>
       <c r="P14" s="29"/>
       <c r="Q14" s="29"/>
@@ -7829,57 +7845,57 @@
       <c r="V14" s="29"/>
       <c r="W14" s="29"/>
       <c r="AX14" s="42"/>
-      <c r="AY14" s="259"/>
-      <c r="BD14" s="267" t="s">
+      <c r="AY14" s="291"/>
+      <c r="BD14" s="287" t="s">
         <v>338</v>
       </c>
-      <c r="BE14" s="268"/>
-      <c r="BF14" s="268"/>
-      <c r="BG14" s="268"/>
-      <c r="BH14" s="268"/>
-      <c r="BI14" s="268"/>
-      <c r="BJ14" s="268"/>
-      <c r="BK14" s="269"/>
-      <c r="BP14" s="267" t="s">
+      <c r="BE14" s="288"/>
+      <c r="BF14" s="288"/>
+      <c r="BG14" s="288"/>
+      <c r="BH14" s="288"/>
+      <c r="BI14" s="288"/>
+      <c r="BJ14" s="288"/>
+      <c r="BK14" s="289"/>
+      <c r="BP14" s="287" t="s">
         <v>327</v>
       </c>
-      <c r="BQ14" s="268"/>
-      <c r="BR14" s="268"/>
-      <c r="BS14" s="268"/>
-      <c r="BT14" s="268"/>
-      <c r="BU14" s="268"/>
-      <c r="BV14" s="268"/>
-      <c r="BW14" s="269"/>
-      <c r="CA14" s="267" t="s">
+      <c r="BQ14" s="288"/>
+      <c r="BR14" s="288"/>
+      <c r="BS14" s="288"/>
+      <c r="BT14" s="288"/>
+      <c r="BU14" s="288"/>
+      <c r="BV14" s="288"/>
+      <c r="BW14" s="289"/>
+      <c r="CA14" s="287" t="s">
         <v>326</v>
       </c>
-      <c r="CB14" s="268"/>
-      <c r="CC14" s="268"/>
-      <c r="CD14" s="268"/>
-      <c r="CE14" s="268"/>
-      <c r="CF14" s="268"/>
-      <c r="CG14" s="268"/>
-      <c r="CH14" s="269"/>
-      <c r="CL14" s="267" t="s">
+      <c r="CB14" s="288"/>
+      <c r="CC14" s="288"/>
+      <c r="CD14" s="288"/>
+      <c r="CE14" s="288"/>
+      <c r="CF14" s="288"/>
+      <c r="CG14" s="288"/>
+      <c r="CH14" s="289"/>
+      <c r="CL14" s="287" t="s">
         <v>329</v>
       </c>
-      <c r="CM14" s="268"/>
-      <c r="CN14" s="268"/>
-      <c r="CO14" s="268"/>
-      <c r="CP14" s="268"/>
-      <c r="CQ14" s="268"/>
-      <c r="CR14" s="268"/>
-      <c r="CS14" s="269"/>
-      <c r="CV14" s="267" t="s">
+      <c r="CM14" s="288"/>
+      <c r="CN14" s="288"/>
+      <c r="CO14" s="288"/>
+      <c r="CP14" s="288"/>
+      <c r="CQ14" s="288"/>
+      <c r="CR14" s="288"/>
+      <c r="CS14" s="289"/>
+      <c r="CV14" s="287" t="s">
         <v>328</v>
       </c>
-      <c r="CW14" s="268"/>
-      <c r="CX14" s="268"/>
-      <c r="CY14" s="268"/>
-      <c r="CZ14" s="268"/>
-      <c r="DA14" s="268"/>
-      <c r="DB14" s="268"/>
-      <c r="DC14" s="269"/>
+      <c r="CW14" s="288"/>
+      <c r="CX14" s="288"/>
+      <c r="CY14" s="288"/>
+      <c r="CZ14" s="288"/>
+      <c r="DA14" s="288"/>
+      <c r="DB14" s="288"/>
+      <c r="DC14" s="289"/>
     </row>
     <row r="15" spans="1:107" thickBot="1">
       <c r="G15" s="117"/>
@@ -7900,7 +7916,7 @@
       <c r="V15" s="29"/>
       <c r="W15" s="29"/>
       <c r="AX15" s="42"/>
-      <c r="AY15" s="259"/>
+      <c r="AY15" s="291"/>
       <c r="BD15" s="117"/>
       <c r="BE15" s="116"/>
       <c r="BF15" s="114"/>
@@ -7961,7 +7977,7 @@
       <c r="V16" s="29"/>
       <c r="W16" s="29"/>
       <c r="AX16" s="42"/>
-      <c r="AY16" s="259"/>
+      <c r="AY16" s="291"/>
       <c r="BD16" s="40"/>
       <c r="BE16" s="29"/>
       <c r="BF16" s="29"/>
@@ -8013,16 +8029,16 @@
       <c r="M17" s="29"/>
       <c r="N17" s="29"/>
       <c r="O17" s="40"/>
-      <c r="P17" s="270"/>
+      <c r="P17" s="293"/>
       <c r="Q17" s="246"/>
       <c r="R17" s="246"/>
       <c r="S17" s="29"/>
-      <c r="T17" s="270"/>
+      <c r="T17" s="293"/>
       <c r="U17" s="246"/>
       <c r="V17" s="246"/>
       <c r="W17" s="246"/>
       <c r="AX17" s="42"/>
-      <c r="AY17" s="259"/>
+      <c r="AY17" s="291"/>
       <c r="BD17" s="40"/>
       <c r="BE17" s="29"/>
       <c r="BF17" s="29"/>
@@ -8040,14 +8056,14 @@
       <c r="BV17" s="29"/>
       <c r="BW17" s="46"/>
       <c r="CA17" s="40"/>
-      <c r="CB17" s="271" t="s">
+      <c r="CB17" s="255" t="s">
         <v>349</v>
       </c>
-      <c r="CC17" s="256"/>
-      <c r="CD17" s="256"/>
-      <c r="CE17" s="256"/>
-      <c r="CF17" s="256"/>
-      <c r="CG17" s="257"/>
+      <c r="CC17" s="258"/>
+      <c r="CD17" s="258"/>
+      <c r="CE17" s="258"/>
+      <c r="CF17" s="258"/>
+      <c r="CG17" s="259"/>
       <c r="CH17" s="46"/>
       <c r="CL17" s="40"/>
       <c r="CM17" s="29"/>
@@ -8070,96 +8086,96 @@
       <c r="G18" s="41"/>
       <c r="O18" s="41"/>
       <c r="AX18" s="42"/>
-      <c r="AY18" s="259"/>
+      <c r="AY18" s="291"/>
       <c r="BD18" s="41"/>
-      <c r="BE18" s="255" t="s">
+      <c r="BE18" s="269" t="s">
         <v>335</v>
       </c>
-      <c r="BF18" s="256"/>
-      <c r="BG18" s="256"/>
-      <c r="BH18" s="256"/>
-      <c r="BI18" s="256"/>
-      <c r="BJ18" s="257"/>
+      <c r="BF18" s="258"/>
+      <c r="BG18" s="258"/>
+      <c r="BH18" s="258"/>
+      <c r="BI18" s="258"/>
+      <c r="BJ18" s="259"/>
       <c r="BK18" s="42"/>
       <c r="BP18" s="41"/>
-      <c r="BQ18" s="255" t="s">
+      <c r="BQ18" s="269" t="s">
         <v>331</v>
       </c>
-      <c r="BR18" s="256"/>
-      <c r="BS18" s="256"/>
-      <c r="BT18" s="256"/>
-      <c r="BU18" s="256"/>
-      <c r="BV18" s="257"/>
+      <c r="BR18" s="258"/>
+      <c r="BS18" s="258"/>
+      <c r="BT18" s="258"/>
+      <c r="BU18" s="258"/>
+      <c r="BV18" s="259"/>
       <c r="BW18" s="42"/>
       <c r="CA18" s="41"/>
-      <c r="CB18" s="272" t="s">
+      <c r="CB18" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="CC18" s="273"/>
-      <c r="CD18" s="255"/>
-      <c r="CE18" s="257"/>
-      <c r="CF18" s="272" t="s">
+      <c r="CC18" s="271"/>
+      <c r="CD18" s="269"/>
+      <c r="CE18" s="259"/>
+      <c r="CF18" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="CG18" s="273"/>
+      <c r="CG18" s="271"/>
       <c r="CH18" s="42"/>
       <c r="CL18" s="41"/>
-      <c r="CM18" s="271" t="s">
+      <c r="CM18" s="255" t="s">
         <v>354</v>
       </c>
-      <c r="CN18" s="256"/>
-      <c r="CO18" s="256"/>
-      <c r="CP18" s="256"/>
-      <c r="CQ18" s="256"/>
-      <c r="CR18" s="257"/>
+      <c r="CN18" s="258"/>
+      <c r="CO18" s="258"/>
+      <c r="CP18" s="258"/>
+      <c r="CQ18" s="258"/>
+      <c r="CR18" s="259"/>
       <c r="CS18" s="42"/>
       <c r="CV18" s="41"/>
-      <c r="CW18" s="271" t="s">
+      <c r="CW18" s="255" t="s">
         <v>359</v>
       </c>
-      <c r="CX18" s="256"/>
-      <c r="CY18" s="256"/>
-      <c r="CZ18" s="256"/>
-      <c r="DA18" s="256"/>
-      <c r="DB18" s="257"/>
+      <c r="CX18" s="258"/>
+      <c r="CY18" s="258"/>
+      <c r="CZ18" s="258"/>
+      <c r="DA18" s="258"/>
+      <c r="DB18" s="259"/>
       <c r="DC18" s="42"/>
     </row>
     <row r="19" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G19" s="41"/>
       <c r="O19" s="41"/>
       <c r="AX19" s="42"/>
-      <c r="AY19" s="259"/>
+      <c r="AY19" s="291"/>
       <c r="BD19" s="41"/>
-      <c r="BE19" s="255" t="s">
+      <c r="BE19" s="269" t="s">
         <v>336</v>
       </c>
-      <c r="BF19" s="256"/>
-      <c r="BG19" s="256"/>
-      <c r="BH19" s="256"/>
-      <c r="BI19" s="256"/>
-      <c r="BJ19" s="257"/>
+      <c r="BF19" s="258"/>
+      <c r="BG19" s="258"/>
+      <c r="BH19" s="258"/>
+      <c r="BI19" s="258"/>
+      <c r="BJ19" s="259"/>
       <c r="BK19" s="42"/>
       <c r="BP19" s="41"/>
-      <c r="BQ19" s="255" t="s">
+      <c r="BQ19" s="269" t="s">
         <v>330</v>
       </c>
-      <c r="BR19" s="256"/>
-      <c r="BS19" s="256"/>
-      <c r="BT19" s="256"/>
-      <c r="BU19" s="256"/>
-      <c r="BV19" s="257"/>
+      <c r="BR19" s="258"/>
+      <c r="BS19" s="258"/>
+      <c r="BT19" s="258"/>
+      <c r="BU19" s="258"/>
+      <c r="BV19" s="259"/>
       <c r="BW19" s="42"/>
       <c r="CA19" s="41"/>
       <c r="CH19" s="42"/>
       <c r="CL19" s="41"/>
-      <c r="CM19" s="271" t="s">
+      <c r="CM19" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN19" s="256"/>
-      <c r="CO19" s="256"/>
-      <c r="CP19" s="256"/>
-      <c r="CQ19" s="256"/>
-      <c r="CR19" s="257"/>
+      <c r="CN19" s="258"/>
+      <c r="CO19" s="258"/>
+      <c r="CP19" s="258"/>
+      <c r="CQ19" s="258"/>
+      <c r="CR19" s="259"/>
       <c r="CS19" s="42"/>
       <c r="CV19" s="41"/>
       <c r="DC19" s="42"/>
@@ -8168,114 +8184,114 @@
       <c r="G20" s="41"/>
       <c r="O20" s="41"/>
       <c r="AX20" s="42"/>
-      <c r="AY20" s="259"/>
+      <c r="AY20" s="291"/>
       <c r="BD20" s="41"/>
       <c r="BK20" s="42"/>
       <c r="BP20" s="41"/>
       <c r="BW20" s="42"/>
       <c r="CA20" s="41"/>
-      <c r="CB20" s="271" t="s">
+      <c r="CB20" s="255" t="s">
         <v>350</v>
       </c>
-      <c r="CC20" s="256"/>
-      <c r="CD20" s="256"/>
-      <c r="CE20" s="256"/>
-      <c r="CF20" s="256"/>
-      <c r="CG20" s="257"/>
+      <c r="CC20" s="258"/>
+      <c r="CD20" s="258"/>
+      <c r="CE20" s="258"/>
+      <c r="CF20" s="258"/>
+      <c r="CG20" s="259"/>
       <c r="CH20" s="42"/>
       <c r="CL20" s="41"/>
       <c r="CS20" s="42"/>
       <c r="CV20" s="41"/>
-      <c r="CW20" s="271" t="s">
+      <c r="CW20" s="255" t="s">
         <v>360</v>
       </c>
-      <c r="CX20" s="256"/>
-      <c r="CY20" s="256"/>
-      <c r="CZ20" s="256"/>
-      <c r="DA20" s="256"/>
-      <c r="DB20" s="257"/>
+      <c r="CX20" s="258"/>
+      <c r="CY20" s="258"/>
+      <c r="CZ20" s="258"/>
+      <c r="DA20" s="258"/>
+      <c r="DB20" s="259"/>
       <c r="DC20" s="42"/>
     </row>
     <row r="21" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G21" s="41"/>
       <c r="O21" s="41"/>
       <c r="AX21" s="42"/>
-      <c r="AY21" s="259"/>
+      <c r="AY21" s="291"/>
       <c r="BD21" s="41"/>
-      <c r="BE21" s="255" t="s">
+      <c r="BE21" s="269" t="s">
         <v>337</v>
       </c>
-      <c r="BF21" s="256"/>
-      <c r="BG21" s="256"/>
-      <c r="BH21" s="256"/>
-      <c r="BI21" s="256"/>
-      <c r="BJ21" s="257"/>
+      <c r="BF21" s="258"/>
+      <c r="BG21" s="258"/>
+      <c r="BH21" s="258"/>
+      <c r="BI21" s="258"/>
+      <c r="BJ21" s="259"/>
       <c r="BK21" s="42"/>
       <c r="BP21" s="41"/>
-      <c r="BQ21" s="255" t="s">
+      <c r="BQ21" s="269" t="s">
         <v>332</v>
       </c>
-      <c r="BR21" s="256"/>
-      <c r="BS21" s="256"/>
-      <c r="BT21" s="256"/>
-      <c r="BU21" s="256"/>
-      <c r="BV21" s="257"/>
+      <c r="BR21" s="258"/>
+      <c r="BS21" s="258"/>
+      <c r="BT21" s="258"/>
+      <c r="BU21" s="258"/>
+      <c r="BV21" s="259"/>
       <c r="BW21" s="42"/>
       <c r="CA21" s="41"/>
-      <c r="CB21" s="271" t="s">
+      <c r="CB21" s="255" t="s">
         <v>336</v>
       </c>
-      <c r="CC21" s="256"/>
-      <c r="CD21" s="256"/>
-      <c r="CE21" s="256"/>
-      <c r="CF21" s="256"/>
-      <c r="CG21" s="257"/>
+      <c r="CC21" s="258"/>
+      <c r="CD21" s="258"/>
+      <c r="CE21" s="258"/>
+      <c r="CF21" s="258"/>
+      <c r="CG21" s="259"/>
       <c r="CH21" s="42"/>
       <c r="CL21" s="41"/>
-      <c r="CM21" s="271" t="s">
+      <c r="CM21" s="255" t="s">
         <v>356</v>
       </c>
-      <c r="CN21" s="256"/>
-      <c r="CO21" s="256"/>
-      <c r="CP21" s="256"/>
-      <c r="CQ21" s="256"/>
-      <c r="CR21" s="257"/>
+      <c r="CN21" s="258"/>
+      <c r="CO21" s="258"/>
+      <c r="CP21" s="258"/>
+      <c r="CQ21" s="258"/>
+      <c r="CR21" s="259"/>
       <c r="CS21" s="42"/>
       <c r="CV21" s="41"/>
-      <c r="CW21" s="271" t="s">
+      <c r="CW21" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CX21" s="256"/>
-      <c r="CY21" s="256"/>
-      <c r="CZ21" s="256"/>
-      <c r="DA21" s="256"/>
-      <c r="DB21" s="257"/>
+      <c r="CX21" s="258"/>
+      <c r="CY21" s="258"/>
+      <c r="CZ21" s="258"/>
+      <c r="DA21" s="258"/>
+      <c r="DB21" s="259"/>
       <c r="DC21" s="42"/>
     </row>
     <row r="22" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G22" s="41"/>
       <c r="O22" s="41"/>
       <c r="AX22" s="42"/>
-      <c r="AY22" s="259"/>
+      <c r="AY22" s="291"/>
       <c r="BD22" s="41"/>
-      <c r="BE22" s="255" t="s">
+      <c r="BE22" s="269" t="s">
         <v>336</v>
       </c>
-      <c r="BF22" s="256"/>
-      <c r="BG22" s="256"/>
-      <c r="BH22" s="256"/>
-      <c r="BI22" s="256"/>
-      <c r="BJ22" s="257"/>
+      <c r="BF22" s="258"/>
+      <c r="BG22" s="258"/>
+      <c r="BH22" s="258"/>
+      <c r="BI22" s="258"/>
+      <c r="BJ22" s="259"/>
       <c r="BK22" s="42"/>
       <c r="BP22" s="41"/>
-      <c r="BQ22" s="255" t="s">
+      <c r="BQ22" s="269" t="s">
         <v>330</v>
       </c>
-      <c r="BR22" s="256"/>
-      <c r="BS22" s="256"/>
-      <c r="BT22" s="256"/>
-      <c r="BU22" s="256"/>
-      <c r="BV22" s="257"/>
+      <c r="BR22" s="258"/>
+      <c r="BS22" s="258"/>
+      <c r="BT22" s="258"/>
+      <c r="BU22" s="258"/>
+      <c r="BV22" s="259"/>
       <c r="BW22" s="42"/>
       <c r="CA22" s="41"/>
       <c r="CH22" s="42"/>
@@ -8288,7 +8304,7 @@
       <c r="G23" s="41"/>
       <c r="O23" s="41"/>
       <c r="AX23" s="42"/>
-      <c r="AY23" s="259"/>
+      <c r="AY23" s="291"/>
       <c r="BD23" s="41"/>
       <c r="BK23" s="42"/>
       <c r="BP23" s="41"/>
@@ -8297,57 +8313,57 @@
       <c r="CB23" s="29"/>
       <c r="CC23" s="29"/>
       <c r="CD23" s="29"/>
-      <c r="CE23" s="282" t="s">
+      <c r="CE23" s="278" t="s">
         <v>348</v>
       </c>
-      <c r="CF23" s="283"/>
-      <c r="CG23" s="283"/>
-      <c r="CH23" s="284"/>
+      <c r="CF23" s="279"/>
+      <c r="CG23" s="279"/>
+      <c r="CH23" s="280"/>
       <c r="CL23" s="41"/>
-      <c r="CM23" s="271" t="s">
+      <c r="CM23" s="255" t="s">
         <v>357</v>
       </c>
-      <c r="CN23" s="256"/>
-      <c r="CO23" s="256"/>
-      <c r="CP23" s="256"/>
-      <c r="CQ23" s="256"/>
-      <c r="CR23" s="257"/>
+      <c r="CN23" s="258"/>
+      <c r="CO23" s="258"/>
+      <c r="CP23" s="258"/>
+      <c r="CQ23" s="258"/>
+      <c r="CR23" s="259"/>
       <c r="CS23" s="42"/>
       <c r="CV23" s="41"/>
-      <c r="CW23" s="271" t="s">
+      <c r="CW23" s="255" t="s">
         <v>361</v>
       </c>
-      <c r="CX23" s="256"/>
-      <c r="CY23" s="256"/>
-      <c r="CZ23" s="256"/>
-      <c r="DA23" s="256"/>
-      <c r="DB23" s="257"/>
+      <c r="CX23" s="258"/>
+      <c r="CY23" s="258"/>
+      <c r="CZ23" s="258"/>
+      <c r="DA23" s="258"/>
+      <c r="DB23" s="259"/>
       <c r="DC23" s="42"/>
     </row>
     <row r="24" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G24" s="41"/>
       <c r="O24" s="41"/>
       <c r="AX24" s="42"/>
-      <c r="AY24" s="259"/>
+      <c r="AY24" s="291"/>
       <c r="BD24" s="41"/>
-      <c r="BE24" s="255" t="s">
+      <c r="BE24" s="269" t="s">
         <v>339</v>
       </c>
-      <c r="BF24" s="256"/>
-      <c r="BG24" s="256"/>
-      <c r="BH24" s="256"/>
-      <c r="BI24" s="256"/>
-      <c r="BJ24" s="257"/>
+      <c r="BF24" s="258"/>
+      <c r="BG24" s="258"/>
+      <c r="BH24" s="258"/>
+      <c r="BI24" s="258"/>
+      <c r="BJ24" s="259"/>
       <c r="BK24" s="42"/>
       <c r="BP24" s="41"/>
-      <c r="BQ24" s="255" t="s">
+      <c r="BQ24" s="269" t="s">
         <v>333</v>
       </c>
-      <c r="BR24" s="256"/>
-      <c r="BS24" s="256"/>
-      <c r="BT24" s="256"/>
-      <c r="BU24" s="256"/>
-      <c r="BV24" s="257"/>
+      <c r="BR24" s="258"/>
+      <c r="BS24" s="258"/>
+      <c r="BT24" s="258"/>
+      <c r="BU24" s="258"/>
+      <c r="BV24" s="259"/>
       <c r="BW24" s="42"/>
       <c r="CA24" s="40"/>
       <c r="CB24" s="29"/>
@@ -8358,60 +8374,60 @@
       <c r="CG24" s="29"/>
       <c r="CH24" s="46"/>
       <c r="CL24" s="41"/>
-      <c r="CM24" s="271" t="s">
+      <c r="CM24" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN24" s="256"/>
-      <c r="CO24" s="256"/>
-      <c r="CP24" s="256"/>
-      <c r="CQ24" s="256"/>
-      <c r="CR24" s="257"/>
+      <c r="CN24" s="258"/>
+      <c r="CO24" s="258"/>
+      <c r="CP24" s="258"/>
+      <c r="CQ24" s="258"/>
+      <c r="CR24" s="259"/>
       <c r="CS24" s="42"/>
       <c r="CV24" s="41"/>
-      <c r="CW24" s="271" t="s">
+      <c r="CW24" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CX24" s="256"/>
-      <c r="CY24" s="256"/>
-      <c r="CZ24" s="256"/>
-      <c r="DA24" s="256"/>
-      <c r="DB24" s="257"/>
+      <c r="CX24" s="258"/>
+      <c r="CY24" s="258"/>
+      <c r="CZ24" s="258"/>
+      <c r="DA24" s="258"/>
+      <c r="DB24" s="259"/>
       <c r="DC24" s="42"/>
     </row>
     <row r="25" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G25" s="41"/>
       <c r="O25" s="41"/>
       <c r="AX25" s="42"/>
-      <c r="AY25" s="259"/>
+      <c r="AY25" s="291"/>
       <c r="BD25" s="41"/>
-      <c r="BE25" s="255" t="s">
+      <c r="BE25" s="269" t="s">
         <v>336</v>
       </c>
-      <c r="BF25" s="256"/>
-      <c r="BG25" s="256"/>
-      <c r="BH25" s="256"/>
-      <c r="BI25" s="256"/>
-      <c r="BJ25" s="257"/>
+      <c r="BF25" s="258"/>
+      <c r="BG25" s="258"/>
+      <c r="BH25" s="258"/>
+      <c r="BI25" s="258"/>
+      <c r="BJ25" s="259"/>
       <c r="BK25" s="42"/>
       <c r="BP25" s="41"/>
-      <c r="BQ25" s="255" t="s">
+      <c r="BQ25" s="269" t="s">
         <v>330</v>
       </c>
-      <c r="BR25" s="256"/>
-      <c r="BS25" s="256"/>
-      <c r="BT25" s="256"/>
-      <c r="BU25" s="256"/>
-      <c r="BV25" s="257"/>
+      <c r="BR25" s="258"/>
+      <c r="BS25" s="258"/>
+      <c r="BT25" s="258"/>
+      <c r="BU25" s="258"/>
+      <c r="BV25" s="259"/>
       <c r="BW25" s="42"/>
       <c r="CA25" s="41"/>
-      <c r="CB25" s="271" t="s">
+      <c r="CB25" s="255" t="s">
         <v>343</v>
       </c>
-      <c r="CC25" s="280"/>
-      <c r="CD25" s="280"/>
-      <c r="CE25" s="280"/>
-      <c r="CF25" s="280"/>
-      <c r="CG25" s="281"/>
+      <c r="CC25" s="256"/>
+      <c r="CD25" s="256"/>
+      <c r="CE25" s="256"/>
+      <c r="CF25" s="256"/>
+      <c r="CG25" s="257"/>
       <c r="CH25" s="42"/>
       <c r="CL25" s="41"/>
       <c r="CS25" s="42"/>
@@ -8422,128 +8438,128 @@
       <c r="G26" s="41"/>
       <c r="O26" s="41"/>
       <c r="AX26" s="42"/>
-      <c r="AY26" s="259"/>
+      <c r="AY26" s="291"/>
       <c r="BD26" s="41"/>
       <c r="BK26" s="42"/>
       <c r="BP26" s="41"/>
       <c r="BW26" s="42"/>
       <c r="CA26" s="41"/>
-      <c r="CB26" s="272" t="s">
+      <c r="CB26" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="CC26" s="273"/>
-      <c r="CD26" s="255"/>
-      <c r="CE26" s="257"/>
-      <c r="CF26" s="272" t="s">
+      <c r="CC26" s="271"/>
+      <c r="CD26" s="269"/>
+      <c r="CE26" s="259"/>
+      <c r="CF26" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="CG26" s="273"/>
+      <c r="CG26" s="271"/>
       <c r="CH26" s="42"/>
       <c r="CL26" s="41"/>
-      <c r="CM26" s="255" t="s">
+      <c r="CM26" s="269" t="s">
         <v>331</v>
       </c>
-      <c r="CN26" s="256"/>
-      <c r="CO26" s="256"/>
-      <c r="CP26" s="256"/>
-      <c r="CQ26" s="256"/>
-      <c r="CR26" s="257"/>
+      <c r="CN26" s="258"/>
+      <c r="CO26" s="258"/>
+      <c r="CP26" s="258"/>
+      <c r="CQ26" s="258"/>
+      <c r="CR26" s="259"/>
       <c r="CS26" s="42"/>
       <c r="CV26" s="41"/>
-      <c r="CW26" s="271" t="s">
+      <c r="CW26" s="255" t="s">
         <v>362</v>
       </c>
-      <c r="CX26" s="256"/>
-      <c r="CY26" s="256"/>
-      <c r="CZ26" s="256"/>
-      <c r="DA26" s="256"/>
-      <c r="DB26" s="257"/>
+      <c r="CX26" s="258"/>
+      <c r="CY26" s="258"/>
+      <c r="CZ26" s="258"/>
+      <c r="DA26" s="258"/>
+      <c r="DB26" s="259"/>
       <c r="DC26" s="42"/>
     </row>
     <row r="27" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G27" s="41"/>
       <c r="O27" s="41"/>
       <c r="AX27" s="42"/>
-      <c r="AY27" s="259"/>
+      <c r="AY27" s="291"/>
       <c r="BD27" s="41"/>
-      <c r="BE27" s="255" t="s">
+      <c r="BE27" s="269" t="s">
         <v>340</v>
       </c>
-      <c r="BF27" s="256"/>
-      <c r="BG27" s="256"/>
-      <c r="BH27" s="256"/>
-      <c r="BI27" s="256"/>
-      <c r="BJ27" s="257"/>
+      <c r="BF27" s="258"/>
+      <c r="BG27" s="258"/>
+      <c r="BH27" s="258"/>
+      <c r="BI27" s="258"/>
+      <c r="BJ27" s="259"/>
       <c r="BK27" s="42"/>
       <c r="BP27" s="41"/>
-      <c r="BQ27" s="255" t="s">
+      <c r="BQ27" s="269" t="s">
         <v>334</v>
       </c>
-      <c r="BR27" s="256"/>
-      <c r="BS27" s="256"/>
-      <c r="BT27" s="256"/>
-      <c r="BU27" s="256"/>
-      <c r="BV27" s="257"/>
+      <c r="BR27" s="258"/>
+      <c r="BS27" s="258"/>
+      <c r="BT27" s="258"/>
+      <c r="BU27" s="258"/>
+      <c r="BV27" s="259"/>
       <c r="BW27" s="42"/>
       <c r="CA27" s="41"/>
       <c r="CH27" s="42"/>
       <c r="CL27" s="41"/>
-      <c r="CM27" s="271" t="s">
+      <c r="CM27" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN27" s="256"/>
-      <c r="CO27" s="256"/>
-      <c r="CP27" s="256"/>
-      <c r="CQ27" s="256"/>
-      <c r="CR27" s="257"/>
+      <c r="CN27" s="258"/>
+      <c r="CO27" s="258"/>
+      <c r="CP27" s="258"/>
+      <c r="CQ27" s="258"/>
+      <c r="CR27" s="259"/>
       <c r="CS27" s="42"/>
       <c r="CV27" s="41"/>
-      <c r="CW27" s="271" t="s">
+      <c r="CW27" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CX27" s="256"/>
-      <c r="CY27" s="256"/>
-      <c r="CZ27" s="256"/>
-      <c r="DA27" s="256"/>
-      <c r="DB27" s="257"/>
+      <c r="CX27" s="258"/>
+      <c r="CY27" s="258"/>
+      <c r="CZ27" s="258"/>
+      <c r="DA27" s="258"/>
+      <c r="DB27" s="259"/>
       <c r="DC27" s="42"/>
     </row>
     <row r="28" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G28" s="41"/>
       <c r="O28" s="41"/>
       <c r="AX28" s="42"/>
-      <c r="AY28" s="259"/>
+      <c r="AY28" s="291"/>
       <c r="BD28" s="119"/>
-      <c r="BE28" s="272" t="s">
+      <c r="BE28" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="BF28" s="273"/>
-      <c r="BG28" s="255"/>
-      <c r="BH28" s="257"/>
-      <c r="BI28" s="272" t="s">
+      <c r="BF28" s="271"/>
+      <c r="BG28" s="269"/>
+      <c r="BH28" s="259"/>
+      <c r="BI28" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="BJ28" s="273"/>
+      <c r="BJ28" s="271"/>
       <c r="BK28" s="42"/>
       <c r="BP28" s="41"/>
-      <c r="BQ28" s="255" t="s">
+      <c r="BQ28" s="269" t="s">
         <v>330</v>
       </c>
-      <c r="BR28" s="256"/>
-      <c r="BS28" s="256"/>
-      <c r="BT28" s="256"/>
-      <c r="BU28" s="256"/>
-      <c r="BV28" s="257"/>
+      <c r="BR28" s="258"/>
+      <c r="BS28" s="258"/>
+      <c r="BT28" s="258"/>
+      <c r="BU28" s="258"/>
+      <c r="BV28" s="259"/>
       <c r="BW28" s="42"/>
       <c r="CA28" s="41"/>
-      <c r="CB28" s="271" t="s">
+      <c r="CB28" s="255" t="s">
         <v>344</v>
       </c>
-      <c r="CC28" s="280"/>
-      <c r="CD28" s="280"/>
-      <c r="CE28" s="280"/>
-      <c r="CF28" s="280"/>
-      <c r="CG28" s="281"/>
+      <c r="CC28" s="256"/>
+      <c r="CD28" s="256"/>
+      <c r="CE28" s="256"/>
+      <c r="CF28" s="256"/>
+      <c r="CG28" s="257"/>
       <c r="CH28" s="42"/>
       <c r="CL28" s="41"/>
       <c r="CS28" s="42"/>
@@ -8554,49 +8570,49 @@
       <c r="G29" s="41"/>
       <c r="O29" s="41"/>
       <c r="AX29" s="42"/>
-      <c r="AY29" s="259"/>
+      <c r="AY29" s="291"/>
       <c r="BD29" s="41"/>
       <c r="BK29" s="42"/>
       <c r="BP29" s="41"/>
       <c r="BW29" s="42"/>
       <c r="CA29" s="41"/>
-      <c r="CB29" s="272" t="s">
+      <c r="CB29" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="CC29" s="273"/>
-      <c r="CD29" s="255"/>
-      <c r="CE29" s="257"/>
-      <c r="CF29" s="272" t="s">
+      <c r="CC29" s="271"/>
+      <c r="CD29" s="269"/>
+      <c r="CE29" s="259"/>
+      <c r="CF29" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="CG29" s="273"/>
+      <c r="CG29" s="271"/>
       <c r="CH29" s="42"/>
       <c r="CL29" s="41"/>
-      <c r="CM29" s="255" t="s">
+      <c r="CM29" s="269" t="s">
         <v>332</v>
       </c>
-      <c r="CN29" s="256"/>
-      <c r="CO29" s="256"/>
-      <c r="CP29" s="256"/>
-      <c r="CQ29" s="256"/>
-      <c r="CR29" s="257"/>
+      <c r="CN29" s="258"/>
+      <c r="CO29" s="258"/>
+      <c r="CP29" s="258"/>
+      <c r="CQ29" s="258"/>
+      <c r="CR29" s="259"/>
       <c r="CS29" s="42"/>
       <c r="CV29" s="41"/>
-      <c r="CW29" s="271" t="s">
+      <c r="CW29" s="255" t="s">
         <v>363</v>
       </c>
-      <c r="CX29" s="256"/>
-      <c r="CY29" s="256"/>
-      <c r="CZ29" s="256"/>
-      <c r="DA29" s="256"/>
-      <c r="DB29" s="257"/>
+      <c r="CX29" s="258"/>
+      <c r="CY29" s="258"/>
+      <c r="CZ29" s="258"/>
+      <c r="DA29" s="258"/>
+      <c r="DB29" s="259"/>
       <c r="DC29" s="42"/>
     </row>
     <row r="30" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G30" s="41"/>
       <c r="O30" s="41"/>
       <c r="AX30" s="42"/>
-      <c r="AY30" s="259"/>
+      <c r="AY30" s="291"/>
       <c r="BD30" s="41"/>
       <c r="BK30" s="42"/>
       <c r="BP30" s="41"/>
@@ -8604,44 +8620,44 @@
       <c r="CA30" s="41"/>
       <c r="CH30" s="42"/>
       <c r="CL30" s="41"/>
-      <c r="CM30" s="271" t="s">
+      <c r="CM30" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN30" s="256"/>
-      <c r="CO30" s="256"/>
-      <c r="CP30" s="256"/>
-      <c r="CQ30" s="256"/>
-      <c r="CR30" s="257"/>
+      <c r="CN30" s="258"/>
+      <c r="CO30" s="258"/>
+      <c r="CP30" s="258"/>
+      <c r="CQ30" s="258"/>
+      <c r="CR30" s="259"/>
       <c r="CS30" s="42"/>
       <c r="CV30" s="41"/>
-      <c r="CW30" s="271" t="s">
+      <c r="CW30" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CX30" s="280"/>
-      <c r="CY30" s="280"/>
-      <c r="CZ30" s="280"/>
-      <c r="DA30" s="280"/>
-      <c r="DB30" s="281"/>
+      <c r="CX30" s="256"/>
+      <c r="CY30" s="256"/>
+      <c r="CZ30" s="256"/>
+      <c r="DA30" s="256"/>
+      <c r="DB30" s="257"/>
       <c r="DC30" s="42"/>
     </row>
     <row r="31" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G31" s="41"/>
       <c r="O31" s="41"/>
       <c r="AX31" s="42"/>
-      <c r="AY31" s="259"/>
+      <c r="AY31" s="291"/>
       <c r="BD31" s="41"/>
       <c r="BK31" s="42"/>
       <c r="BP31" s="41"/>
       <c r="BW31" s="42"/>
       <c r="CA31" s="41"/>
-      <c r="CB31" s="271" t="s">
+      <c r="CB31" s="255" t="s">
         <v>345</v>
       </c>
-      <c r="CC31" s="280"/>
-      <c r="CD31" s="280"/>
-      <c r="CE31" s="280"/>
-      <c r="CF31" s="280"/>
-      <c r="CG31" s="281"/>
+      <c r="CC31" s="256"/>
+      <c r="CD31" s="256"/>
+      <c r="CE31" s="256"/>
+      <c r="CF31" s="256"/>
+      <c r="CG31" s="257"/>
       <c r="CH31" s="42"/>
       <c r="CL31" s="41"/>
       <c r="CS31" s="42"/>
@@ -8652,122 +8668,122 @@
       <c r="G32" s="41"/>
       <c r="O32" s="41"/>
       <c r="AX32" s="42"/>
-      <c r="AY32" s="259"/>
+      <c r="AY32" s="291"/>
       <c r="BD32" s="41"/>
-      <c r="BE32" s="274" t="s">
+      <c r="BE32" s="272" t="s">
         <v>277</v>
       </c>
-      <c r="BF32" s="275"/>
-      <c r="BG32" s="275"/>
-      <c r="BH32" s="275"/>
-      <c r="BI32" s="275"/>
-      <c r="BJ32" s="276"/>
+      <c r="BF32" s="273"/>
+      <c r="BG32" s="273"/>
+      <c r="BH32" s="273"/>
+      <c r="BI32" s="273"/>
+      <c r="BJ32" s="274"/>
       <c r="BK32" s="42"/>
       <c r="BP32" s="41"/>
-      <c r="BQ32" s="274" t="s">
+      <c r="BQ32" s="272" t="s">
         <v>352</v>
       </c>
-      <c r="BR32" s="275"/>
-      <c r="BS32" s="275"/>
-      <c r="BT32" s="275"/>
-      <c r="BU32" s="275"/>
-      <c r="BV32" s="276"/>
+      <c r="BR32" s="273"/>
+      <c r="BS32" s="273"/>
+      <c r="BT32" s="273"/>
+      <c r="BU32" s="273"/>
+      <c r="BV32" s="274"/>
       <c r="BW32" s="42"/>
       <c r="CA32" s="41"/>
-      <c r="CB32" s="272" t="s">
+      <c r="CB32" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="CC32" s="273"/>
-      <c r="CD32" s="255"/>
-      <c r="CE32" s="257"/>
-      <c r="CF32" s="272" t="s">
+      <c r="CC32" s="271"/>
+      <c r="CD32" s="269"/>
+      <c r="CE32" s="259"/>
+      <c r="CF32" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="CG32" s="273"/>
+      <c r="CG32" s="271"/>
       <c r="CH32" s="42"/>
       <c r="CL32" s="41"/>
-      <c r="CM32" s="255" t="s">
+      <c r="CM32" s="269" t="s">
         <v>333</v>
       </c>
-      <c r="CN32" s="256"/>
-      <c r="CO32" s="256"/>
-      <c r="CP32" s="256"/>
-      <c r="CQ32" s="256"/>
-      <c r="CR32" s="257"/>
+      <c r="CN32" s="258"/>
+      <c r="CO32" s="258"/>
+      <c r="CP32" s="258"/>
+      <c r="CQ32" s="258"/>
+      <c r="CR32" s="259"/>
       <c r="CS32" s="42"/>
       <c r="CV32" s="41"/>
-      <c r="CW32" s="271" t="s">
+      <c r="CW32" s="255" t="s">
         <v>364</v>
       </c>
-      <c r="CX32" s="256"/>
-      <c r="CY32" s="256"/>
-      <c r="CZ32" s="256"/>
-      <c r="DA32" s="256"/>
-      <c r="DB32" s="257"/>
+      <c r="CX32" s="258"/>
+      <c r="CY32" s="258"/>
+      <c r="CZ32" s="258"/>
+      <c r="DA32" s="258"/>
+      <c r="DB32" s="259"/>
       <c r="DC32" s="42"/>
     </row>
     <row r="33" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G33" s="41"/>
       <c r="O33" s="41"/>
       <c r="AX33" s="42"/>
-      <c r="AY33" s="259"/>
+      <c r="AY33" s="291"/>
       <c r="BD33" s="41"/>
-      <c r="BE33" s="277"/>
-      <c r="BF33" s="278"/>
-      <c r="BG33" s="278"/>
-      <c r="BH33" s="278"/>
-      <c r="BI33" s="278"/>
-      <c r="BJ33" s="279"/>
+      <c r="BE33" s="275"/>
+      <c r="BF33" s="276"/>
+      <c r="BG33" s="276"/>
+      <c r="BH33" s="276"/>
+      <c r="BI33" s="276"/>
+      <c r="BJ33" s="277"/>
       <c r="BK33" s="42"/>
       <c r="BP33" s="41"/>
-      <c r="BQ33" s="277"/>
-      <c r="BR33" s="278"/>
-      <c r="BS33" s="278"/>
-      <c r="BT33" s="278"/>
-      <c r="BU33" s="278"/>
-      <c r="BV33" s="279"/>
+      <c r="BQ33" s="275"/>
+      <c r="BR33" s="276"/>
+      <c r="BS33" s="276"/>
+      <c r="BT33" s="276"/>
+      <c r="BU33" s="276"/>
+      <c r="BV33" s="277"/>
       <c r="BW33" s="42"/>
       <c r="CA33" s="41"/>
       <c r="CH33" s="42"/>
       <c r="CL33" s="41"/>
-      <c r="CM33" s="271" t="s">
+      <c r="CM33" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN33" s="280"/>
-      <c r="CO33" s="280"/>
-      <c r="CP33" s="280"/>
-      <c r="CQ33" s="280"/>
-      <c r="CR33" s="281"/>
+      <c r="CN33" s="256"/>
+      <c r="CO33" s="256"/>
+      <c r="CP33" s="256"/>
+      <c r="CQ33" s="256"/>
+      <c r="CR33" s="257"/>
       <c r="CS33" s="42"/>
       <c r="CV33" s="41"/>
-      <c r="CW33" s="271" t="s">
+      <c r="CW33" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CX33" s="280"/>
-      <c r="CY33" s="280"/>
-      <c r="CZ33" s="280"/>
-      <c r="DA33" s="280"/>
-      <c r="DB33" s="281"/>
+      <c r="CX33" s="256"/>
+      <c r="CY33" s="256"/>
+      <c r="CZ33" s="256"/>
+      <c r="DA33" s="256"/>
+      <c r="DB33" s="257"/>
       <c r="DC33" s="42"/>
     </row>
     <row r="34" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G34" s="41"/>
       <c r="O34" s="41"/>
       <c r="AX34" s="42"/>
-      <c r="AY34" s="259"/>
+      <c r="AY34" s="291"/>
       <c r="BD34" s="41"/>
       <c r="BK34" s="42"/>
       <c r="BP34" s="41"/>
       <c r="BW34" s="42"/>
       <c r="CA34" s="41"/>
-      <c r="CB34" s="271" t="s">
+      <c r="CB34" s="255" t="s">
         <v>346</v>
       </c>
-      <c r="CC34" s="280"/>
-      <c r="CD34" s="280"/>
-      <c r="CE34" s="280"/>
-      <c r="CF34" s="280"/>
-      <c r="CG34" s="281"/>
+      <c r="CC34" s="256"/>
+      <c r="CD34" s="256"/>
+      <c r="CE34" s="256"/>
+      <c r="CF34" s="256"/>
+      <c r="CG34" s="257"/>
       <c r="CH34" s="42"/>
       <c r="CL34" s="41"/>
       <c r="CS34" s="42"/>
@@ -8778,95 +8794,95 @@
       <c r="G35" s="41"/>
       <c r="O35" s="41"/>
       <c r="AX35" s="42"/>
-      <c r="AY35" s="259"/>
+      <c r="AY35" s="291"/>
       <c r="BD35" s="41"/>
       <c r="BK35" s="42"/>
       <c r="BP35" s="41"/>
-      <c r="BQ35" s="271" t="s">
+      <c r="BQ35" s="255" t="s">
         <v>351</v>
       </c>
-      <c r="BR35" s="256"/>
-      <c r="BS35" s="256"/>
-      <c r="BT35" s="256"/>
-      <c r="BU35" s="256"/>
-      <c r="BV35" s="257"/>
+      <c r="BR35" s="258"/>
+      <c r="BS35" s="258"/>
+      <c r="BT35" s="258"/>
+      <c r="BU35" s="258"/>
+      <c r="BV35" s="259"/>
       <c r="BW35" s="42"/>
       <c r="CA35" s="41"/>
-      <c r="CB35" s="272" t="s">
+      <c r="CB35" s="270" t="s">
         <v>342</v>
       </c>
-      <c r="CC35" s="273"/>
-      <c r="CD35" s="255"/>
-      <c r="CE35" s="257"/>
-      <c r="CF35" s="272" t="s">
+      <c r="CC35" s="271"/>
+      <c r="CD35" s="269"/>
+      <c r="CE35" s="259"/>
+      <c r="CF35" s="270" t="s">
         <v>341</v>
       </c>
-      <c r="CG35" s="273"/>
+      <c r="CG35" s="271"/>
       <c r="CH35" s="42"/>
       <c r="CL35" s="41"/>
-      <c r="CM35" s="271" t="s">
+      <c r="CM35" s="255" t="s">
         <v>358</v>
       </c>
-      <c r="CN35" s="256"/>
-      <c r="CO35" s="256"/>
-      <c r="CP35" s="256"/>
-      <c r="CQ35" s="256"/>
-      <c r="CR35" s="257"/>
+      <c r="CN35" s="258"/>
+      <c r="CO35" s="258"/>
+      <c r="CP35" s="258"/>
+      <c r="CQ35" s="258"/>
+      <c r="CR35" s="259"/>
       <c r="CS35" s="42"/>
       <c r="CV35" s="41"/>
-      <c r="CW35" s="271" t="s">
+      <c r="CW35" s="255" t="s">
         <v>365</v>
       </c>
-      <c r="CX35" s="256"/>
-      <c r="CY35" s="256"/>
-      <c r="CZ35" s="256"/>
-      <c r="DA35" s="256"/>
-      <c r="DB35" s="257"/>
+      <c r="CX35" s="258"/>
+      <c r="CY35" s="258"/>
+      <c r="CZ35" s="258"/>
+      <c r="DA35" s="258"/>
+      <c r="DB35" s="259"/>
       <c r="DC35" s="42"/>
     </row>
     <row r="36" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G36" s="41"/>
       <c r="O36" s="41"/>
       <c r="AX36" s="42"/>
-      <c r="AY36" s="259"/>
+      <c r="AY36" s="291"/>
       <c r="BD36" s="41"/>
       <c r="BK36" s="42"/>
       <c r="BP36" s="41"/>
-      <c r="BQ36" s="271" t="s">
+      <c r="BQ36" s="255" t="s">
         <v>353</v>
       </c>
-      <c r="BR36" s="256"/>
-      <c r="BS36" s="256"/>
-      <c r="BT36" s="256"/>
-      <c r="BU36" s="256"/>
-      <c r="BV36" s="257"/>
+      <c r="BR36" s="258"/>
+      <c r="BS36" s="258"/>
+      <c r="BT36" s="258"/>
+      <c r="BU36" s="258"/>
+      <c r="BV36" s="259"/>
       <c r="BW36" s="42"/>
       <c r="CA36" s="41"/>
       <c r="CH36" s="42"/>
       <c r="CL36" s="41"/>
-      <c r="CM36" s="271" t="s">
+      <c r="CM36" s="255" t="s">
         <v>355</v>
       </c>
-      <c r="CN36" s="280"/>
-      <c r="CO36" s="280"/>
-      <c r="CP36" s="280"/>
-      <c r="CQ36" s="280"/>
-      <c r="CR36" s="281"/>
+      <c r="CN36" s="256"/>
+      <c r="CO36" s="256"/>
+      <c r="CP36" s="256"/>
+      <c r="CQ36" s="256"/>
+      <c r="CR36" s="257"/>
       <c r="CS36" s="42"/>
       <c r="CV36" s="41"/>
-      <c r="CW36" s="285"/>
-      <c r="CX36" s="286"/>
-      <c r="CY36" s="286"/>
-      <c r="CZ36" s="286"/>
-      <c r="DA36" s="286"/>
-      <c r="DB36" s="287"/>
+      <c r="CW36" s="260"/>
+      <c r="CX36" s="261"/>
+      <c r="CY36" s="261"/>
+      <c r="CZ36" s="261"/>
+      <c r="DA36" s="261"/>
+      <c r="DB36" s="262"/>
       <c r="DC36" s="42"/>
     </row>
     <row r="37" spans="7:107" ht="15.75" customHeight="1">
       <c r="G37" s="41"/>
       <c r="O37" s="41"/>
       <c r="AX37" s="42"/>
-      <c r="AY37" s="259"/>
+      <c r="AY37" s="291"/>
       <c r="BD37" s="41"/>
       <c r="BK37" s="42"/>
       <c r="BP37" s="41"/>
@@ -8876,19 +8892,19 @@
       <c r="CL37" s="41"/>
       <c r="CS37" s="42"/>
       <c r="CV37" s="41"/>
-      <c r="CW37" s="288"/>
-      <c r="CX37" s="289"/>
-      <c r="CY37" s="289"/>
-      <c r="CZ37" s="289"/>
-      <c r="DA37" s="289"/>
-      <c r="DB37" s="290"/>
+      <c r="CW37" s="263"/>
+      <c r="CX37" s="264"/>
+      <c r="CY37" s="264"/>
+      <c r="CZ37" s="264"/>
+      <c r="DA37" s="264"/>
+      <c r="DB37" s="265"/>
       <c r="DC37" s="42"/>
     </row>
     <row r="38" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G38" s="41"/>
       <c r="O38" s="41"/>
       <c r="AX38" s="42"/>
-      <c r="AY38" s="259"/>
+      <c r="AY38" s="291"/>
       <c r="BD38" s="41"/>
       <c r="BK38" s="42"/>
       <c r="BP38" s="41"/>
@@ -8898,70 +8914,70 @@
       <c r="CL38" s="41"/>
       <c r="CS38" s="42"/>
       <c r="CV38" s="41"/>
-      <c r="CW38" s="288"/>
-      <c r="CX38" s="289"/>
-      <c r="CY38" s="289"/>
-      <c r="CZ38" s="289"/>
-      <c r="DA38" s="289"/>
-      <c r="DB38" s="290"/>
+      <c r="CW38" s="263"/>
+      <c r="CX38" s="264"/>
+      <c r="CY38" s="264"/>
+      <c r="CZ38" s="264"/>
+      <c r="DA38" s="264"/>
+      <c r="DB38" s="265"/>
       <c r="DC38" s="42"/>
     </row>
     <row r="39" spans="7:107" ht="15.75" customHeight="1">
       <c r="G39" s="41"/>
       <c r="O39" s="41"/>
       <c r="AX39" s="42"/>
-      <c r="AY39" s="259"/>
+      <c r="AY39" s="291"/>
       <c r="BD39" s="41"/>
       <c r="BK39" s="42"/>
       <c r="BP39" s="41"/>
       <c r="BW39" s="42"/>
       <c r="CA39" s="41"/>
-      <c r="CB39" s="274" t="s">
+      <c r="CB39" s="272" t="s">
         <v>347</v>
       </c>
-      <c r="CC39" s="275"/>
-      <c r="CD39" s="275"/>
-      <c r="CE39" s="275"/>
-      <c r="CF39" s="275"/>
-      <c r="CG39" s="276"/>
+      <c r="CC39" s="273"/>
+      <c r="CD39" s="273"/>
+      <c r="CE39" s="273"/>
+      <c r="CF39" s="273"/>
+      <c r="CG39" s="274"/>
       <c r="CH39" s="42"/>
       <c r="CL39" s="41"/>
       <c r="CS39" s="42"/>
       <c r="CV39" s="41"/>
-      <c r="CW39" s="288"/>
-      <c r="CX39" s="289"/>
-      <c r="CY39" s="289"/>
-      <c r="CZ39" s="289"/>
-      <c r="DA39" s="289"/>
-      <c r="DB39" s="290"/>
+      <c r="CW39" s="263"/>
+      <c r="CX39" s="264"/>
+      <c r="CY39" s="264"/>
+      <c r="CZ39" s="264"/>
+      <c r="DA39" s="264"/>
+      <c r="DB39" s="265"/>
       <c r="DC39" s="42"/>
     </row>
     <row r="40" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
       <c r="G40" s="41"/>
       <c r="O40" s="41"/>
       <c r="AX40" s="42"/>
-      <c r="AY40" s="260"/>
+      <c r="AY40" s="292"/>
       <c r="BD40" s="41"/>
       <c r="BK40" s="42"/>
       <c r="BP40" s="41"/>
       <c r="BW40" s="42"/>
       <c r="CA40" s="41"/>
-      <c r="CB40" s="277"/>
-      <c r="CC40" s="278"/>
-      <c r="CD40" s="278"/>
-      <c r="CE40" s="278"/>
-      <c r="CF40" s="278"/>
-      <c r="CG40" s="279"/>
+      <c r="CB40" s="275"/>
+      <c r="CC40" s="276"/>
+      <c r="CD40" s="276"/>
+      <c r="CE40" s="276"/>
+      <c r="CF40" s="276"/>
+      <c r="CG40" s="277"/>
       <c r="CH40" s="42"/>
       <c r="CL40" s="41"/>
       <c r="CS40" s="42"/>
       <c r="CV40" s="41"/>
-      <c r="CW40" s="291"/>
-      <c r="CX40" s="292"/>
-      <c r="CY40" s="292"/>
-      <c r="CZ40" s="292"/>
-      <c r="DA40" s="292"/>
-      <c r="DB40" s="293"/>
+      <c r="CW40" s="266"/>
+      <c r="CX40" s="267"/>
+      <c r="CY40" s="267"/>
+      <c r="CZ40" s="267"/>
+      <c r="DA40" s="267"/>
+      <c r="DB40" s="268"/>
       <c r="DC40" s="42"/>
     </row>
     <row r="41" spans="7:107" ht="15.75" customHeight="1" thickBot="1">
@@ -9024,43 +9040,43 @@
       <c r="M42" s="44"/>
       <c r="N42" s="44"/>
       <c r="O42" s="115"/>
-      <c r="P42" s="255" t="s">
+      <c r="P42" s="269" t="s">
         <v>323</v>
       </c>
-      <c r="Q42" s="256"/>
-      <c r="R42" s="256"/>
-      <c r="S42" s="256"/>
-      <c r="T42" s="256"/>
-      <c r="U42" s="256"/>
-      <c r="V42" s="256"/>
-      <c r="W42" s="256"/>
-      <c r="X42" s="256"/>
-      <c r="Y42" s="256"/>
-      <c r="Z42" s="256"/>
-      <c r="AA42" s="256"/>
-      <c r="AB42" s="256"/>
-      <c r="AC42" s="256"/>
-      <c r="AD42" s="256"/>
-      <c r="AE42" s="256"/>
-      <c r="AF42" s="256"/>
-      <c r="AG42" s="256"/>
-      <c r="AH42" s="256"/>
-      <c r="AI42" s="256"/>
-      <c r="AJ42" s="256"/>
-      <c r="AK42" s="256"/>
-      <c r="AL42" s="256"/>
-      <c r="AM42" s="256"/>
-      <c r="AN42" s="256"/>
-      <c r="AO42" s="256"/>
-      <c r="AP42" s="256"/>
-      <c r="AQ42" s="256"/>
-      <c r="AR42" s="256"/>
-      <c r="AS42" s="256"/>
-      <c r="AT42" s="256"/>
-      <c r="AU42" s="256"/>
-      <c r="AV42" s="256"/>
-      <c r="AW42" s="256"/>
-      <c r="AX42" s="257"/>
+      <c r="Q42" s="258"/>
+      <c r="R42" s="258"/>
+      <c r="S42" s="258"/>
+      <c r="T42" s="258"/>
+      <c r="U42" s="258"/>
+      <c r="V42" s="258"/>
+      <c r="W42" s="258"/>
+      <c r="X42" s="258"/>
+      <c r="Y42" s="258"/>
+      <c r="Z42" s="258"/>
+      <c r="AA42" s="258"/>
+      <c r="AB42" s="258"/>
+      <c r="AC42" s="258"/>
+      <c r="AD42" s="258"/>
+      <c r="AE42" s="258"/>
+      <c r="AF42" s="258"/>
+      <c r="AG42" s="258"/>
+      <c r="AH42" s="258"/>
+      <c r="AI42" s="258"/>
+      <c r="AJ42" s="258"/>
+      <c r="AK42" s="258"/>
+      <c r="AL42" s="258"/>
+      <c r="AM42" s="258"/>
+      <c r="AN42" s="258"/>
+      <c r="AO42" s="258"/>
+      <c r="AP42" s="258"/>
+      <c r="AQ42" s="258"/>
+      <c r="AR42" s="258"/>
+      <c r="AS42" s="258"/>
+      <c r="AT42" s="258"/>
+      <c r="AU42" s="258"/>
+      <c r="AV42" s="258"/>
+      <c r="AW42" s="258"/>
+      <c r="AX42" s="259"/>
       <c r="AY42" s="115"/>
       <c r="BD42" s="43"/>
       <c r="BE42" s="44"/>
@@ -9105,6 +9121,78 @@
     </row>
   </sheetData>
   <mergeCells count="88">
+    <mergeCell ref="P42:AX42"/>
+    <mergeCell ref="AY12:AY40"/>
+    <mergeCell ref="G11:N12"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="T17:W17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="BD11:BK12"/>
+    <mergeCell ref="BD14:BK14"/>
+    <mergeCell ref="BP11:BW12"/>
+    <mergeCell ref="BP14:BW14"/>
+    <mergeCell ref="CA11:CH12"/>
+    <mergeCell ref="CA14:CH14"/>
+    <mergeCell ref="CL11:CS12"/>
+    <mergeCell ref="CL14:CS14"/>
+    <mergeCell ref="CV11:DC12"/>
+    <mergeCell ref="CV14:DC14"/>
+    <mergeCell ref="BQ24:BV24"/>
+    <mergeCell ref="CM18:CR18"/>
+    <mergeCell ref="CM19:CR19"/>
+    <mergeCell ref="CM21:CR21"/>
+    <mergeCell ref="CM24:CR24"/>
+    <mergeCell ref="CM23:CR23"/>
+    <mergeCell ref="BE19:BJ19"/>
+    <mergeCell ref="BE18:BJ18"/>
+    <mergeCell ref="BE21:BJ21"/>
+    <mergeCell ref="BE22:BJ22"/>
+    <mergeCell ref="BQ19:BV19"/>
+    <mergeCell ref="BQ18:BV18"/>
+    <mergeCell ref="BQ21:BV21"/>
+    <mergeCell ref="BQ22:BV22"/>
+    <mergeCell ref="BE24:BJ24"/>
+    <mergeCell ref="BE25:BJ25"/>
+    <mergeCell ref="BE27:BJ27"/>
+    <mergeCell ref="BE28:BF28"/>
+    <mergeCell ref="BI28:BJ28"/>
+    <mergeCell ref="BG28:BH28"/>
+    <mergeCell ref="BE32:BJ33"/>
+    <mergeCell ref="CF29:CG29"/>
+    <mergeCell ref="CD29:CE29"/>
+    <mergeCell ref="CB29:CC29"/>
+    <mergeCell ref="CB28:CG28"/>
+    <mergeCell ref="BQ28:BV28"/>
+    <mergeCell ref="CB39:CG40"/>
+    <mergeCell ref="CB17:CG17"/>
+    <mergeCell ref="CB18:CC18"/>
+    <mergeCell ref="CD18:CE18"/>
+    <mergeCell ref="CF18:CG18"/>
+    <mergeCell ref="CB20:CG20"/>
+    <mergeCell ref="CF26:CG26"/>
+    <mergeCell ref="CD26:CE26"/>
+    <mergeCell ref="CB26:CC26"/>
+    <mergeCell ref="CB25:CG25"/>
+    <mergeCell ref="CE23:CH23"/>
+    <mergeCell ref="CB21:CG21"/>
+    <mergeCell ref="BQ36:BV36"/>
+    <mergeCell ref="CB31:CG31"/>
+    <mergeCell ref="CB32:CC32"/>
+    <mergeCell ref="CD32:CE32"/>
+    <mergeCell ref="CF32:CG32"/>
+    <mergeCell ref="CB34:CG34"/>
+    <mergeCell ref="CB35:CC35"/>
+    <mergeCell ref="CD35:CE35"/>
+    <mergeCell ref="CF35:CG35"/>
+    <mergeCell ref="BQ32:BV33"/>
+    <mergeCell ref="BQ25:BV25"/>
+    <mergeCell ref="BQ27:BV27"/>
+    <mergeCell ref="CM32:CR32"/>
+    <mergeCell ref="CM33:CR33"/>
+    <mergeCell ref="CM35:CR35"/>
+    <mergeCell ref="CM27:CR27"/>
+    <mergeCell ref="CM26:CR26"/>
+    <mergeCell ref="BQ35:BV35"/>
     <mergeCell ref="CM36:CR36"/>
     <mergeCell ref="CW18:DB18"/>
     <mergeCell ref="CW20:DB20"/>
@@ -9121,78 +9209,6 @@
     <mergeCell ref="CW36:DB40"/>
     <mergeCell ref="CM29:CR29"/>
     <mergeCell ref="CM30:CR30"/>
-    <mergeCell ref="BQ25:BV25"/>
-    <mergeCell ref="BQ27:BV27"/>
-    <mergeCell ref="CM32:CR32"/>
-    <mergeCell ref="CM33:CR33"/>
-    <mergeCell ref="CM35:CR35"/>
-    <mergeCell ref="CM27:CR27"/>
-    <mergeCell ref="CM26:CR26"/>
-    <mergeCell ref="BQ35:BV35"/>
-    <mergeCell ref="BQ36:BV36"/>
-    <mergeCell ref="CB31:CG31"/>
-    <mergeCell ref="CB32:CC32"/>
-    <mergeCell ref="CD32:CE32"/>
-    <mergeCell ref="CF32:CG32"/>
-    <mergeCell ref="CB34:CG34"/>
-    <mergeCell ref="CB35:CC35"/>
-    <mergeCell ref="CD35:CE35"/>
-    <mergeCell ref="CF35:CG35"/>
-    <mergeCell ref="BQ32:BV33"/>
-    <mergeCell ref="CB39:CG40"/>
-    <mergeCell ref="CB17:CG17"/>
-    <mergeCell ref="CB18:CC18"/>
-    <mergeCell ref="CD18:CE18"/>
-    <mergeCell ref="CF18:CG18"/>
-    <mergeCell ref="CB20:CG20"/>
-    <mergeCell ref="CF26:CG26"/>
-    <mergeCell ref="CD26:CE26"/>
-    <mergeCell ref="CB26:CC26"/>
-    <mergeCell ref="CB25:CG25"/>
-    <mergeCell ref="CE23:CH23"/>
-    <mergeCell ref="CB21:CG21"/>
-    <mergeCell ref="BE32:BJ33"/>
-    <mergeCell ref="CF29:CG29"/>
-    <mergeCell ref="CD29:CE29"/>
-    <mergeCell ref="CB29:CC29"/>
-    <mergeCell ref="CB28:CG28"/>
-    <mergeCell ref="BQ28:BV28"/>
-    <mergeCell ref="BE24:BJ24"/>
-    <mergeCell ref="BE25:BJ25"/>
-    <mergeCell ref="BE27:BJ27"/>
-    <mergeCell ref="BE28:BF28"/>
-    <mergeCell ref="BI28:BJ28"/>
-    <mergeCell ref="BG28:BH28"/>
-    <mergeCell ref="BE19:BJ19"/>
-    <mergeCell ref="BE18:BJ18"/>
-    <mergeCell ref="BE21:BJ21"/>
-    <mergeCell ref="BE22:BJ22"/>
-    <mergeCell ref="BQ19:BV19"/>
-    <mergeCell ref="BQ18:BV18"/>
-    <mergeCell ref="BQ21:BV21"/>
-    <mergeCell ref="BQ22:BV22"/>
-    <mergeCell ref="CL11:CS12"/>
-    <mergeCell ref="CL14:CS14"/>
-    <mergeCell ref="CV11:DC12"/>
-    <mergeCell ref="CV14:DC14"/>
-    <mergeCell ref="BQ24:BV24"/>
-    <mergeCell ref="CM18:CR18"/>
-    <mergeCell ref="CM19:CR19"/>
-    <mergeCell ref="CM21:CR21"/>
-    <mergeCell ref="CM24:CR24"/>
-    <mergeCell ref="CM23:CR23"/>
-    <mergeCell ref="BD11:BK12"/>
-    <mergeCell ref="BD14:BK14"/>
-    <mergeCell ref="BP11:BW12"/>
-    <mergeCell ref="BP14:BW14"/>
-    <mergeCell ref="CA11:CH12"/>
-    <mergeCell ref="CA14:CH14"/>
-    <mergeCell ref="P42:AX42"/>
-    <mergeCell ref="AY12:AY40"/>
-    <mergeCell ref="G11:N12"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="T17:W17"/>
-    <mergeCell ref="P17:R17"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9251,14 +9267,14 @@
         <v>476</v>
       </c>
       <c r="C3" s="28"/>
-      <c r="D3" s="299" t="s">
+      <c r="D3" s="296" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="300"/>
-      <c r="F3" s="300"/>
-      <c r="G3" s="300"/>
-      <c r="H3" s="300"/>
-      <c r="I3" s="301"/>
+      <c r="E3" s="297"/>
+      <c r="F3" s="297"/>
+      <c r="G3" s="297"/>
+      <c r="H3" s="297"/>
+      <c r="I3" s="298"/>
     </row>
     <row r="4" spans="1:16" ht="21" customHeight="1">
       <c r="A4" s="156" t="s">
@@ -9397,15 +9413,15 @@
         <v>375</v>
       </c>
       <c r="F12" s="132"/>
-      <c r="H12" s="294" t="s">
+      <c r="H12" s="299" t="s">
         <v>400</v>
       </c>
-      <c r="I12" s="302"/>
+      <c r="I12" s="300"/>
       <c r="J12" s="140" t="s">
         <v>404</v>
       </c>
       <c r="K12" s="132"/>
-      <c r="M12" s="294" t="s">
+      <c r="M12" s="299" t="s">
         <v>415</v>
       </c>
       <c r="N12" s="295"/>
@@ -9422,15 +9438,15 @@
         <v>368</v>
       </c>
       <c r="F13" s="132"/>
-      <c r="H13" s="294" t="s">
+      <c r="H13" s="299" t="s">
         <v>401</v>
       </c>
-      <c r="I13" s="302"/>
+      <c r="I13" s="300"/>
       <c r="J13" s="140" t="s">
         <v>403</v>
       </c>
       <c r="K13" s="132"/>
-      <c r="M13" s="294" t="s">
+      <c r="M13" s="299" t="s">
         <v>216</v>
       </c>
       <c r="N13" s="295"/>
@@ -9445,15 +9461,15 @@
       </c>
       <c r="E14" s="131"/>
       <c r="F14" s="132"/>
-      <c r="H14" s="294" t="s">
+      <c r="H14" s="299" t="s">
         <v>402</v>
       </c>
-      <c r="I14" s="302"/>
+      <c r="I14" s="300"/>
       <c r="J14" s="140" t="s">
         <v>369</v>
       </c>
       <c r="K14" s="132"/>
-      <c r="M14" s="294" t="s">
+      <c r="M14" s="299" t="s">
         <v>215</v>
       </c>
       <c r="N14" s="295"/>
@@ -9468,11 +9484,11 @@
       </c>
       <c r="E15" s="140"/>
       <c r="F15" s="132"/>
-      <c r="H15" s="297"/>
-      <c r="I15" s="298"/>
+      <c r="H15" s="301"/>
+      <c r="I15" s="302"/>
       <c r="J15" s="140"/>
       <c r="K15" s="132"/>
-      <c r="M15" s="294" t="s">
+      <c r="M15" s="299" t="s">
         <v>211</v>
       </c>
       <c r="N15" s="295"/>
@@ -9487,11 +9503,11 @@
       </c>
       <c r="E16" s="131"/>
       <c r="F16" s="134"/>
-      <c r="H16" s="297"/>
-      <c r="I16" s="298"/>
+      <c r="H16" s="301"/>
+      <c r="I16" s="302"/>
       <c r="J16" s="140"/>
       <c r="K16" s="132"/>
-      <c r="M16" s="294" t="s">
+      <c r="M16" s="299" t="s">
         <v>212</v>
       </c>
       <c r="N16" s="295"/>
@@ -9510,7 +9526,7 @@
       <c r="I17" s="135"/>
       <c r="J17" s="136"/>
       <c r="K17" s="137"/>
-      <c r="M17" s="294" t="s">
+      <c r="M17" s="299" t="s">
         <v>416</v>
       </c>
       <c r="N17" s="295"/>
@@ -9523,7 +9539,7 @@
       <c r="C18" s="133"/>
       <c r="E18" s="131"/>
       <c r="F18" s="134"/>
-      <c r="M18" s="294" t="s">
+      <c r="M18" s="299" t="s">
         <v>213</v>
       </c>
       <c r="N18" s="295"/>
@@ -9546,7 +9562,7 @@
       <c r="K19" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="M19" s="294" t="s">
+      <c r="M19" s="299" t="s">
         <v>290</v>
       </c>
       <c r="N19" s="295"/>
@@ -9567,7 +9583,7 @@
       <c r="I20" s="29"/>
       <c r="J20" s="29"/>
       <c r="K20" s="127"/>
-      <c r="M20" s="296" t="s">
+      <c r="M20" s="294" t="s">
         <v>423</v>
       </c>
       <c r="N20" s="295"/>
@@ -9584,7 +9600,7 @@
       <c r="I21" s="29"/>
       <c r="J21" s="29"/>
       <c r="K21" s="127"/>
-      <c r="M21" s="296" t="s">
+      <c r="M21" s="294" t="s">
         <v>424</v>
       </c>
       <c r="N21" s="295"/>
@@ -9604,21 +9620,21 @@
         <v>84</v>
       </c>
       <c r="K22" s="130"/>
-      <c r="M22" s="296"/>
+      <c r="M22" s="294"/>
       <c r="N22" s="295"/>
       <c r="O22" s="131"/>
       <c r="P22" s="132"/>
     </row>
     <row r="23" spans="3:16" ht="15.75" customHeight="1" thickBot="1">
-      <c r="H23" s="294" t="s">
+      <c r="H23" s="299" t="s">
         <v>405</v>
       </c>
-      <c r="I23" s="302"/>
+      <c r="I23" s="300"/>
       <c r="J23" s="140" t="s">
         <v>369</v>
       </c>
       <c r="K23" s="132"/>
-      <c r="M23" s="296"/>
+      <c r="M23" s="294"/>
       <c r="N23" s="295"/>
       <c r="O23" s="131"/>
       <c r="P23" s="132"/>
@@ -9632,11 +9648,11 @@
       <c r="F24" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="H24" s="294"/>
-      <c r="I24" s="302"/>
+      <c r="H24" s="299"/>
+      <c r="I24" s="300"/>
       <c r="J24" s="140"/>
       <c r="K24" s="132"/>
-      <c r="M24" s="296"/>
+      <c r="M24" s="294"/>
       <c r="N24" s="295"/>
       <c r="O24" s="131"/>
       <c r="P24" s="132"/>
@@ -9650,11 +9666,11 @@
       <c r="F25" s="143" t="s">
         <v>373</v>
       </c>
-      <c r="H25" s="294"/>
-      <c r="I25" s="302"/>
+      <c r="H25" s="299"/>
+      <c r="I25" s="300"/>
       <c r="J25" s="140"/>
       <c r="K25" s="132"/>
-      <c r="M25" s="296"/>
+      <c r="M25" s="294"/>
       <c r="N25" s="295"/>
       <c r="O25" s="131"/>
       <c r="P25" s="132"/>
@@ -9664,11 +9680,11 @@
       <c r="D26" s="29"/>
       <c r="E26" s="29"/>
       <c r="F26" s="127"/>
-      <c r="H26" s="297"/>
-      <c r="I26" s="298"/>
+      <c r="H26" s="301"/>
+      <c r="I26" s="302"/>
       <c r="J26" s="140"/>
       <c r="K26" s="132"/>
-      <c r="M26" s="296"/>
+      <c r="M26" s="294"/>
       <c r="N26" s="295"/>
       <c r="O26" s="131"/>
       <c r="P26" s="132"/>
@@ -9682,11 +9698,11 @@
         <v>84</v>
       </c>
       <c r="F27" s="130"/>
-      <c r="H27" s="297"/>
-      <c r="I27" s="298"/>
+      <c r="H27" s="301"/>
+      <c r="I27" s="302"/>
       <c r="J27" s="140"/>
       <c r="K27" s="132"/>
-      <c r="M27" s="296"/>
+      <c r="M27" s="294"/>
       <c r="N27" s="295"/>
       <c r="O27" s="131"/>
       <c r="P27" s="132"/>
@@ -9703,7 +9719,7 @@
       <c r="I28" s="135"/>
       <c r="J28" s="136"/>
       <c r="K28" s="137"/>
-      <c r="M28" s="296"/>
+      <c r="M28" s="294"/>
       <c r="N28" s="295"/>
       <c r="O28" s="131"/>
       <c r="P28" s="132"/>
@@ -9716,7 +9732,7 @@
         <v>388</v>
       </c>
       <c r="F29" s="132"/>
-      <c r="M29" s="296"/>
+      <c r="M29" s="294"/>
       <c r="N29" s="295"/>
       <c r="O29" s="131"/>
       <c r="P29" s="132"/>
@@ -9727,7 +9743,7 @@
       </c>
       <c r="E30" s="140"/>
       <c r="F30" s="132"/>
-      <c r="M30" s="296"/>
+      <c r="M30" s="294"/>
       <c r="N30" s="295"/>
       <c r="O30" s="131"/>
       <c r="P30" s="132"/>
@@ -9808,7 +9824,7 @@
       <c r="C37" s="133"/>
       <c r="E37" s="131"/>
       <c r="F37" s="134"/>
-      <c r="M37" s="294" t="s">
+      <c r="M37" s="299" t="s">
         <v>428</v>
       </c>
       <c r="N37" s="295"/>
@@ -9821,7 +9837,7 @@
       <c r="C38" s="133"/>
       <c r="E38" s="131"/>
       <c r="F38" s="134"/>
-      <c r="M38" s="296" t="s">
+      <c r="M38" s="294" t="s">
         <v>429</v>
       </c>
       <c r="N38" s="295"/>
@@ -9835,7 +9851,7 @@
       <c r="D39" s="135"/>
       <c r="E39" s="136"/>
       <c r="F39" s="139"/>
-      <c r="M39" s="296"/>
+      <c r="M39" s="294"/>
       <c r="N39" s="295"/>
       <c r="O39" s="131" t="s">
         <v>432</v>
@@ -9843,7 +9859,7 @@
       <c r="P39" s="132"/>
     </row>
     <row r="40" spans="3:16" ht="15.75" customHeight="1" thickBot="1">
-      <c r="M40" s="296"/>
+      <c r="M40" s="294"/>
       <c r="N40" s="295"/>
       <c r="O40" s="131" t="s">
         <v>433</v>
@@ -9859,7 +9875,7 @@
       <c r="F41" s="125" t="s">
         <v>81</v>
       </c>
-      <c r="M41" s="296"/>
+      <c r="M41" s="294"/>
       <c r="N41" s="295"/>
       <c r="O41" s="131" t="s">
         <v>435</v>
@@ -9875,7 +9891,7 @@
       <c r="F42" s="143" t="s">
         <v>373</v>
       </c>
-      <c r="M42" s="296"/>
+      <c r="M42" s="294"/>
       <c r="N42" s="295"/>
       <c r="O42" s="131" t="s">
         <v>434</v>
@@ -9970,7 +9986,7 @@
         <v>397</v>
       </c>
       <c r="F49" s="134"/>
-      <c r="M49" s="294" t="s">
+      <c r="M49" s="299" t="s">
         <v>436</v>
       </c>
       <c r="N49" s="295"/>
@@ -9987,7 +10003,7 @@
         <v>334</v>
       </c>
       <c r="F50" s="134"/>
-      <c r="M50" s="296" t="s">
+      <c r="M50" s="294" t="s">
         <v>437</v>
       </c>
       <c r="N50" s="295"/>
@@ -10004,7 +10020,7 @@
         <v>369</v>
       </c>
       <c r="F51" s="134"/>
-      <c r="M51" s="296" t="s">
+      <c r="M51" s="294" t="s">
         <v>438</v>
       </c>
       <c r="N51" s="295"/>
@@ -10017,7 +10033,7 @@
         <v>456</v>
       </c>
       <c r="F52" s="134"/>
-      <c r="M52" s="296" t="s">
+      <c r="M52" s="294" t="s">
         <v>441</v>
       </c>
       <c r="N52" s="295"/>
@@ -10031,7 +10047,7 @@
         <v>457</v>
       </c>
       <c r="F53" s="137"/>
-      <c r="M53" s="296"/>
+      <c r="M53" s="294"/>
       <c r="N53" s="295"/>
       <c r="O53" s="131"/>
       <c r="P53" s="132"/>
@@ -10084,7 +10100,7 @@
       </c>
     </row>
     <row r="60" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M60" s="294" t="s">
+      <c r="M60" s="299" t="s">
         <v>442</v>
       </c>
       <c r="N60" s="295"/>
@@ -10096,7 +10112,7 @@
       </c>
     </row>
     <row r="61" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M61" s="296" t="s">
+      <c r="M61" s="294" t="s">
         <v>443</v>
       </c>
       <c r="N61" s="295"/>
@@ -10108,7 +10124,7 @@
       </c>
     </row>
     <row r="62" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M62" s="294" t="s">
+      <c r="M62" s="299" t="s">
         <v>448</v>
       </c>
       <c r="N62" s="295"/>
@@ -10120,13 +10136,13 @@
       </c>
     </row>
     <row r="63" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M63" s="296"/>
+      <c r="M63" s="294"/>
       <c r="N63" s="295"/>
       <c r="O63" s="131"/>
       <c r="P63" s="132"/>
     </row>
     <row r="64" spans="3:16" ht="15.75" customHeight="1">
-      <c r="M64" s="296"/>
+      <c r="M64" s="294"/>
       <c r="N64" s="295"/>
       <c r="O64" s="131"/>
       <c r="P64" s="132"/>
@@ -10175,7 +10191,7 @@
       <c r="P70" s="130"/>
     </row>
     <row r="71" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M71" s="294" t="s">
+      <c r="M71" s="299" t="s">
         <v>449</v>
       </c>
       <c r="N71" s="295"/>
@@ -10185,7 +10201,7 @@
       <c r="P71" s="132"/>
     </row>
     <row r="72" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M72" s="294" t="s">
+      <c r="M72" s="299" t="s">
         <v>450</v>
       </c>
       <c r="N72" s="295"/>
@@ -10195,19 +10211,19 @@
       <c r="P72" s="132"/>
     </row>
     <row r="73" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M73" s="296"/>
+      <c r="M73" s="294"/>
       <c r="N73" s="295"/>
       <c r="O73" s="131"/>
       <c r="P73" s="132"/>
     </row>
     <row r="74" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M74" s="296"/>
+      <c r="M74" s="294"/>
       <c r="N74" s="295"/>
       <c r="O74" s="131"/>
       <c r="P74" s="132"/>
     </row>
     <row r="75" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M75" s="296"/>
+      <c r="M75" s="294"/>
       <c r="N75" s="295"/>
       <c r="O75" s="131"/>
       <c r="P75" s="132"/>
@@ -10256,7 +10272,7 @@
       <c r="P81" s="130"/>
     </row>
     <row r="82" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M82" s="294" t="s">
+      <c r="M82" s="299" t="s">
         <v>449</v>
       </c>
       <c r="N82" s="295"/>
@@ -10266,7 +10282,7 @@
       <c r="P82" s="132"/>
     </row>
     <row r="83" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M83" s="294" t="s">
+      <c r="M83" s="299" t="s">
         <v>452</v>
       </c>
       <c r="N83" s="295"/>
@@ -10276,19 +10292,19 @@
       <c r="P83" s="132"/>
     </row>
     <row r="84" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M84" s="296"/>
+      <c r="M84" s="294"/>
       <c r="N84" s="295"/>
       <c r="O84" s="131"/>
       <c r="P84" s="132"/>
     </row>
     <row r="85" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M85" s="296"/>
+      <c r="M85" s="294"/>
       <c r="N85" s="295"/>
       <c r="O85" s="131"/>
       <c r="P85" s="132"/>
     </row>
     <row r="86" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M86" s="296"/>
+      <c r="M86" s="294"/>
       <c r="N86" s="295"/>
       <c r="O86" s="131"/>
       <c r="P86" s="132"/>
@@ -10335,7 +10351,7 @@
       <c r="P92" s="130"/>
     </row>
     <row r="93" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M93" s="294" t="s">
+      <c r="M93" s="299" t="s">
         <v>216</v>
       </c>
       <c r="N93" s="295"/>
@@ -10345,7 +10361,7 @@
       <c r="P93" s="132"/>
     </row>
     <row r="94" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M94" s="296"/>
+      <c r="M94" s="294"/>
       <c r="N94" s="295"/>
       <c r="O94" s="140" t="s">
         <v>454</v>
@@ -10353,7 +10369,7 @@
       <c r="P94" s="132"/>
     </row>
     <row r="95" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M95" s="296"/>
+      <c r="M95" s="294"/>
       <c r="N95" s="295"/>
       <c r="O95" s="140" t="s">
         <v>455</v>
@@ -10361,13 +10377,13 @@
       <c r="P95" s="132"/>
     </row>
     <row r="96" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M96" s="296"/>
+      <c r="M96" s="294"/>
       <c r="N96" s="295"/>
       <c r="O96" s="131"/>
       <c r="P96" s="132"/>
     </row>
     <row r="97" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M97" s="296"/>
+      <c r="M97" s="294"/>
       <c r="N97" s="295"/>
       <c r="O97" s="131"/>
       <c r="P97" s="132"/>
@@ -10414,7 +10430,7 @@
       <c r="P103" s="130"/>
     </row>
     <row r="104" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M104" s="294" t="s">
+      <c r="M104" s="299" t="s">
         <v>465</v>
       </c>
       <c r="N104" s="295"/>
@@ -10424,7 +10440,7 @@
       <c r="P104" s="132"/>
     </row>
     <row r="105" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M105" s="294" t="s">
+      <c r="M105" s="299" t="s">
         <v>466</v>
       </c>
       <c r="N105" s="295"/>
@@ -10434,7 +10450,7 @@
       <c r="P105" s="132"/>
     </row>
     <row r="106" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M106" s="294" t="s">
+      <c r="M106" s="299" t="s">
         <v>467</v>
       </c>
       <c r="N106" s="295"/>
@@ -10444,7 +10460,7 @@
       <c r="P106" s="132"/>
     </row>
     <row r="107" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M107" s="296"/>
+      <c r="M107" s="294"/>
       <c r="N107" s="295"/>
       <c r="O107" s="140" t="s">
         <v>464</v>
@@ -10452,7 +10468,7 @@
       <c r="P107" s="132"/>
     </row>
     <row r="108" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M108" s="296"/>
+      <c r="M108" s="294"/>
       <c r="N108" s="295"/>
       <c r="O108" s="131"/>
       <c r="P108" s="132"/>
@@ -10501,7 +10517,7 @@
       <c r="P114" s="130"/>
     </row>
     <row r="115" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M115" s="294" t="s">
+      <c r="M115" s="299" t="s">
         <v>482</v>
       </c>
       <c r="N115" s="295"/>
@@ -10511,31 +10527,31 @@
       <c r="P115" s="132"/>
     </row>
     <row r="116" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M116" s="296"/>
+      <c r="M116" s="294"/>
       <c r="N116" s="295"/>
       <c r="O116" s="131"/>
       <c r="P116" s="132"/>
     </row>
     <row r="117" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M117" s="296"/>
+      <c r="M117" s="294"/>
       <c r="N117" s="295"/>
       <c r="O117" s="131"/>
       <c r="P117" s="132"/>
     </row>
     <row r="118" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M118" s="296"/>
+      <c r="M118" s="294"/>
       <c r="N118" s="295"/>
       <c r="O118" s="131"/>
       <c r="P118" s="132"/>
     </row>
     <row r="119" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M119" s="296"/>
+      <c r="M119" s="294"/>
       <c r="N119" s="295"/>
       <c r="O119" s="131"/>
       <c r="P119" s="132"/>
     </row>
     <row r="120" spans="13:16" ht="15.75" customHeight="1">
-      <c r="M120" s="296"/>
+      <c r="M120" s="294"/>
       <c r="N120" s="295"/>
       <c r="O120" s="131"/>
       <c r="P120" s="132"/>
@@ -10548,6 +10564,62 @@
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="M105:N105"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="M107:N107"/>
+    <mergeCell ref="M108:N108"/>
+    <mergeCell ref="M94:N94"/>
+    <mergeCell ref="M95:N95"/>
+    <mergeCell ref="M96:N96"/>
+    <mergeCell ref="M97:N97"/>
+    <mergeCell ref="M104:N104"/>
+    <mergeCell ref="M83:N83"/>
+    <mergeCell ref="M84:N84"/>
+    <mergeCell ref="M85:N85"/>
+    <mergeCell ref="M86:N86"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="M72:N72"/>
+    <mergeCell ref="M73:N73"/>
+    <mergeCell ref="M74:N74"/>
+    <mergeCell ref="M75:N75"/>
+    <mergeCell ref="M82:N82"/>
+    <mergeCell ref="M61:N61"/>
+    <mergeCell ref="M62:N62"/>
+    <mergeCell ref="M63:N63"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M71:N71"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="M60:N60"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M41:N41"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="M42:N42"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="M23:N23"/>
     <mergeCell ref="M119:N119"/>
     <mergeCell ref="M120:N120"/>
     <mergeCell ref="D3:I3"/>
@@ -10564,62 +10636,6 @@
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="H25:I25"/>
     <mergeCell ref="H26:I26"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M29:N29"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="M23:N23"/>
-    <mergeCell ref="M24:N24"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="M27:N27"/>
-    <mergeCell ref="M28:N28"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M41:N41"/>
-    <mergeCell ref="M49:N49"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="M51:N51"/>
-    <mergeCell ref="M52:N52"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="M60:N60"/>
-    <mergeCell ref="M61:N61"/>
-    <mergeCell ref="M62:N62"/>
-    <mergeCell ref="M63:N63"/>
-    <mergeCell ref="M64:N64"/>
-    <mergeCell ref="M71:N71"/>
-    <mergeCell ref="M72:N72"/>
-    <mergeCell ref="M73:N73"/>
-    <mergeCell ref="M74:N74"/>
-    <mergeCell ref="M75:N75"/>
-    <mergeCell ref="M82:N82"/>
-    <mergeCell ref="M83:N83"/>
-    <mergeCell ref="M84:N84"/>
-    <mergeCell ref="M85:N85"/>
-    <mergeCell ref="M86:N86"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="M105:N105"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="M107:N107"/>
-    <mergeCell ref="M108:N108"/>
-    <mergeCell ref="M94:N94"/>
-    <mergeCell ref="M95:N95"/>
-    <mergeCell ref="M96:N96"/>
-    <mergeCell ref="M97:N97"/>
-    <mergeCell ref="M104:N104"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
@@ -10632,8 +10648,8 @@
   </sheetPr>
   <dimension ref="B1:H141"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
@@ -15716,17 +15732,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:U217"/>
+  <dimension ref="B2:U222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="76.7109375" customWidth="1"/>
+    <col min="3" max="3" width="99.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
@@ -15739,7 +15755,7 @@
     <col min="13" max="13" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.42578125" customWidth="1"/>
-    <col min="16" max="16" width="17.140625" customWidth="1"/>
+    <col min="16" max="16" width="38" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.85546875" customWidth="1"/>
     <col min="18" max="26" width="11.42578125" customWidth="1"/>
   </cols>
@@ -15836,7 +15852,7 @@
     </row>
     <row r="7" spans="2:21" ht="21.75" customHeight="1" thickBot="1">
       <c r="B7" s="183" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C7" s="184"/>
       <c r="D7" s="185"/>
@@ -16032,13 +16048,13 @@
     <row r="14" spans="2:21" ht="20.25" customHeight="1">
       <c r="B14" s="218"/>
       <c r="C14" s="229" t="s">
+        <v>637</v>
+      </c>
+      <c r="D14" s="218" t="s">
+        <v>640</v>
+      </c>
+      <c r="E14" s="231" t="s">
         <v>638</v>
-      </c>
-      <c r="D14" s="218" t="s">
-        <v>641</v>
-      </c>
-      <c r="E14" s="231" t="s">
-        <v>639</v>
       </c>
       <c r="F14" s="243"/>
       <c r="G14" s="217"/>
@@ -16062,10 +16078,10 @@
         <v>628</v>
       </c>
       <c r="D15" s="218" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E15" s="231" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F15" s="243"/>
       <c r="G15" s="217"/>
@@ -16089,10 +16105,10 @@
         <v>629</v>
       </c>
       <c r="D16" s="218" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E16" s="231" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F16" s="243"/>
       <c r="G16" s="217"/>
@@ -16160,10 +16176,10 @@
         <v>631</v>
       </c>
       <c r="D19" s="218" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E19" s="231" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F19" s="243"/>
       <c r="G19" s="217"/>
@@ -16187,10 +16203,10 @@
         <v>632</v>
       </c>
       <c r="D20" s="218" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E20" s="231" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F20" s="243"/>
       <c r="G20" s="217"/>
@@ -16258,10 +16274,10 @@
         <v>634</v>
       </c>
       <c r="D23" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E23" s="231" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F23" s="243"/>
       <c r="G23" s="217"/>
@@ -16326,10 +16342,10 @@
     <row r="26" spans="2:21" ht="20.25" customHeight="1">
       <c r="B26" s="218"/>
       <c r="C26" s="229" t="s">
+        <v>646</v>
+      </c>
+      <c r="D26" s="229" t="s">
         <v>647</v>
-      </c>
-      <c r="D26" s="229" t="s">
-        <v>648</v>
       </c>
       <c r="E26" s="231"/>
       <c r="F26" s="232"/>
@@ -16351,10 +16367,10 @@
     <row r="27" spans="2:21" ht="20.25" customHeight="1">
       <c r="B27" s="218"/>
       <c r="C27" s="229" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D27" s="229" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E27" s="231"/>
       <c r="F27" s="232"/>
@@ -16399,13 +16415,13 @@
     <row r="29" spans="2:21" ht="20.25" customHeight="1">
       <c r="B29" s="242"/>
       <c r="C29" s="229" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D29" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E29" s="231" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F29" s="243"/>
       <c r="G29" s="217"/>
@@ -16426,16 +16442,16 @@
     <row r="30" spans="2:21" ht="20.25" customHeight="1">
       <c r="B30" s="242"/>
       <c r="C30" s="229" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D30" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E30" s="231"/>
       <c r="F30" s="232"/>
       <c r="G30" s="217"/>
       <c r="H30" s="244" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I30" s="243"/>
       <c r="J30" s="217"/>
@@ -16452,7 +16468,7 @@
     </row>
     <row r="31" spans="2:21" ht="20.25" customHeight="1">
       <c r="B31" s="242" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C31" s="229"/>
       <c r="D31" s="218"/>
@@ -16476,16 +16492,16 @@
     <row r="32" spans="2:21" ht="20.25" customHeight="1">
       <c r="B32" s="242"/>
       <c r="C32" s="229" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D32" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E32" s="231"/>
       <c r="F32" s="232"/>
       <c r="G32" s="217"/>
       <c r="H32" s="244" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I32" s="243"/>
       <c r="J32" s="217"/>
@@ -16503,16 +16519,16 @@
     <row r="33" spans="2:21" ht="20.25" customHeight="1">
       <c r="B33" s="242"/>
       <c r="C33" s="229" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D33" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E33" s="231"/>
       <c r="F33" s="232"/>
       <c r="G33" s="217"/>
       <c r="H33" s="244" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I33" s="243"/>
       <c r="J33" s="217"/>
@@ -16553,16 +16569,16 @@
     <row r="35" spans="2:21" ht="20.25" customHeight="1">
       <c r="B35" s="242"/>
       <c r="C35" s="229" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="D35" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E35" s="231"/>
       <c r="F35" s="232"/>
       <c r="G35" s="217"/>
       <c r="H35" s="244" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I35" s="243"/>
       <c r="J35" s="217"/>
@@ -16645,16 +16661,16 @@
     <row r="39" spans="2:21" ht="20.25" customHeight="1">
       <c r="B39" s="242"/>
       <c r="C39" s="229" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D39" s="218" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E39" s="231"/>
       <c r="F39" s="232"/>
       <c r="G39" s="217"/>
       <c r="H39" s="244" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I39" s="243"/>
       <c r="J39" s="217"/>
@@ -16675,13 +16691,13 @@
         <v>635</v>
       </c>
       <c r="D40" s="218" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E40" s="231"/>
       <c r="F40" s="232"/>
       <c r="G40" s="217"/>
       <c r="H40" s="244" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I40" s="243"/>
       <c r="J40" s="217"/>
@@ -16719,7 +16735,7 @@
     </row>
     <row r="42" spans="2:21" ht="20.25" customHeight="1">
       <c r="B42" s="242" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C42" s="229"/>
       <c r="D42" s="218"/>
@@ -16743,10 +16759,10 @@
     <row r="43" spans="2:21" ht="20.25" customHeight="1">
       <c r="B43" s="242"/>
       <c r="C43" s="229" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D43" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E43" s="231"/>
       <c r="F43" s="232"/>
@@ -16755,7 +16771,7 @@
       <c r="I43" s="216"/>
       <c r="J43" s="217"/>
       <c r="K43" s="244" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="L43" s="243"/>
       <c r="M43" s="217"/>
@@ -16770,10 +16786,10 @@
     <row r="44" spans="2:21" ht="20.25" customHeight="1">
       <c r="B44" s="242"/>
       <c r="C44" s="229" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D44" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E44" s="231"/>
       <c r="F44" s="232"/>
@@ -16782,11 +16798,11 @@
       <c r="I44" s="216"/>
       <c r="J44" s="217"/>
       <c r="K44" s="244" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="L44" s="243"/>
       <c r="M44" s="217" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N44" s="231"/>
       <c r="O44" s="216"/>
@@ -16799,10 +16815,10 @@
     <row r="45" spans="2:21" ht="20.25" customHeight="1">
       <c r="B45" s="242"/>
       <c r="C45" s="229" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D45" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E45" s="231"/>
       <c r="F45" s="232"/>
@@ -16811,7 +16827,7 @@
       <c r="I45" s="216"/>
       <c r="J45" s="217"/>
       <c r="K45" s="244" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="L45" s="243"/>
       <c r="M45" s="217"/>
@@ -16826,10 +16842,10 @@
     <row r="46" spans="2:21" ht="20.25" customHeight="1">
       <c r="B46" s="242"/>
       <c r="C46" s="229" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D46" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E46" s="231"/>
       <c r="F46" s="232"/>
@@ -16838,7 +16854,7 @@
       <c r="I46" s="216"/>
       <c r="J46" s="217"/>
       <c r="K46" s="244" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="L46" s="243"/>
       <c r="M46" s="217"/>
@@ -16853,10 +16869,10 @@
     <row r="47" spans="2:21" ht="20.25" customHeight="1">
       <c r="B47" s="242"/>
       <c r="C47" s="229" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D47" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E47" s="231"/>
       <c r="F47" s="232"/>
@@ -16868,7 +16884,7 @@
       <c r="L47" s="216"/>
       <c r="M47" s="217"/>
       <c r="N47" s="231" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O47" s="243"/>
       <c r="P47" s="217"/>
@@ -16880,10 +16896,10 @@
     <row r="48" spans="2:21" ht="20.25" customHeight="1">
       <c r="B48" s="242"/>
       <c r="C48" s="229" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D48" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E48" s="231"/>
       <c r="F48" s="232"/>
@@ -16895,7 +16911,7 @@
       <c r="L48" s="216"/>
       <c r="M48" s="217"/>
       <c r="N48" s="231" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O48" s="243"/>
       <c r="P48" s="217"/>
@@ -16907,10 +16923,10 @@
     <row r="49" spans="2:21" ht="20.25" customHeight="1">
       <c r="B49" s="242"/>
       <c r="C49" s="229" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D49" s="218" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E49" s="231"/>
       <c r="F49" s="232"/>
@@ -16922,7 +16938,7 @@
       <c r="L49" s="216"/>
       <c r="M49" s="217"/>
       <c r="N49" s="231" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O49" s="243"/>
       <c r="P49" s="217"/>
@@ -16954,7 +16970,7 @@
     </row>
     <row r="51" spans="2:21" ht="20.25" customHeight="1">
       <c r="B51" s="242" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C51" s="229"/>
       <c r="D51" s="218"/>
@@ -16977,13 +16993,13 @@
     </row>
     <row r="52" spans="2:21" ht="20.25" customHeight="1">
       <c r="B52" s="242" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C52" s="218" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D52" s="218" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E52" s="231"/>
       <c r="F52" s="232"/>
@@ -16995,10 +17011,12 @@
       <c r="L52" s="216"/>
       <c r="M52" s="217"/>
       <c r="N52" s="231" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O52" s="243"/>
-      <c r="P52" s="217"/>
+      <c r="P52" s="314" t="s">
+        <v>678</v>
+      </c>
       <c r="R52" s="307"/>
       <c r="S52" s="308"/>
       <c r="T52" s="308"/>
@@ -17006,7 +17024,7 @@
     </row>
     <row r="53" spans="2:21" ht="20.25" customHeight="1">
       <c r="B53" s="242" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C53" s="218"/>
       <c r="D53" s="218"/>
@@ -17030,10 +17048,10 @@
     <row r="54" spans="2:21" ht="20.25" customHeight="1">
       <c r="B54" s="242"/>
       <c r="C54" s="229" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D54" s="218" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E54" s="231"/>
       <c r="F54" s="232"/>
@@ -17044,9 +17062,13 @@
       <c r="K54" s="231"/>
       <c r="L54" s="216"/>
       <c r="M54" s="217"/>
-      <c r="N54" s="231"/>
-      <c r="O54" s="216"/>
-      <c r="P54" s="217"/>
+      <c r="N54" s="231" t="s">
+        <v>673</v>
+      </c>
+      <c r="O54" s="243"/>
+      <c r="P54" s="314" t="s">
+        <v>678</v>
+      </c>
       <c r="R54" s="307"/>
       <c r="S54" s="308"/>
       <c r="T54" s="308"/>
@@ -17055,10 +17077,10 @@
     <row r="55" spans="2:21" ht="20.25" customHeight="1">
       <c r="B55" s="242"/>
       <c r="C55" s="229" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D55" s="218" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E55" s="231"/>
       <c r="F55" s="232"/>
@@ -17069,9 +17091,13 @@
       <c r="K55" s="231"/>
       <c r="L55" s="216"/>
       <c r="M55" s="217"/>
-      <c r="N55" s="231"/>
-      <c r="O55" s="216"/>
-      <c r="P55" s="217"/>
+      <c r="N55" s="231" t="s">
+        <v>673</v>
+      </c>
+      <c r="O55" s="243"/>
+      <c r="P55" s="314" t="s">
+        <v>677</v>
+      </c>
       <c r="R55" s="307"/>
       <c r="S55" s="308"/>
       <c r="T55" s="308"/>
@@ -17080,10 +17106,10 @@
     <row r="56" spans="2:21" ht="20.25" customHeight="1">
       <c r="B56" s="242"/>
       <c r="C56" s="229" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D56" s="218" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E56" s="231"/>
       <c r="F56" s="232"/>
@@ -17094,9 +17120,13 @@
       <c r="K56" s="231"/>
       <c r="L56" s="216"/>
       <c r="M56" s="217"/>
-      <c r="N56" s="231"/>
-      <c r="O56" s="216"/>
-      <c r="P56" s="217"/>
+      <c r="N56" s="231" t="s">
+        <v>673</v>
+      </c>
+      <c r="O56" s="243"/>
+      <c r="P56" s="314" t="s">
+        <v>677</v>
+      </c>
       <c r="R56" s="307"/>
       <c r="S56" s="308"/>
       <c r="T56" s="308"/>
@@ -17125,7 +17155,7 @@
     </row>
     <row r="58" spans="2:21" ht="20.25" customHeight="1">
       <c r="B58" s="242" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C58" s="229"/>
       <c r="D58" s="218"/>
@@ -17149,10 +17179,10 @@
     <row r="59" spans="2:21" ht="20.25" customHeight="1">
       <c r="B59" s="242"/>
       <c r="C59" s="229" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D59" s="229" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E59" s="231"/>
       <c r="F59" s="232"/>
@@ -17161,7 +17191,7 @@
       <c r="I59" s="216"/>
       <c r="J59" s="217"/>
       <c r="K59" s="244" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="L59" s="243"/>
       <c r="M59" s="217"/>
@@ -17176,10 +17206,10 @@
     <row r="60" spans="2:21" ht="20.25" customHeight="1">
       <c r="B60" s="242"/>
       <c r="C60" s="229" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D60" s="229" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E60" s="231"/>
       <c r="F60" s="232"/>
@@ -17191,7 +17221,7 @@
       <c r="L60" s="216"/>
       <c r="M60" s="217"/>
       <c r="N60" s="231" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O60" s="243"/>
       <c r="P60" s="217"/>
@@ -17203,10 +17233,10 @@
     <row r="61" spans="2:21" ht="20.25" customHeight="1">
       <c r="B61" s="242"/>
       <c r="C61" s="229" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D61" s="229" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E61" s="231"/>
       <c r="F61" s="232"/>
@@ -17218,7 +17248,7 @@
       <c r="L61" s="216"/>
       <c r="M61" s="217"/>
       <c r="N61" s="231" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O61" s="243"/>
       <c r="P61" s="217"/>
@@ -17230,10 +17260,10 @@
     <row r="62" spans="2:21" ht="20.25" customHeight="1">
       <c r="B62" s="242"/>
       <c r="C62" s="229" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D62" s="229" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E62" s="231"/>
       <c r="F62" s="232"/>
@@ -17242,7 +17272,7 @@
       <c r="I62" s="216"/>
       <c r="J62" s="217"/>
       <c r="K62" s="244" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="L62" s="243"/>
       <c r="M62" s="217"/>
@@ -17276,7 +17306,10 @@
       <c r="U63" s="309"/>
     </row>
     <row r="64" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B64" s="242"/>
+      <c r="B64" s="242" t="s">
+        <v>681</v>
+      </c>
+      <c r="C64" s="218"/>
       <c r="D64" s="218"/>
       <c r="E64" s="231"/>
       <c r="F64" s="232"/>
@@ -17296,11 +17329,13 @@
       <c r="U64" s="309"/>
     </row>
     <row r="65" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B65" s="242" t="s">
-        <v>427</v>
-      </c>
-      <c r="C65" s="218"/>
-      <c r="D65" s="218"/>
+      <c r="B65" s="242"/>
+      <c r="C65" s="229" t="s">
+        <v>679</v>
+      </c>
+      <c r="D65" s="229" t="s">
+        <v>595</v>
+      </c>
       <c r="E65" s="231"/>
       <c r="F65" s="232"/>
       <c r="G65" s="217"/>
@@ -17319,11 +17354,13 @@
       <c r="U65" s="309"/>
     </row>
     <row r="66" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B66" s="218"/>
+      <c r="B66" s="242"/>
       <c r="C66" s="229" t="s">
-        <v>636</v>
-      </c>
-      <c r="D66" s="218"/>
+        <v>680</v>
+      </c>
+      <c r="D66" s="229" t="s">
+        <v>595</v>
+      </c>
       <c r="E66" s="231"/>
       <c r="F66" s="232"/>
       <c r="G66" s="217"/>
@@ -17342,9 +17379,13 @@
       <c r="U66" s="309"/>
     </row>
     <row r="67" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B67" s="218"/>
-      <c r="C67" s="218"/>
-      <c r="D67" s="218"/>
+      <c r="B67" s="242"/>
+      <c r="C67" s="229" t="s">
+        <v>682</v>
+      </c>
+      <c r="D67" s="229" t="s">
+        <v>595</v>
+      </c>
       <c r="E67" s="231"/>
       <c r="F67" s="232"/>
       <c r="G67" s="217"/>
@@ -17363,8 +17404,8 @@
       <c r="U67" s="309"/>
     </row>
     <row r="68" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B68" s="218"/>
-      <c r="C68" s="218"/>
+      <c r="B68" s="242"/>
+      <c r="C68" s="229"/>
       <c r="D68" s="218"/>
       <c r="E68" s="231"/>
       <c r="F68" s="232"/>
@@ -17384,7 +17425,7 @@
       <c r="U68" s="309"/>
     </row>
     <row r="69" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B69" s="218"/>
+      <c r="B69" s="242"/>
       <c r="C69" s="218"/>
       <c r="D69" s="218"/>
       <c r="E69" s="231"/>
@@ -17405,7 +17446,9 @@
       <c r="U69" s="309"/>
     </row>
     <row r="70" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B70" s="218"/>
+      <c r="B70" s="242" t="s">
+        <v>427</v>
+      </c>
       <c r="C70" s="218"/>
       <c r="D70" s="218"/>
       <c r="E70" s="231"/>
@@ -20264,18 +20307,18 @@
       <c r="B206" s="218"/>
       <c r="C206" s="218"/>
       <c r="D206" s="218"/>
-      <c r="E206" s="219"/>
-      <c r="F206" s="220"/>
-      <c r="G206" s="221"/>
-      <c r="H206" s="219"/>
-      <c r="I206" s="218"/>
-      <c r="J206" s="221"/>
-      <c r="K206" s="219"/>
-      <c r="L206" s="218"/>
-      <c r="M206" s="221"/>
-      <c r="N206" s="219"/>
-      <c r="O206" s="218"/>
-      <c r="P206" s="221"/>
+      <c r="E206" s="231"/>
+      <c r="F206" s="232"/>
+      <c r="G206" s="217"/>
+      <c r="H206" s="231"/>
+      <c r="I206" s="216"/>
+      <c r="J206" s="217"/>
+      <c r="K206" s="231"/>
+      <c r="L206" s="216"/>
+      <c r="M206" s="217"/>
+      <c r="N206" s="231"/>
+      <c r="O206" s="216"/>
+      <c r="P206" s="217"/>
       <c r="R206" s="307"/>
       <c r="S206" s="308"/>
       <c r="T206" s="308"/>
@@ -20285,18 +20328,18 @@
       <c r="B207" s="218"/>
       <c r="C207" s="218"/>
       <c r="D207" s="218"/>
-      <c r="E207" s="222"/>
-      <c r="F207" s="218"/>
-      <c r="G207" s="221"/>
-      <c r="H207" s="222"/>
-      <c r="I207" s="218"/>
-      <c r="J207" s="221"/>
-      <c r="K207" s="222"/>
-      <c r="L207" s="218"/>
-      <c r="M207" s="221"/>
-      <c r="N207" s="222"/>
-      <c r="O207" s="218"/>
-      <c r="P207" s="221"/>
+      <c r="E207" s="231"/>
+      <c r="F207" s="232"/>
+      <c r="G207" s="217"/>
+      <c r="H207" s="231"/>
+      <c r="I207" s="216"/>
+      <c r="J207" s="217"/>
+      <c r="K207" s="231"/>
+      <c r="L207" s="216"/>
+      <c r="M207" s="217"/>
+      <c r="N207" s="231"/>
+      <c r="O207" s="216"/>
+      <c r="P207" s="217"/>
       <c r="R207" s="307"/>
       <c r="S207" s="308"/>
       <c r="T207" s="308"/>
@@ -20306,18 +20349,18 @@
       <c r="B208" s="218"/>
       <c r="C208" s="218"/>
       <c r="D208" s="218"/>
-      <c r="E208" s="222"/>
-      <c r="F208" s="218"/>
-      <c r="G208" s="221"/>
-      <c r="H208" s="222"/>
-      <c r="I208" s="218"/>
-      <c r="J208" s="221"/>
-      <c r="K208" s="222"/>
-      <c r="L208" s="218"/>
-      <c r="M208" s="221"/>
-      <c r="N208" s="222"/>
-      <c r="O208" s="218"/>
-      <c r="P208" s="221"/>
+      <c r="E208" s="231"/>
+      <c r="F208" s="232"/>
+      <c r="G208" s="217"/>
+      <c r="H208" s="231"/>
+      <c r="I208" s="216"/>
+      <c r="J208" s="217"/>
+      <c r="K208" s="231"/>
+      <c r="L208" s="216"/>
+      <c r="M208" s="217"/>
+      <c r="N208" s="231"/>
+      <c r="O208" s="216"/>
+      <c r="P208" s="217"/>
       <c r="R208" s="307"/>
       <c r="S208" s="308"/>
       <c r="T208" s="308"/>
@@ -20327,18 +20370,18 @@
       <c r="B209" s="218"/>
       <c r="C209" s="218"/>
       <c r="D209" s="218"/>
-      <c r="E209" s="219"/>
-      <c r="F209" s="223"/>
-      <c r="G209" s="224"/>
-      <c r="H209" s="219"/>
-      <c r="I209" s="223"/>
-      <c r="J209" s="224"/>
-      <c r="K209" s="219"/>
-      <c r="L209" s="223"/>
-      <c r="M209" s="224"/>
-      <c r="N209" s="219"/>
-      <c r="O209" s="223"/>
-      <c r="P209" s="224"/>
+      <c r="E209" s="231"/>
+      <c r="F209" s="232"/>
+      <c r="G209" s="217"/>
+      <c r="H209" s="231"/>
+      <c r="I209" s="216"/>
+      <c r="J209" s="217"/>
+      <c r="K209" s="231"/>
+      <c r="L209" s="216"/>
+      <c r="M209" s="217"/>
+      <c r="N209" s="231"/>
+      <c r="O209" s="216"/>
+      <c r="P209" s="217"/>
       <c r="R209" s="307"/>
       <c r="S209" s="308"/>
       <c r="T209" s="308"/>
@@ -20348,39 +20391,39 @@
       <c r="B210" s="218"/>
       <c r="C210" s="218"/>
       <c r="D210" s="218"/>
-      <c r="E210" s="222"/>
-      <c r="F210" s="223"/>
-      <c r="G210" s="224"/>
-      <c r="H210" s="222"/>
-      <c r="I210" s="223"/>
-      <c r="J210" s="224"/>
-      <c r="K210" s="222"/>
-      <c r="L210" s="223"/>
-      <c r="M210" s="224"/>
-      <c r="N210" s="222"/>
-      <c r="O210" s="223"/>
-      <c r="P210" s="224"/>
+      <c r="E210" s="231"/>
+      <c r="F210" s="232"/>
+      <c r="G210" s="217"/>
+      <c r="H210" s="231"/>
+      <c r="I210" s="216"/>
+      <c r="J210" s="217"/>
+      <c r="K210" s="231"/>
+      <c r="L210" s="216"/>
+      <c r="M210" s="217"/>
+      <c r="N210" s="231"/>
+      <c r="O210" s="216"/>
+      <c r="P210" s="217"/>
       <c r="R210" s="307"/>
       <c r="S210" s="308"/>
       <c r="T210" s="308"/>
       <c r="U210" s="309"/>
     </row>
     <row r="211" spans="2:21" ht="20.25" customHeight="1">
-      <c r="B211" s="229"/>
+      <c r="B211" s="218"/>
       <c r="C211" s="218"/>
       <c r="D211" s="218"/>
-      <c r="E211" s="222"/>
-      <c r="F211" s="223"/>
-      <c r="G211" s="224"/>
-      <c r="H211" s="222"/>
-      <c r="I211" s="223"/>
-      <c r="J211" s="224"/>
-      <c r="K211" s="222"/>
-      <c r="L211" s="223"/>
-      <c r="M211" s="224"/>
-      <c r="N211" s="222"/>
-      <c r="O211" s="223"/>
-      <c r="P211" s="224"/>
+      <c r="E211" s="219"/>
+      <c r="F211" s="220"/>
+      <c r="G211" s="221"/>
+      <c r="H211" s="219"/>
+      <c r="I211" s="218"/>
+      <c r="J211" s="221"/>
+      <c r="K211" s="219"/>
+      <c r="L211" s="218"/>
+      <c r="M211" s="221"/>
+      <c r="N211" s="219"/>
+      <c r="O211" s="218"/>
+      <c r="P211" s="221"/>
       <c r="R211" s="307"/>
       <c r="S211" s="308"/>
       <c r="T211" s="308"/>
@@ -20390,18 +20433,18 @@
       <c r="B212" s="218"/>
       <c r="C212" s="218"/>
       <c r="D212" s="218"/>
-      <c r="E212" s="219"/>
-      <c r="F212" s="223"/>
-      <c r="G212" s="224"/>
-      <c r="H212" s="219"/>
-      <c r="I212" s="223"/>
-      <c r="J212" s="224"/>
-      <c r="K212" s="219"/>
-      <c r="L212" s="223"/>
-      <c r="M212" s="224"/>
-      <c r="N212" s="219"/>
-      <c r="O212" s="223"/>
-      <c r="P212" s="224"/>
+      <c r="E212" s="222"/>
+      <c r="F212" s="218"/>
+      <c r="G212" s="221"/>
+      <c r="H212" s="222"/>
+      <c r="I212" s="218"/>
+      <c r="J212" s="221"/>
+      <c r="K212" s="222"/>
+      <c r="L212" s="218"/>
+      <c r="M212" s="221"/>
+      <c r="N212" s="222"/>
+      <c r="O212" s="218"/>
+      <c r="P212" s="221"/>
       <c r="R212" s="307"/>
       <c r="S212" s="308"/>
       <c r="T212" s="308"/>
@@ -20412,17 +20455,17 @@
       <c r="C213" s="218"/>
       <c r="D213" s="218"/>
       <c r="E213" s="222"/>
-      <c r="F213" s="223"/>
-      <c r="G213" s="224"/>
+      <c r="F213" s="218"/>
+      <c r="G213" s="221"/>
       <c r="H213" s="222"/>
-      <c r="I213" s="223"/>
-      <c r="J213" s="224"/>
+      <c r="I213" s="218"/>
+      <c r="J213" s="221"/>
       <c r="K213" s="222"/>
-      <c r="L213" s="223"/>
-      <c r="M213" s="224"/>
+      <c r="L213" s="218"/>
+      <c r="M213" s="221"/>
       <c r="N213" s="222"/>
-      <c r="O213" s="223"/>
-      <c r="P213" s="224"/>
+      <c r="O213" s="218"/>
+      <c r="P213" s="221"/>
       <c r="R213" s="307"/>
       <c r="S213" s="308"/>
       <c r="T213" s="308"/>
@@ -20432,16 +20475,16 @@
       <c r="B214" s="218"/>
       <c r="C214" s="218"/>
       <c r="D214" s="218"/>
-      <c r="E214" s="222"/>
+      <c r="E214" s="219"/>
       <c r="F214" s="223"/>
       <c r="G214" s="224"/>
-      <c r="H214" s="222"/>
+      <c r="H214" s="219"/>
       <c r="I214" s="223"/>
       <c r="J214" s="224"/>
-      <c r="K214" s="222"/>
+      <c r="K214" s="219"/>
       <c r="L214" s="223"/>
       <c r="M214" s="224"/>
-      <c r="N214" s="222"/>
+      <c r="N214" s="219"/>
       <c r="O214" s="223"/>
       <c r="P214" s="224"/>
       <c r="R214" s="307"/>
@@ -20453,16 +20496,16 @@
       <c r="B215" s="218"/>
       <c r="C215" s="218"/>
       <c r="D215" s="218"/>
-      <c r="E215" s="219"/>
+      <c r="E215" s="222"/>
       <c r="F215" s="223"/>
       <c r="G215" s="224"/>
-      <c r="H215" s="219"/>
+      <c r="H215" s="222"/>
       <c r="I215" s="223"/>
       <c r="J215" s="224"/>
-      <c r="K215" s="219"/>
+      <c r="K215" s="222"/>
       <c r="L215" s="223"/>
       <c r="M215" s="224"/>
-      <c r="N215" s="219"/>
+      <c r="N215" s="222"/>
       <c r="O215" s="223"/>
       <c r="P215" s="224"/>
       <c r="R215" s="307"/>
@@ -20470,51 +20513,156 @@
       <c r="T215" s="308"/>
       <c r="U215" s="309"/>
     </row>
-    <row r="216" spans="2:21" ht="20.25" customHeight="1" thickBot="1">
-      <c r="B216" s="225"/>
-      <c r="C216" s="226"/>
-      <c r="D216" s="227"/>
-      <c r="E216" s="230"/>
-      <c r="F216" s="226"/>
-      <c r="G216" s="228"/>
-      <c r="H216" s="230"/>
-      <c r="I216" s="226"/>
-      <c r="J216" s="228"/>
-      <c r="K216" s="230"/>
-      <c r="L216" s="226"/>
-      <c r="M216" s="228"/>
-      <c r="N216" s="230"/>
-      <c r="O216" s="226"/>
-      <c r="P216" s="228"/>
-      <c r="R216" s="310"/>
-      <c r="S216" s="311"/>
-      <c r="T216" s="311"/>
-      <c r="U216" s="312"/>
-    </row>
-    <row r="217" spans="2:21" ht="15.75" customHeight="1">
-      <c r="B217" s="186"/>
-      <c r="C217" s="186"/>
-      <c r="D217" s="186"/>
-      <c r="E217" s="186"/>
-      <c r="F217" s="186"/>
-      <c r="G217" s="186"/>
-      <c r="H217" s="186"/>
-      <c r="I217" s="186"/>
-      <c r="J217" s="186"/>
-      <c r="K217" s="186"/>
-      <c r="L217" s="186"/>
-      <c r="M217" s="186"/>
-      <c r="N217" s="186"/>
-      <c r="O217" s="186"/>
-      <c r="P217" s="186"/>
-      <c r="Q217" s="186"/>
+    <row r="216" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B216" s="229"/>
+      <c r="C216" s="218"/>
+      <c r="D216" s="218"/>
+      <c r="E216" s="222"/>
+      <c r="F216" s="223"/>
+      <c r="G216" s="224"/>
+      <c r="H216" s="222"/>
+      <c r="I216" s="223"/>
+      <c r="J216" s="224"/>
+      <c r="K216" s="222"/>
+      <c r="L216" s="223"/>
+      <c r="M216" s="224"/>
+      <c r="N216" s="222"/>
+      <c r="O216" s="223"/>
+      <c r="P216" s="224"/>
+      <c r="R216" s="307"/>
+      <c r="S216" s="308"/>
+      <c r="T216" s="308"/>
+      <c r="U216" s="309"/>
+    </row>
+    <row r="217" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B217" s="218"/>
+      <c r="C217" s="218"/>
+      <c r="D217" s="218"/>
+      <c r="E217" s="219"/>
+      <c r="F217" s="223"/>
+      <c r="G217" s="224"/>
+      <c r="H217" s="219"/>
+      <c r="I217" s="223"/>
+      <c r="J217" s="224"/>
+      <c r="K217" s="219"/>
+      <c r="L217" s="223"/>
+      <c r="M217" s="224"/>
+      <c r="N217" s="219"/>
+      <c r="O217" s="223"/>
+      <c r="P217" s="224"/>
+      <c r="R217" s="307"/>
+      <c r="S217" s="308"/>
+      <c r="T217" s="308"/>
+      <c r="U217" s="309"/>
+    </row>
+    <row r="218" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B218" s="218"/>
+      <c r="C218" s="218"/>
+      <c r="D218" s="218"/>
+      <c r="E218" s="222"/>
+      <c r="F218" s="223"/>
+      <c r="G218" s="224"/>
+      <c r="H218" s="222"/>
+      <c r="I218" s="223"/>
+      <c r="J218" s="224"/>
+      <c r="K218" s="222"/>
+      <c r="L218" s="223"/>
+      <c r="M218" s="224"/>
+      <c r="N218" s="222"/>
+      <c r="O218" s="223"/>
+      <c r="P218" s="224"/>
+      <c r="R218" s="307"/>
+      <c r="S218" s="308"/>
+      <c r="T218" s="308"/>
+      <c r="U218" s="309"/>
+    </row>
+    <row r="219" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B219" s="218"/>
+      <c r="C219" s="218"/>
+      <c r="D219" s="218"/>
+      <c r="E219" s="222"/>
+      <c r="F219" s="223"/>
+      <c r="G219" s="224"/>
+      <c r="H219" s="222"/>
+      <c r="I219" s="223"/>
+      <c r="J219" s="224"/>
+      <c r="K219" s="222"/>
+      <c r="L219" s="223"/>
+      <c r="M219" s="224"/>
+      <c r="N219" s="222"/>
+      <c r="O219" s="223"/>
+      <c r="P219" s="224"/>
+      <c r="R219" s="307"/>
+      <c r="S219" s="308"/>
+      <c r="T219" s="308"/>
+      <c r="U219" s="309"/>
+    </row>
+    <row r="220" spans="2:21" ht="20.25" customHeight="1">
+      <c r="B220" s="218"/>
+      <c r="C220" s="218"/>
+      <c r="D220" s="218"/>
+      <c r="E220" s="219"/>
+      <c r="F220" s="223"/>
+      <c r="G220" s="224"/>
+      <c r="H220" s="219"/>
+      <c r="I220" s="223"/>
+      <c r="J220" s="224"/>
+      <c r="K220" s="219"/>
+      <c r="L220" s="223"/>
+      <c r="M220" s="224"/>
+      <c r="N220" s="219"/>
+      <c r="O220" s="223"/>
+      <c r="P220" s="224"/>
+      <c r="R220" s="307"/>
+      <c r="S220" s="308"/>
+      <c r="T220" s="308"/>
+      <c r="U220" s="309"/>
+    </row>
+    <row r="221" spans="2:21" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B221" s="225"/>
+      <c r="C221" s="226"/>
+      <c r="D221" s="227"/>
+      <c r="E221" s="230"/>
+      <c r="F221" s="226"/>
+      <c r="G221" s="228"/>
+      <c r="H221" s="230"/>
+      <c r="I221" s="226"/>
+      <c r="J221" s="228"/>
+      <c r="K221" s="230"/>
+      <c r="L221" s="226"/>
+      <c r="M221" s="228"/>
+      <c r="N221" s="230"/>
+      <c r="O221" s="226"/>
+      <c r="P221" s="228"/>
+      <c r="R221" s="310"/>
+      <c r="S221" s="311"/>
+      <c r="T221" s="311"/>
+      <c r="U221" s="312"/>
+    </row>
+    <row r="222" spans="2:21" ht="15.75" customHeight="1">
+      <c r="B222" s="186"/>
+      <c r="C222" s="186"/>
+      <c r="D222" s="186"/>
+      <c r="E222" s="186"/>
+      <c r="F222" s="186"/>
+      <c r="G222" s="186"/>
+      <c r="H222" s="186"/>
+      <c r="I222" s="186"/>
+      <c r="J222" s="186"/>
+      <c r="K222" s="186"/>
+      <c r="L222" s="186"/>
+      <c r="M222" s="186"/>
+      <c r="N222" s="186"/>
+      <c r="O222" s="186"/>
+      <c r="P222" s="186"/>
+      <c r="Q222" s="186"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="H3:P3"/>
-    <mergeCell ref="R6:U216"/>
+    <mergeCell ref="R6:U221"/>
   </mergeCells>
-  <conditionalFormatting sqref="B12:D27 C28:C38 B28:B215 D38 C40:C51 D53 C53:C63 C66:C222">
+  <conditionalFormatting sqref="B12:D27 C28:C38 B28:B220 D38 C40:C51 D53 C53:C227">
     <cfRule type="expression" dxfId="8" priority="7">
       <formula>IF((B12&lt;&gt;"")*AND(F12&lt;&gt;""),1,0)</formula>
     </cfRule>
@@ -20534,11 +20682,6 @@
       <formula>IF((C52&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="4" priority="18">
-      <formula>IF((C65&lt;&gt;"")*AND(G64&lt;&gt;""),1,0)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C28:D37">
     <cfRule type="expression" dxfId="3" priority="14">
       <formula>IF((C28&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
@@ -20554,7 +20697,7 @@
       <formula>IF((D54&lt;&gt;"")*AND(#REF!&lt;&gt;""),1,0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D59:D215">
+  <conditionalFormatting sqref="D59:D220">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF((D59&lt;&gt;"")*AND(H59&lt;&gt;""),1,0)</formula>
     </cfRule>

</xml_diff>